<commit_message>
Added  books to book ranking
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="79">
   <si>
     <t>Book Ranking</t>
   </si>
@@ -245,6 +245,15 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Bringin up Bebe</t>
+  </si>
+  <si>
+    <t>Fiasco</t>
+  </si>
+  <si>
+    <t>The Relativity of Wrong (Asimov)</t>
   </si>
 </sst>
 </file>
@@ -608,11 +617,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,17 +1180,17 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B32" s="3">
         <v>4</v>
       </c>
       <c r="C32" s="3">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D32" s="7">
         <f>B32/C32</f>
-        <v>9.1743119266055051E-3</v>
+        <v>9.2592592592592587E-3</v>
       </c>
       <c r="E32" t="s">
         <v>75</v>
@@ -1189,17 +1198,17 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B33" s="3">
         <v>4</v>
       </c>
       <c r="C33" s="3">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="D33" s="7">
         <f>B33/C33</f>
-        <v>9.0090090090090089E-3</v>
+        <v>9.1743119266055051E-3</v>
       </c>
       <c r="E33" t="s">
         <v>75</v>
@@ -1207,17 +1216,17 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="B34" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C34" s="3">
-        <v>336</v>
+        <v>444</v>
       </c>
       <c r="D34" s="7">
         <f>B34/C34</f>
-        <v>8.9285714285714281E-3</v>
+        <v>9.0090090090090089E-3</v>
       </c>
       <c r="E34" t="s">
         <v>75</v>
@@ -1225,17 +1234,17 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="B35" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" s="3">
-        <v>464</v>
+        <v>336</v>
       </c>
       <c r="D35" s="7">
         <f>B35/C35</f>
-        <v>8.6206896551724137E-3</v>
+        <v>8.9285714285714281E-3</v>
       </c>
       <c r="E35" t="s">
         <v>75</v>
@@ -1243,17 +1252,17 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B36" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C36" s="3">
-        <v>464</v>
+        <v>225</v>
       </c>
       <c r="D36" s="7">
         <f>B36/C36</f>
-        <v>8.6206896551724137E-3</v>
+        <v>8.8888888888888889E-3</v>
       </c>
       <c r="E36" t="s">
         <v>75</v>
@@ -1261,17 +1270,17 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B37" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C37" s="3">
-        <v>352</v>
+        <v>464</v>
       </c>
       <c r="D37" s="7">
         <f>B37/C37</f>
-        <v>8.5227272727272721E-3</v>
+        <v>8.6206896551724137E-3</v>
       </c>
       <c r="E37" t="s">
         <v>75</v>
@@ -1279,17 +1288,17 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="B38" s="3">
         <v>4</v>
       </c>
       <c r="C38" s="3">
-        <v>480</v>
+        <v>464</v>
       </c>
       <c r="D38" s="7">
         <f>B38/C38</f>
-        <v>8.3333333333333332E-3</v>
+        <v>8.6206896551724137E-3</v>
       </c>
       <c r="E38" t="s">
         <v>75</v>
@@ -1297,17 +1306,17 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B39" s="3">
         <v>3</v>
       </c>
       <c r="C39" s="3">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D39" s="7">
         <f>B39/C39</f>
-        <v>8.3333333333333332E-3</v>
+        <v>8.5227272727272721E-3</v>
       </c>
       <c r="E39" t="s">
         <v>75</v>
@@ -1315,13 +1324,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B40" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C40" s="3">
-        <v>240</v>
+        <v>480</v>
       </c>
       <c r="D40" s="7">
         <f>B40/C40</f>
@@ -1333,17 +1342,17 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B41" s="3">
         <v>3</v>
       </c>
       <c r="C41" s="3">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="D41" s="7">
         <f>B41/C41</f>
-        <v>8.152173913043478E-3</v>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E41" t="s">
         <v>75</v>
@@ -1351,17 +1360,17 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B42" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" s="3">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="D42" s="7">
         <f>B42/C42</f>
-        <v>8.152173913043478E-3</v>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E42" t="s">
         <v>75</v>
@@ -1369,17 +1378,17 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B43" s="3">
         <v>3</v>
       </c>
       <c r="C43" s="3">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D43" s="7">
         <f>B43/C43</f>
-        <v>8.0862533692722376E-3</v>
+        <v>8.152173913043478E-3</v>
       </c>
       <c r="E43" t="s">
         <v>75</v>
@@ -1387,17 +1396,17 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B44" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44" s="3">
-        <v>499</v>
+        <v>368</v>
       </c>
       <c r="D44" s="7">
         <f>B44/C44</f>
-        <v>8.0160320641282558E-3</v>
+        <v>8.152173913043478E-3</v>
       </c>
       <c r="E44" t="s">
         <v>75</v>
@@ -1405,17 +1414,17 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="B45" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C45" s="3">
-        <v>250</v>
+        <v>371</v>
       </c>
       <c r="D45" s="7">
         <f>B45/C45</f>
-        <v>8.0000000000000002E-3</v>
+        <v>8.0862533692722376E-3</v>
       </c>
       <c r="E45" t="s">
         <v>75</v>
@@ -1423,17 +1432,17 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B46" s="3">
         <v>4</v>
       </c>
       <c r="C46" s="3">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="D46" s="7">
         <f>B46/C46</f>
-        <v>7.8125E-3</v>
+        <v>8.0160320641282558E-3</v>
       </c>
       <c r="E46" t="s">
         <v>75</v>
@@ -1441,17 +1450,17 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B47" s="3">
         <v>2</v>
       </c>
       <c r="C47" s="3">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="D47" s="7">
         <f>B47/C47</f>
-        <v>7.575757575757576E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E47" t="s">
         <v>75</v>
@@ -1459,17 +1468,17 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B48" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C48" s="3">
-        <v>400</v>
+        <v>512</v>
       </c>
       <c r="D48" s="7">
         <f>B48/C48</f>
-        <v>7.4999999999999997E-3</v>
+        <v>7.8125E-3</v>
       </c>
       <c r="E48" t="s">
         <v>75</v>
@@ -1477,17 +1486,17 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B49" s="3">
         <v>4</v>
       </c>
       <c r="C49" s="3">
-        <v>544</v>
+        <v>512</v>
       </c>
       <c r="D49" s="7">
         <f>B49/C49</f>
-        <v>7.3529411764705881E-3</v>
+        <v>7.8125E-3</v>
       </c>
       <c r="E49" t="s">
         <v>75</v>
@@ -1495,17 +1504,17 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B50" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C50" s="3">
-        <v>560</v>
+        <v>264</v>
       </c>
       <c r="D50" s="7">
         <f>B50/C50</f>
-        <v>7.1428571428571426E-3</v>
+        <v>7.575757575757576E-3</v>
       </c>
       <c r="E50" t="s">
         <v>75</v>
@@ -1513,17 +1522,17 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="B51" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C51" s="3">
-        <v>284</v>
+        <v>400</v>
       </c>
       <c r="D51" s="7">
         <f>B51/C51</f>
-        <v>7.0422535211267607E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E51" t="s">
         <v>75</v>
@@ -1531,17 +1540,17 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B52" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C52" s="3">
-        <v>288</v>
+        <v>544</v>
       </c>
       <c r="D52" s="7">
         <f>B52/C52</f>
-        <v>6.9444444444444441E-3</v>
+        <v>7.3529411764705881E-3</v>
       </c>
       <c r="E52" t="s">
         <v>75</v>
@@ -1549,17 +1558,17 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="B53" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C53" s="3">
-        <v>148</v>
+        <v>560</v>
       </c>
       <c r="D53" s="7">
         <f>B53/C53</f>
-        <v>6.7567567567567571E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
       <c r="E53" t="s">
         <v>75</v>
@@ -1567,17 +1576,17 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B54" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" s="3">
-        <v>480</v>
+        <v>284</v>
       </c>
       <c r="D54" s="7">
         <f>B54/C54</f>
-        <v>6.2500000000000003E-3</v>
+        <v>7.0422535211267607E-3</v>
       </c>
       <c r="E54" t="s">
         <v>75</v>
@@ -1585,17 +1594,17 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B55" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55" s="3">
-        <v>480</v>
+        <v>288</v>
       </c>
       <c r="D55" s="7">
         <f>B55/C55</f>
-        <v>6.2500000000000003E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="E55" t="s">
         <v>75</v>
@@ -1603,17 +1612,17 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B56" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C56" s="3">
-        <v>488</v>
+        <v>148</v>
       </c>
       <c r="D56" s="7">
         <f>B56/C56</f>
-        <v>6.1475409836065573E-3</v>
+        <v>6.7567567567567571E-3</v>
       </c>
       <c r="E56" t="s">
         <v>75</v>
@@ -1621,17 +1630,17 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="B57" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C57" s="3">
-        <v>332</v>
+        <v>480</v>
       </c>
       <c r="D57" s="7">
         <f>B57/C57</f>
-        <v>6.024096385542169E-3</v>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E57" t="s">
         <v>75</v>
@@ -1639,17 +1648,17 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B58" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58" s="3">
-        <v>704</v>
+        <v>480</v>
       </c>
       <c r="D58" s="7">
         <f>B58/C58</f>
-        <v>5.681818181818182E-3</v>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E58" t="s">
         <v>75</v>
@@ -1657,17 +1666,17 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="B59" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C59" s="3">
-        <v>736</v>
+        <v>488</v>
       </c>
       <c r="D59" s="7">
         <f>B59/C59</f>
-        <v>5.434782608695652E-3</v>
+        <v>6.1475409836065573E-3</v>
       </c>
       <c r="E59" t="s">
         <v>75</v>
@@ -1675,17 +1684,17 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B60" s="3">
         <v>2</v>
       </c>
       <c r="C60" s="3">
-        <v>373</v>
+        <v>332</v>
       </c>
       <c r="D60" s="7">
         <f>B60/C60</f>
-        <v>5.3619302949061663E-3</v>
+        <v>6.024096385542169E-3</v>
       </c>
       <c r="E60" t="s">
         <v>75</v>
@@ -1693,17 +1702,17 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B61" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C61" s="3">
-        <v>560</v>
+        <v>704</v>
       </c>
       <c r="D61" s="7">
         <f>B61/C61</f>
-        <v>5.3571428571428572E-3</v>
+        <v>5.681818181818182E-3</v>
       </c>
       <c r="E61" t="s">
         <v>75</v>
@@ -1711,17 +1720,17 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="B62" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C62" s="3">
-        <v>560</v>
+        <v>736</v>
       </c>
       <c r="D62" s="7">
         <f>B62/C62</f>
-        <v>5.3571428571428572E-3</v>
+        <v>5.434782608695652E-3</v>
       </c>
       <c r="E62" t="s">
         <v>75</v>
@@ -1729,17 +1738,17 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B63" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63" s="3">
-        <v>576</v>
+        <v>373</v>
       </c>
       <c r="D63" s="7">
         <f>B63/C63</f>
-        <v>5.208333333333333E-3</v>
+        <v>5.3619302949061663E-3</v>
       </c>
       <c r="E63" t="s">
         <v>75</v>
@@ -1747,17 +1756,17 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B64" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C64" s="3">
-        <v>384</v>
+        <v>560</v>
       </c>
       <c r="D64" s="7">
         <f>B64/C64</f>
-        <v>5.208333333333333E-3</v>
+        <v>5.3571428571428572E-3</v>
       </c>
       <c r="E64" t="s">
         <v>75</v>
@@ -1765,17 +1774,17 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B65" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C65" s="3">
-        <v>400</v>
+        <v>560</v>
       </c>
       <c r="D65" s="7">
         <f>B65/C65</f>
-        <v>5.0000000000000001E-3</v>
+        <v>5.3571428571428572E-3</v>
       </c>
       <c r="E65" t="s">
         <v>75</v>
@@ -1783,17 +1792,17 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B66" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C66" s="3">
-        <v>416</v>
+        <v>576</v>
       </c>
       <c r="D66" s="7">
         <f>B66/C66</f>
-        <v>4.807692307692308E-3</v>
+        <v>5.208333333333333E-3</v>
       </c>
       <c r="E66" t="s">
         <v>75</v>
@@ -1801,17 +1810,17 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="B67" s="3">
         <v>2</v>
       </c>
       <c r="C67" s="3">
-        <v>416</v>
+        <v>384</v>
       </c>
       <c r="D67" s="7">
         <f>B67/C67</f>
-        <v>4.807692307692308E-3</v>
+        <v>5.208333333333333E-3</v>
       </c>
       <c r="E67" t="s">
         <v>75</v>
@@ -1819,17 +1828,17 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B68" s="3">
         <v>2</v>
       </c>
       <c r="C68" s="3">
-        <v>528</v>
+        <v>400</v>
       </c>
       <c r="D68" s="7">
         <f>B68/C68</f>
-        <v>3.787878787878788E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E68" t="s">
         <v>75</v>
@@ -1837,17 +1846,17 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="B69" s="3">
         <v>2</v>
       </c>
       <c r="C69" s="3">
-        <v>544</v>
+        <v>416</v>
       </c>
       <c r="D69" s="7">
         <f>B69/C69</f>
-        <v>3.6764705882352941E-3</v>
+        <v>4.807692307692308E-3</v>
       </c>
       <c r="E69" t="s">
         <v>75</v>
@@ -1855,17 +1864,17 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="B70" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" s="3">
-        <v>848</v>
+        <v>416</v>
       </c>
       <c r="D70" s="7">
         <f>B70/C70</f>
-        <v>3.5377358490566039E-3</v>
+        <v>4.807692307692308E-3</v>
       </c>
       <c r="E70" t="s">
         <v>75</v>
@@ -1873,25 +1882,79 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B71" s="3">
         <v>2</v>
       </c>
       <c r="C71" s="3">
-        <v>616</v>
+        <v>528</v>
       </c>
       <c r="D71" s="7">
         <f>B71/C71</f>
+        <v>3.787878787878788E-3</v>
+      </c>
+      <c r="E71" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72" s="3">
+        <v>2</v>
+      </c>
+      <c r="C72" s="3">
+        <v>544</v>
+      </c>
+      <c r="D72" s="7">
+        <f>B72/C72</f>
+        <v>3.6764705882352941E-3</v>
+      </c>
+      <c r="E72" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="3">
+        <v>3</v>
+      </c>
+      <c r="C73" s="3">
+        <v>848</v>
+      </c>
+      <c r="D73" s="7">
+        <f>B73/C73</f>
+        <v>3.5377358490566039E-3</v>
+      </c>
+      <c r="E73" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="3">
+        <v>2</v>
+      </c>
+      <c r="C74" s="3">
+        <v>616</v>
+      </c>
+      <c r="D74" s="7">
+        <f>B74/C74</f>
         <v>3.246753246753247E-3</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E74" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D70">
-    <sortState ref="A3:D71">
+    <sortState ref="A3:D74">
       <sortCondition descending="1" ref="D2:D70"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Added books to book list
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
   <si>
     <t>Book Ranking</t>
   </si>
@@ -254,6 +254,24 @@
   </si>
   <si>
     <t>The Relativity of Wrong (Asimov)</t>
+  </si>
+  <si>
+    <t>The Hero with a Thousand Faces</t>
+  </si>
+  <si>
+    <t>Maneuver Warfare Handbook</t>
+  </si>
+  <si>
+    <t>Markings (Dag)</t>
+  </si>
+  <si>
+    <t>The Penguin Guide to the United States Constitution</t>
+  </si>
+  <si>
+    <t>Buddhism: An Introduction and Guide</t>
+  </si>
+  <si>
+    <t>Letters from a Stoic</t>
   </si>
 </sst>
 </file>
@@ -617,11 +635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E74" sqref="E74"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,17 +748,17 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="B7" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D7" s="7">
         <f>B7/C7</f>
-        <v>3.0303030303030304E-2</v>
+        <v>3.7593984962406013E-2</v>
       </c>
       <c r="E7" t="s">
         <v>75</v>
@@ -748,17 +766,17 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
       <c r="C8" s="3">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="D8" s="7">
         <f>B8/C8</f>
-        <v>2.5000000000000001E-2</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="E8" t="s">
         <v>75</v>
@@ -766,13 +784,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="B9" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9" s="3">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="D9" s="7">
         <f>B9/C9</f>
@@ -784,17 +802,17 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B10" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="3">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="D10" s="7">
         <f>B10/C10</f>
-        <v>2.34375E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E10" t="s">
         <v>75</v>
@@ -802,17 +820,17 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3">
-        <v>228</v>
+        <v>128</v>
       </c>
       <c r="D11" s="7">
         <f>B11/C11</f>
-        <v>2.1929824561403508E-2</v>
+        <v>2.34375E-2</v>
       </c>
       <c r="E11" t="s">
         <v>75</v>
@@ -820,17 +838,17 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B12" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3">
-        <v>192</v>
+        <v>228</v>
       </c>
       <c r="D12" s="7">
         <f>B12/C12</f>
-        <v>2.0833333333333332E-2</v>
+        <v>2.1929824561403508E-2</v>
       </c>
       <c r="E12" t="s">
         <v>75</v>
@@ -838,17 +856,17 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="B13" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="3">
-        <v>160</v>
+        <v>191</v>
       </c>
       <c r="D13" s="7">
         <f>B13/C13</f>
-        <v>1.8749999999999999E-2</v>
+        <v>2.0942408376963352E-2</v>
       </c>
       <c r="E13" t="s">
         <v>75</v>
@@ -856,17 +874,17 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
       </c>
       <c r="C14" s="3">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="D14" s="7">
         <f>B14/C14</f>
-        <v>1.7857142857142856E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="E14" t="s">
         <v>75</v>
@@ -874,17 +892,17 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B15" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" s="3">
-        <v>288</v>
+        <v>160</v>
       </c>
       <c r="D15" s="7">
         <f>B15/C15</f>
-        <v>1.7361111111111112E-2</v>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="E15" t="s">
         <v>75</v>
@@ -892,17 +910,17 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="B16" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" s="3">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="D16" s="7">
         <f>B16/C16</f>
-        <v>1.6483516483516484E-2</v>
+        <v>1.7857142857142856E-2</v>
       </c>
       <c r="E16" t="s">
         <v>75</v>
@@ -910,17 +928,17 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="B17" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" s="3">
-        <v>250</v>
+        <v>288</v>
       </c>
       <c r="D17" s="7">
         <f>B17/C17</f>
-        <v>1.6E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="E17" t="s">
         <v>75</v>
@@ -928,17 +946,17 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="B18" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="3">
-        <v>336</v>
+        <v>231</v>
       </c>
       <c r="D18" s="7">
         <f>B18/C18</f>
-        <v>1.488095238095238E-2</v>
+        <v>1.7316017316017316E-2</v>
       </c>
       <c r="E18" t="s">
         <v>75</v>
@@ -946,17 +964,17 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B19" s="3">
         <v>3</v>
       </c>
       <c r="C19" s="3">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="D19" s="7">
         <f>B19/C19</f>
-        <v>1.4423076923076924E-2</v>
+        <v>1.6483516483516484E-2</v>
       </c>
       <c r="E19" t="s">
         <v>75</v>
@@ -964,17 +982,17 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="B20" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="3">
-        <v>368</v>
+        <v>250</v>
       </c>
       <c r="D20" s="7">
         <f>B20/C20</f>
-        <v>1.358695652173913E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="E20" t="s">
         <v>75</v>
@@ -982,17 +1000,17 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B21" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" s="3">
-        <v>320</v>
+        <v>336</v>
       </c>
       <c r="D21" s="7">
         <f>B21/C21</f>
-        <v>1.2500000000000001E-2</v>
+        <v>1.488095238095238E-2</v>
       </c>
       <c r="E21" t="s">
         <v>75</v>
@@ -1000,17 +1018,17 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B22" s="3">
         <v>4</v>
       </c>
       <c r="C22" s="3">
-        <v>336</v>
+        <v>276</v>
       </c>
       <c r="D22" s="7">
         <f>B22/C22</f>
-        <v>1.1904761904761904E-2</v>
+        <v>1.4492753623188406E-2</v>
       </c>
       <c r="E22" t="s">
         <v>75</v>
@@ -1018,17 +1036,17 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B23" s="3">
         <v>3</v>
       </c>
       <c r="C23" s="3">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="D23" s="7">
         <f>B23/C23</f>
-        <v>1.171875E-2</v>
+        <v>1.4423076923076924E-2</v>
       </c>
       <c r="E23" t="s">
         <v>75</v>
@@ -1036,17 +1054,17 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="B24" s="3">
         <v>3</v>
       </c>
       <c r="C24" s="3">
-        <v>264</v>
+        <v>213</v>
       </c>
       <c r="D24" s="7">
         <f>B24/C24</f>
-        <v>1.1363636363636364E-2</v>
+        <v>1.4084507042253521E-2</v>
       </c>
       <c r="E24" t="s">
         <v>75</v>
@@ -1054,17 +1072,17 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="B25" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" s="3">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="D25" s="7">
         <f>B25/C25</f>
-        <v>1.0416666666666666E-2</v>
+        <v>1.358695652173913E-2</v>
       </c>
       <c r="E25" t="s">
         <v>75</v>
@@ -1072,17 +1090,17 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B26" s="3">
         <v>4</v>
       </c>
       <c r="C26" s="3">
-        <v>384</v>
+        <v>320</v>
       </c>
       <c r="D26" s="7">
         <f>B26/C26</f>
-        <v>1.0416666666666666E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="E26" t="s">
         <v>75</v>
@@ -1090,17 +1108,17 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="B27" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27" s="3">
-        <v>288</v>
+        <v>336</v>
       </c>
       <c r="D27" s="7">
         <f>B27/C27</f>
-        <v>1.0416666666666666E-2</v>
+        <v>1.1904761904761904E-2</v>
       </c>
       <c r="E27" t="s">
         <v>75</v>
@@ -1108,17 +1126,17 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B28" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" s="3">
-        <v>400</v>
+        <v>256</v>
       </c>
       <c r="D28" s="7">
         <f>B28/C28</f>
-        <v>0.01</v>
+        <v>1.171875E-2</v>
       </c>
       <c r="E28" t="s">
         <v>75</v>
@@ -1126,17 +1144,17 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="B29" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C29" s="3">
-        <v>416</v>
+        <v>432</v>
       </c>
       <c r="D29" s="7">
         <f>B29/C29</f>
-        <v>9.6153846153846159E-3</v>
+        <v>1.1574074074074073E-2</v>
       </c>
       <c r="E29" t="s">
         <v>75</v>
@@ -1144,17 +1162,17 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="B30" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3">
-        <v>208</v>
+        <v>264</v>
       </c>
       <c r="D30" s="7">
         <f>B30/C30</f>
-        <v>9.6153846153846159E-3</v>
+        <v>1.1363636363636364E-2</v>
       </c>
       <c r="E30" t="s">
         <v>75</v>
@@ -1162,17 +1180,17 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="B31" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C31" s="3">
-        <v>208</v>
+        <v>384</v>
       </c>
       <c r="D31" s="7">
         <f>B31/C31</f>
-        <v>9.6153846153846159E-3</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E31" t="s">
         <v>75</v>
@@ -1180,17 +1198,17 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B32" s="3">
         <v>4</v>
       </c>
       <c r="C32" s="3">
-        <v>432</v>
+        <v>384</v>
       </c>
       <c r="D32" s="7">
         <f>B32/C32</f>
-        <v>9.2592592592592587E-3</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E32" t="s">
         <v>75</v>
@@ -1198,17 +1216,17 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B33" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33" s="3">
-        <v>436</v>
+        <v>288</v>
       </c>
       <c r="D33" s="7">
         <f>B33/C33</f>
-        <v>9.1743119266055051E-3</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E33" t="s">
         <v>75</v>
@@ -1216,17 +1234,17 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B34" s="3">
         <v>4</v>
       </c>
       <c r="C34" s="3">
-        <v>444</v>
+        <v>400</v>
       </c>
       <c r="D34" s="7">
         <f>B34/C34</f>
-        <v>9.0090090090090089E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E34" t="s">
         <v>75</v>
@@ -1234,17 +1252,17 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B35" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35" s="3">
-        <v>336</v>
+        <v>416</v>
       </c>
       <c r="D35" s="7">
         <f>B35/C35</f>
-        <v>8.9285714285714281E-3</v>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E35" t="s">
         <v>75</v>
@@ -1252,17 +1270,17 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="B36" s="3">
         <v>2</v>
       </c>
       <c r="C36" s="3">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="D36" s="7">
         <f>B36/C36</f>
-        <v>8.8888888888888889E-3</v>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E36" t="s">
         <v>75</v>
@@ -1270,17 +1288,17 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="B37" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C37" s="3">
-        <v>464</v>
+        <v>208</v>
       </c>
       <c r="D37" s="7">
         <f>B37/C37</f>
-        <v>8.6206896551724137E-3</v>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E37" t="s">
         <v>75</v>
@@ -1288,17 +1306,17 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B38" s="3">
         <v>4</v>
       </c>
       <c r="C38" s="3">
-        <v>464</v>
+        <v>432</v>
       </c>
       <c r="D38" s="7">
         <f>B38/C38</f>
-        <v>8.6206896551724137E-3</v>
+        <v>9.2592592592592587E-3</v>
       </c>
       <c r="E38" t="s">
         <v>75</v>
@@ -1306,17 +1324,17 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B39" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C39" s="3">
-        <v>352</v>
+        <v>436</v>
       </c>
       <c r="D39" s="7">
         <f>B39/C39</f>
-        <v>8.5227272727272721E-3</v>
+        <v>9.1743119266055051E-3</v>
       </c>
       <c r="E39" t="s">
         <v>75</v>
@@ -1324,17 +1342,17 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B40" s="3">
         <v>4</v>
       </c>
       <c r="C40" s="3">
-        <v>480</v>
+        <v>444</v>
       </c>
       <c r="D40" s="7">
         <f>B40/C40</f>
-        <v>8.3333333333333332E-3</v>
+        <v>9.0090090090090089E-3</v>
       </c>
       <c r="E40" t="s">
         <v>75</v>
@@ -1342,17 +1360,17 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B41" s="3">
         <v>3</v>
       </c>
       <c r="C41" s="3">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="D41" s="7">
         <f>B41/C41</f>
-        <v>8.3333333333333332E-3</v>
+        <v>8.9285714285714281E-3</v>
       </c>
       <c r="E41" t="s">
         <v>75</v>
@@ -1360,17 +1378,17 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="B42" s="3">
         <v>2</v>
       </c>
       <c r="C42" s="3">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="D42" s="7">
         <f>B42/C42</f>
-        <v>8.3333333333333332E-3</v>
+        <v>8.8888888888888889E-3</v>
       </c>
       <c r="E42" t="s">
         <v>75</v>
@@ -1378,17 +1396,17 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B43" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C43" s="3">
-        <v>368</v>
+        <v>464</v>
       </c>
       <c r="D43" s="7">
         <f>B43/C43</f>
-        <v>8.152173913043478E-3</v>
+        <v>8.6206896551724137E-3</v>
       </c>
       <c r="E43" t="s">
         <v>75</v>
@@ -1396,17 +1414,17 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="B44" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C44" s="3">
-        <v>368</v>
+        <v>464</v>
       </c>
       <c r="D44" s="7">
         <f>B44/C44</f>
-        <v>8.152173913043478E-3</v>
+        <v>8.6206896551724137E-3</v>
       </c>
       <c r="E44" t="s">
         <v>75</v>
@@ -1414,17 +1432,17 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B45" s="3">
         <v>3</v>
       </c>
       <c r="C45" s="3">
-        <v>371</v>
+        <v>352</v>
       </c>
       <c r="D45" s="7">
         <f>B45/C45</f>
-        <v>8.0862533692722376E-3</v>
+        <v>8.5227272727272721E-3</v>
       </c>
       <c r="E45" t="s">
         <v>75</v>
@@ -1432,17 +1450,17 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B46" s="3">
         <v>4</v>
       </c>
       <c r="C46" s="3">
-        <v>499</v>
+        <v>480</v>
       </c>
       <c r="D46" s="7">
         <f>B46/C46</f>
-        <v>8.0160320641282558E-3</v>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E46" t="s">
         <v>75</v>
@@ -1450,17 +1468,17 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B47" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" s="3">
-        <v>250</v>
+        <v>360</v>
       </c>
       <c r="D47" s="7">
         <f>B47/C47</f>
-        <v>8.0000000000000002E-3</v>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E47" t="s">
         <v>75</v>
@@ -1468,17 +1486,17 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B48" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C48" s="3">
-        <v>512</v>
+        <v>240</v>
       </c>
       <c r="D48" s="7">
         <f>B48/C48</f>
-        <v>7.8125E-3</v>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E48" t="s">
         <v>75</v>
@@ -1486,17 +1504,17 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="B49" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" s="3">
-        <v>512</v>
+        <v>368</v>
       </c>
       <c r="D49" s="7">
         <f>B49/C49</f>
-        <v>7.8125E-3</v>
+        <v>8.152173913043478E-3</v>
       </c>
       <c r="E49" t="s">
         <v>75</v>
@@ -1504,17 +1522,17 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B50" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C50" s="3">
-        <v>264</v>
+        <v>368</v>
       </c>
       <c r="D50" s="7">
         <f>B50/C50</f>
-        <v>7.575757575757576E-3</v>
+        <v>8.152173913043478E-3</v>
       </c>
       <c r="E50" t="s">
         <v>75</v>
@@ -1522,17 +1540,17 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="B51" s="3">
         <v>3</v>
       </c>
       <c r="C51" s="3">
-        <v>400</v>
+        <v>371</v>
       </c>
       <c r="D51" s="7">
         <f>B51/C51</f>
-        <v>7.4999999999999997E-3</v>
+        <v>8.0862533692722376E-3</v>
       </c>
       <c r="E51" t="s">
         <v>75</v>
@@ -1540,17 +1558,17 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="B52" s="3">
         <v>4</v>
       </c>
       <c r="C52" s="3">
-        <v>544</v>
+        <v>499</v>
       </c>
       <c r="D52" s="7">
         <f>B52/C52</f>
-        <v>7.3529411764705881E-3</v>
+        <v>8.0160320641282558E-3</v>
       </c>
       <c r="E52" t="s">
         <v>75</v>
@@ -1558,17 +1576,17 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B53" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C53" s="3">
-        <v>560</v>
+        <v>250</v>
       </c>
       <c r="D53" s="7">
         <f>B53/C53</f>
-        <v>7.1428571428571426E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E53" t="s">
         <v>75</v>
@@ -1576,17 +1594,17 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B54" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C54" s="3">
-        <v>284</v>
+        <v>512</v>
       </c>
       <c r="D54" s="7">
         <f>B54/C54</f>
-        <v>7.0422535211267607E-3</v>
+        <v>7.8125E-3</v>
       </c>
       <c r="E54" t="s">
         <v>75</v>
@@ -1594,17 +1612,17 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="B55" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C55" s="3">
-        <v>288</v>
+        <v>512</v>
       </c>
       <c r="D55" s="7">
         <f>B55/C55</f>
-        <v>6.9444444444444441E-3</v>
+        <v>7.8125E-3</v>
       </c>
       <c r="E55" t="s">
         <v>75</v>
@@ -1612,17 +1630,17 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B56" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" s="3">
-        <v>148</v>
+        <v>264</v>
       </c>
       <c r="D56" s="7">
         <f>B56/C56</f>
-        <v>6.7567567567567571E-3</v>
+        <v>7.575757575757576E-3</v>
       </c>
       <c r="E56" t="s">
         <v>75</v>
@@ -1630,17 +1648,17 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B57" s="3">
         <v>3</v>
       </c>
       <c r="C57" s="3">
-        <v>480</v>
+        <v>400</v>
       </c>
       <c r="D57" s="7">
         <f>B57/C57</f>
-        <v>6.2500000000000003E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E57" t="s">
         <v>75</v>
@@ -1648,17 +1666,17 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B58" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C58" s="3">
-        <v>480</v>
+        <v>544</v>
       </c>
       <c r="D58" s="7">
         <f>B58/C58</f>
-        <v>6.2500000000000003E-3</v>
+        <v>7.3529411764705881E-3</v>
       </c>
       <c r="E58" t="s">
         <v>75</v>
@@ -1666,17 +1684,17 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B59" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C59" s="3">
-        <v>488</v>
+        <v>560</v>
       </c>
       <c r="D59" s="7">
         <f>B59/C59</f>
-        <v>6.1475409836065573E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
       <c r="E59" t="s">
         <v>75</v>
@@ -1684,17 +1702,17 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B60" s="3">
         <v>2</v>
       </c>
       <c r="C60" s="3">
-        <v>332</v>
+        <v>284</v>
       </c>
       <c r="D60" s="7">
         <f>B60/C60</f>
-        <v>6.024096385542169E-3</v>
+        <v>7.0422535211267607E-3</v>
       </c>
       <c r="E60" t="s">
         <v>75</v>
@@ -1702,17 +1720,17 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B61" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C61" s="3">
-        <v>704</v>
+        <v>288</v>
       </c>
       <c r="D61" s="7">
         <f>B61/C61</f>
-        <v>5.681818181818182E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="E61" t="s">
         <v>75</v>
@@ -1720,17 +1738,17 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B62" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C62" s="3">
-        <v>736</v>
+        <v>148</v>
       </c>
       <c r="D62" s="7">
         <f>B62/C62</f>
-        <v>5.434782608695652E-3</v>
+        <v>6.7567567567567571E-3</v>
       </c>
       <c r="E62" t="s">
         <v>75</v>
@@ -1738,17 +1756,17 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B63" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63" s="3">
-        <v>373</v>
+        <v>480</v>
       </c>
       <c r="D63" s="7">
         <f>B63/C63</f>
-        <v>5.3619302949061663E-3</v>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E63" t="s">
         <v>75</v>
@@ -1756,17 +1774,17 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B64" s="3">
         <v>3</v>
       </c>
       <c r="C64" s="3">
-        <v>560</v>
+        <v>480</v>
       </c>
       <c r="D64" s="7">
         <f>B64/C64</f>
-        <v>5.3571428571428572E-3</v>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E64" t="s">
         <v>75</v>
@@ -1774,17 +1792,17 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B65" s="3">
         <v>3</v>
       </c>
       <c r="C65" s="3">
-        <v>560</v>
+        <v>488</v>
       </c>
       <c r="D65" s="7">
         <f>B65/C65</f>
-        <v>5.3571428571428572E-3</v>
+        <v>6.1475409836065573E-3</v>
       </c>
       <c r="E65" t="s">
         <v>75</v>
@@ -1792,17 +1810,17 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B66" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" s="3">
-        <v>576</v>
+        <v>332</v>
       </c>
       <c r="D66" s="7">
         <f>B66/C66</f>
-        <v>5.208333333333333E-3</v>
+        <v>6.024096385542169E-3</v>
       </c>
       <c r="E66" t="s">
         <v>75</v>
@@ -1810,17 +1828,17 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B67" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C67" s="3">
-        <v>384</v>
+        <v>704</v>
       </c>
       <c r="D67" s="7">
         <f>B67/C67</f>
-        <v>5.208333333333333E-3</v>
+        <v>5.681818181818182E-3</v>
       </c>
       <c r="E67" t="s">
         <v>75</v>
@@ -1828,17 +1846,17 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="B68" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C68" s="3">
-        <v>400</v>
+        <v>736</v>
       </c>
       <c r="D68" s="7">
         <f>B68/C68</f>
-        <v>5.0000000000000001E-3</v>
+        <v>5.434782608695652E-3</v>
       </c>
       <c r="E68" t="s">
         <v>75</v>
@@ -1846,17 +1864,17 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B69" s="3">
         <v>2</v>
       </c>
       <c r="C69" s="3">
-        <v>416</v>
+        <v>373</v>
       </c>
       <c r="D69" s="7">
         <f>B69/C69</f>
-        <v>4.807692307692308E-3</v>
+        <v>5.3619302949061663E-3</v>
       </c>
       <c r="E69" t="s">
         <v>75</v>
@@ -1864,17 +1882,17 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="B70" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C70" s="3">
-        <v>416</v>
+        <v>560</v>
       </c>
       <c r="D70" s="7">
         <f>B70/C70</f>
-        <v>4.807692307692308E-3</v>
+        <v>5.3571428571428572E-3</v>
       </c>
       <c r="E70" t="s">
         <v>75</v>
@@ -1882,17 +1900,17 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B71" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C71" s="3">
-        <v>528</v>
+        <v>560</v>
       </c>
       <c r="D71" s="7">
         <f>B71/C71</f>
-        <v>3.787878787878788E-3</v>
+        <v>5.3571428571428572E-3</v>
       </c>
       <c r="E71" t="s">
         <v>75</v>
@@ -1900,17 +1918,17 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B72" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C72" s="3">
-        <v>544</v>
+        <v>576</v>
       </c>
       <c r="D72" s="7">
         <f>B72/C72</f>
-        <v>3.6764705882352941E-3</v>
+        <v>5.208333333333333E-3</v>
       </c>
       <c r="E72" t="s">
         <v>75</v>
@@ -1918,17 +1936,17 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B73" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C73" s="3">
-        <v>848</v>
+        <v>384</v>
       </c>
       <c r="D73" s="7">
         <f>B73/C73</f>
-        <v>3.5377358490566039E-3</v>
+        <v>5.208333333333333E-3</v>
       </c>
       <c r="E73" t="s">
         <v>75</v>
@@ -1936,25 +1954,133 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B74" s="3">
         <v>2</v>
       </c>
       <c r="C74" s="3">
-        <v>616</v>
+        <v>400</v>
       </c>
       <c r="D74" s="7">
         <f>B74/C74</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E74" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" s="3">
+        <v>2</v>
+      </c>
+      <c r="C75" s="3">
+        <v>416</v>
+      </c>
+      <c r="D75" s="7">
+        <f>B75/C75</f>
+        <v>4.807692307692308E-3</v>
+      </c>
+      <c r="E75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B76" s="3">
+        <v>2</v>
+      </c>
+      <c r="C76" s="3">
+        <v>416</v>
+      </c>
+      <c r="D76" s="7">
+        <f>B76/C76</f>
+        <v>4.807692307692308E-3</v>
+      </c>
+      <c r="E76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B77" s="3">
+        <v>2</v>
+      </c>
+      <c r="C77" s="3">
+        <v>528</v>
+      </c>
+      <c r="D77" s="7">
+        <f>B77/C77</f>
+        <v>3.787878787878788E-3</v>
+      </c>
+      <c r="E77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B78" s="3">
+        <v>2</v>
+      </c>
+      <c r="C78" s="3">
+        <v>544</v>
+      </c>
+      <c r="D78" s="7">
+        <f>B78/C78</f>
+        <v>3.6764705882352941E-3</v>
+      </c>
+      <c r="E78" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79" s="3">
+        <v>3</v>
+      </c>
+      <c r="C79" s="3">
+        <v>848</v>
+      </c>
+      <c r="D79" s="7">
+        <f>B79/C79</f>
+        <v>3.5377358490566039E-3</v>
+      </c>
+      <c r="E79" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" s="3">
+        <v>2</v>
+      </c>
+      <c r="C80" s="3">
+        <v>616</v>
+      </c>
+      <c r="D80" s="7">
+        <f>B80/C80</f>
         <v>3.246753246753247E-3</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E80" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D70">
-    <sortState ref="A3:D74">
+    <sortState ref="A3:D80">
       <sortCondition descending="1" ref="D2:D70"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Reformatted 2018 books list
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="86">
   <si>
     <t>Book Ranking</t>
   </si>
@@ -157,9 +157,6 @@
     <t xml:space="preserve">Black Earth: The Holocaust as History and Warning  </t>
   </si>
   <si>
-    <t xml:space="preserve"> - The Gamble: General Petraeus and the American Military Adventure in Iraq  </t>
-  </si>
-  <si>
     <t>Wrapped in the Flag: A Personal History of America's Radical Right</t>
   </si>
   <si>
@@ -272,6 +269,12 @@
   </si>
   <si>
     <t>Letters from a Stoic</t>
+  </si>
+  <si>
+    <t>The Great Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Gamble: General Petraeus and the American Military Adventure in Iraq  </t>
   </si>
 </sst>
 </file>
@@ -318,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -331,6 +334,7 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,11 +639,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +675,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -685,16 +689,16 @@
         <v>46</v>
       </c>
       <c r="D3" s="7">
-        <f>B3/C3</f>
+        <f t="shared" ref="D3:D34" si="0">B3/C3</f>
         <v>8.6956521739130432E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -703,11 +707,11 @@
         <v>30</v>
       </c>
       <c r="D4" s="7">
-        <f>B4/C4</f>
+        <f t="shared" si="0"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -721,11 +725,11 @@
         <v>74</v>
       </c>
       <c r="D5" s="7">
-        <f>B5/C5</f>
+        <f t="shared" si="0"/>
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,16 +743,16 @@
         <v>120</v>
       </c>
       <c r="D6" s="7">
-        <f>B6/C6</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="3">
         <v>5</v>
@@ -757,16 +761,16 @@
         <v>133</v>
       </c>
       <c r="D7" s="7">
-        <f>B7/C7</f>
+        <f t="shared" si="0"/>
         <v>3.7593984962406013E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -775,11 +779,11 @@
         <v>132</v>
       </c>
       <c r="D8" s="7">
-        <f>B8/C8</f>
+        <f t="shared" si="0"/>
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -793,16 +797,16 @@
         <v>160</v>
       </c>
       <c r="D9" s="7">
-        <f>B9/C9</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="3">
         <v>2</v>
@@ -811,11 +815,11 @@
         <v>80</v>
       </c>
       <c r="D10" s="7">
-        <f>B10/C10</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -829,11 +833,11 @@
         <v>128</v>
       </c>
       <c r="D11" s="7">
-        <f>B11/C11</f>
+        <f t="shared" si="0"/>
         <v>2.34375E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -847,16 +851,16 @@
         <v>228</v>
       </c>
       <c r="D12" s="7">
-        <f>B12/C12</f>
+        <f t="shared" si="0"/>
         <v>2.1929824561403508E-2</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="3">
         <v>4</v>
@@ -865,11 +869,11 @@
         <v>191</v>
       </c>
       <c r="D13" s="7">
-        <f>B13/C13</f>
+        <f t="shared" si="0"/>
         <v>2.0942408376963352E-2</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -883,16 +887,16 @@
         <v>192</v>
       </c>
       <c r="D14" s="7">
-        <f>B14/C14</f>
+        <f t="shared" si="0"/>
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="3">
         <v>3</v>
@@ -901,16 +905,16 @@
         <v>160</v>
       </c>
       <c r="D15" s="7">
-        <f>B15/C15</f>
+        <f t="shared" si="0"/>
         <v>1.8749999999999999E-2</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="3">
         <v>4</v>
@@ -919,16 +923,16 @@
         <v>224</v>
       </c>
       <c r="D16" s="7">
-        <f>B16/C16</f>
+        <f t="shared" si="0"/>
         <v>1.7857142857142856E-2</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="3">
         <v>5</v>
@@ -937,16 +941,16 @@
         <v>288</v>
       </c>
       <c r="D17" s="7">
-        <f>B17/C17</f>
+        <f t="shared" si="0"/>
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" s="3">
         <v>4</v>
@@ -955,11 +959,11 @@
         <v>231</v>
       </c>
       <c r="D18" s="7">
-        <f>B18/C18</f>
+        <f t="shared" si="0"/>
         <v>1.7316017316017316E-2</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -973,11 +977,11 @@
         <v>182</v>
       </c>
       <c r="D19" s="7">
-        <f>B19/C19</f>
+        <f t="shared" si="0"/>
         <v>1.6483516483516484E-2</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -991,16 +995,16 @@
         <v>250</v>
       </c>
       <c r="D20" s="7">
-        <f>B20/C20</f>
+        <f t="shared" si="0"/>
         <v>1.6E-2</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="3">
         <v>5</v>
@@ -1009,16 +1013,16 @@
         <v>336</v>
       </c>
       <c r="D21" s="7">
-        <f>B21/C21</f>
+        <f t="shared" si="0"/>
         <v>1.488095238095238E-2</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="3">
         <v>4</v>
@@ -1027,11 +1031,11 @@
         <v>276</v>
       </c>
       <c r="D22" s="7">
-        <f>B22/C22</f>
+        <f t="shared" si="0"/>
         <v>1.4492753623188406E-2</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,16 +1049,16 @@
         <v>208</v>
       </c>
       <c r="D23" s="7">
-        <f>B23/C23</f>
+        <f t="shared" si="0"/>
         <v>1.4423076923076924E-2</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B24" s="3">
         <v>3</v>
@@ -1063,16 +1067,16 @@
         <v>213</v>
       </c>
       <c r="D24" s="7">
-        <f>B24/C24</f>
+        <f t="shared" si="0"/>
         <v>1.4084507042253521E-2</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="3">
         <v>5</v>
@@ -1081,16 +1085,16 @@
         <v>368</v>
       </c>
       <c r="D25" s="7">
-        <f>B25/C25</f>
+        <f t="shared" si="0"/>
         <v>1.358695652173913E-2</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" s="3">
         <v>4</v>
@@ -1099,16 +1103,16 @@
         <v>320</v>
       </c>
       <c r="D26" s="7">
-        <f>B26/C26</f>
+        <f t="shared" si="0"/>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="3">
         <v>4</v>
@@ -1117,11 +1121,11 @@
         <v>336</v>
       </c>
       <c r="D27" s="7">
-        <f>B27/C27</f>
+        <f t="shared" si="0"/>
         <v>1.1904761904761904E-2</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1135,16 +1139,16 @@
         <v>256</v>
       </c>
       <c r="D28" s="7">
-        <f>B28/C28</f>
+        <f t="shared" si="0"/>
         <v>1.171875E-2</v>
       </c>
       <c r="E28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B29" s="3">
         <v>5</v>
@@ -1153,16 +1157,16 @@
         <v>432</v>
       </c>
       <c r="D29" s="7">
-        <f>B29/C29</f>
+        <f t="shared" si="0"/>
         <v>1.1574074074074073E-2</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" s="3">
         <v>3</v>
@@ -1171,11 +1175,11 @@
         <v>264</v>
       </c>
       <c r="D30" s="7">
-        <f>B30/C30</f>
+        <f t="shared" si="0"/>
         <v>1.1363636363636364E-2</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1189,16 +1193,16 @@
         <v>384</v>
       </c>
       <c r="D31" s="7">
-        <f>B31/C31</f>
+        <f t="shared" si="0"/>
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="3">
         <v>4</v>
@@ -1207,11 +1211,11 @@
         <v>384</v>
       </c>
       <c r="D32" s="7">
-        <f>B32/C32</f>
+        <f t="shared" si="0"/>
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,11 +1229,11 @@
         <v>288</v>
       </c>
       <c r="D33" s="7">
-        <f>B33/C33</f>
+        <f t="shared" si="0"/>
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1243,16 +1247,16 @@
         <v>400</v>
       </c>
       <c r="D34" s="7">
-        <f>B34/C34</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="B35" s="3">
         <v>4</v>
@@ -1261,34 +1265,34 @@
         <v>416</v>
       </c>
       <c r="D35" s="7">
-        <f>B35/C35</f>
+        <f t="shared" ref="D35:D66" si="1">B35/C35</f>
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="8">
         <v>2</v>
       </c>
       <c r="C36" s="3">
         <v>208</v>
       </c>
       <c r="D36" s="7">
-        <f>B36/C36</f>
+        <f t="shared" si="1"/>
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="3">
         <v>2</v>
@@ -1297,16 +1301,16 @@
         <v>208</v>
       </c>
       <c r="D37" s="7">
-        <f>B37/C37</f>
+        <f t="shared" si="1"/>
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B38" s="3">
         <v>4</v>
@@ -1315,16 +1319,16 @@
         <v>432</v>
       </c>
       <c r="D38" s="7">
-        <f>B38/C38</f>
+        <f t="shared" si="1"/>
         <v>9.2592592592592587E-3</v>
       </c>
       <c r="E38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B39" s="3">
         <v>4</v>
@@ -1333,11 +1337,11 @@
         <v>436</v>
       </c>
       <c r="D39" s="7">
-        <f>B39/C39</f>
+        <f t="shared" si="1"/>
         <v>9.1743119266055051E-3</v>
       </c>
       <c r="E39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1351,16 +1355,16 @@
         <v>444</v>
       </c>
       <c r="D40" s="7">
-        <f>B40/C40</f>
+        <f t="shared" si="1"/>
         <v>9.0090090090090089E-3</v>
       </c>
       <c r="E40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="3">
         <v>3</v>
@@ -1369,16 +1373,16 @@
         <v>336</v>
       </c>
       <c r="D41" s="7">
-        <f>B41/C41</f>
+        <f t="shared" si="1"/>
         <v>8.9285714285714281E-3</v>
       </c>
       <c r="E41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B42" s="3">
         <v>2</v>
@@ -1387,11 +1391,11 @@
         <v>225</v>
       </c>
       <c r="D42" s="7">
-        <f>B42/C42</f>
+        <f t="shared" si="1"/>
         <v>8.8888888888888889E-3</v>
       </c>
       <c r="E42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1405,16 +1409,16 @@
         <v>464</v>
       </c>
       <c r="D43" s="7">
-        <f>B43/C43</f>
+        <f t="shared" si="1"/>
         <v>8.6206896551724137E-3</v>
       </c>
       <c r="E43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B44" s="3">
         <v>4</v>
@@ -1423,11 +1427,11 @@
         <v>464</v>
       </c>
       <c r="D44" s="7">
-        <f>B44/C44</f>
+        <f t="shared" si="1"/>
         <v>8.6206896551724137E-3</v>
       </c>
       <c r="E44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1441,11 +1445,11 @@
         <v>352</v>
       </c>
       <c r="D45" s="7">
-        <f>B45/C45</f>
+        <f t="shared" si="1"/>
         <v>8.5227272727272721E-3</v>
       </c>
       <c r="E45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1459,11 +1463,11 @@
         <v>480</v>
       </c>
       <c r="D46" s="7">
-        <f>B46/C46</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="E46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1477,11 +1481,11 @@
         <v>360</v>
       </c>
       <c r="D47" s="7">
-        <f>B47/C47</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="E47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1495,11 +1499,11 @@
         <v>240</v>
       </c>
       <c r="D48" s="7">
-        <f>B48/C48</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="E48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1513,11 +1517,11 @@
         <v>368</v>
       </c>
       <c r="D49" s="7">
-        <f>B49/C49</f>
+        <f t="shared" si="1"/>
         <v>8.152173913043478E-3</v>
       </c>
       <c r="E49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1531,11 +1535,11 @@
         <v>368</v>
       </c>
       <c r="D50" s="7">
-        <f>B50/C50</f>
+        <f t="shared" si="1"/>
         <v>8.152173913043478E-3</v>
       </c>
       <c r="E50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1549,11 +1553,11 @@
         <v>371</v>
       </c>
       <c r="D51" s="7">
-        <f>B51/C51</f>
+        <f t="shared" si="1"/>
         <v>8.0862533692722376E-3</v>
       </c>
       <c r="E51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1567,16 +1571,16 @@
         <v>499</v>
       </c>
       <c r="D52" s="7">
-        <f>B52/C52</f>
+        <f t="shared" si="1"/>
         <v>8.0160320641282558E-3</v>
       </c>
       <c r="E52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="3">
         <v>2</v>
@@ -1585,11 +1589,11 @@
         <v>250</v>
       </c>
       <c r="D53" s="7">
-        <f>B53/C53</f>
+        <f t="shared" si="1"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="E53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1603,16 +1607,16 @@
         <v>512</v>
       </c>
       <c r="D54" s="7">
-        <f>B54/C54</f>
+        <f t="shared" si="1"/>
         <v>7.8125E-3</v>
       </c>
       <c r="E54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B55" s="3">
         <v>4</v>
@@ -1621,16 +1625,16 @@
         <v>512</v>
       </c>
       <c r="D55" s="7">
-        <f>B55/C55</f>
+        <f t="shared" si="1"/>
         <v>7.8125E-3</v>
       </c>
       <c r="E55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B56" s="3">
         <v>2</v>
@@ -1639,16 +1643,16 @@
         <v>264</v>
       </c>
       <c r="D56" s="7">
-        <f>B56/C56</f>
+        <f t="shared" si="1"/>
         <v>7.575757575757576E-3</v>
       </c>
       <c r="E56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="3">
         <v>3</v>
@@ -1657,16 +1661,16 @@
         <v>400</v>
       </c>
       <c r="D57" s="7">
-        <f>B57/C57</f>
+        <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="E57" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B58" s="3">
         <v>4</v>
@@ -1675,11 +1679,11 @@
         <v>544</v>
       </c>
       <c r="D58" s="7">
-        <f>B58/C58</f>
+        <f t="shared" si="1"/>
         <v>7.3529411764705881E-3</v>
       </c>
       <c r="E58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1693,11 +1697,11 @@
         <v>560</v>
       </c>
       <c r="D59" s="7">
-        <f>B59/C59</f>
+        <f t="shared" si="1"/>
         <v>7.1428571428571426E-3</v>
       </c>
       <c r="E59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1711,16 +1715,16 @@
         <v>284</v>
       </c>
       <c r="D60" s="7">
-        <f>B60/C60</f>
+        <f t="shared" si="1"/>
         <v>7.0422535211267607E-3</v>
       </c>
       <c r="E60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B61" s="3">
         <v>2</v>
@@ -1729,16 +1733,16 @@
         <v>288</v>
       </c>
       <c r="D61" s="7">
-        <f>B61/C61</f>
+        <f t="shared" si="1"/>
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E61" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B62" s="3">
         <v>1</v>
@@ -1747,11 +1751,11 @@
         <v>148</v>
       </c>
       <c r="D62" s="7">
-        <f>B62/C62</f>
+        <f t="shared" si="1"/>
         <v>6.7567567567567571E-3</v>
       </c>
       <c r="E62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1765,11 +1769,11 @@
         <v>480</v>
       </c>
       <c r="D63" s="7">
-        <f>B63/C63</f>
+        <f t="shared" si="1"/>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="E63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1783,11 +1787,11 @@
         <v>480</v>
       </c>
       <c r="D64" s="7">
-        <f>B64/C64</f>
+        <f t="shared" si="1"/>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="E64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1801,16 +1805,16 @@
         <v>488</v>
       </c>
       <c r="D65" s="7">
-        <f>B65/C65</f>
+        <f t="shared" si="1"/>
         <v>6.1475409836065573E-3</v>
       </c>
       <c r="E65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="3">
         <v>2</v>
@@ -1819,11 +1823,11 @@
         <v>332</v>
       </c>
       <c r="D66" s="7">
-        <f>B66/C66</f>
+        <f t="shared" si="1"/>
         <v>6.024096385542169E-3</v>
       </c>
       <c r="E66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1837,16 +1841,16 @@
         <v>704</v>
       </c>
       <c r="D67" s="7">
-        <f>B67/C67</f>
+        <f t="shared" ref="D67:D98" si="2">B67/C67</f>
         <v>5.681818181818182E-3</v>
       </c>
       <c r="E67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B68" s="3">
         <v>4</v>
@@ -1855,11 +1859,11 @@
         <v>736</v>
       </c>
       <c r="D68" s="7">
-        <f>B68/C68</f>
+        <f t="shared" si="2"/>
         <v>5.434782608695652E-3</v>
       </c>
       <c r="E68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1873,11 +1877,11 @@
         <v>373</v>
       </c>
       <c r="D69" s="7">
-        <f>B69/C69</f>
+        <f t="shared" si="2"/>
         <v>5.3619302949061663E-3</v>
       </c>
       <c r="E69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1891,11 +1895,11 @@
         <v>560</v>
       </c>
       <c r="D70" s="7">
-        <f>B70/C70</f>
+        <f t="shared" si="2"/>
         <v>5.3571428571428572E-3</v>
       </c>
       <c r="E70" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1909,11 +1913,11 @@
         <v>560</v>
       </c>
       <c r="D71" s="7">
-        <f>B71/C71</f>
+        <f t="shared" si="2"/>
         <v>5.3571428571428572E-3</v>
       </c>
       <c r="E71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1927,11 +1931,11 @@
         <v>576</v>
       </c>
       <c r="D72" s="7">
-        <f>B72/C72</f>
+        <f t="shared" si="2"/>
         <v>5.208333333333333E-3</v>
       </c>
       <c r="E72" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1945,11 +1949,11 @@
         <v>384</v>
       </c>
       <c r="D73" s="7">
-        <f>B73/C73</f>
+        <f t="shared" si="2"/>
         <v>5.208333333333333E-3</v>
       </c>
       <c r="E73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1963,11 +1967,11 @@
         <v>400</v>
       </c>
       <c r="D74" s="7">
-        <f>B74/C74</f>
+        <f t="shared" si="2"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1981,16 +1985,16 @@
         <v>416</v>
       </c>
       <c r="D75" s="7">
-        <f>B75/C75</f>
+        <f t="shared" si="2"/>
         <v>4.807692307692308E-3</v>
       </c>
       <c r="E75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B76" s="3">
         <v>2</v>
@@ -1999,16 +2003,16 @@
         <v>416</v>
       </c>
       <c r="D76" s="7">
-        <f>B76/C76</f>
+        <f t="shared" si="2"/>
         <v>4.807692307692308E-3</v>
       </c>
       <c r="E76" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B77" s="3">
         <v>2</v>
@@ -2017,16 +2021,16 @@
         <v>528</v>
       </c>
       <c r="D77" s="7">
-        <f>B77/C77</f>
+        <f t="shared" si="2"/>
         <v>3.787878787878788E-3</v>
       </c>
       <c r="E77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B78" s="3">
         <v>2</v>
@@ -2035,11 +2039,11 @@
         <v>544</v>
       </c>
       <c r="D78" s="7">
-        <f>B78/C78</f>
+        <f t="shared" si="2"/>
         <v>3.6764705882352941E-3</v>
       </c>
       <c r="E78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2053,11 +2057,11 @@
         <v>848</v>
       </c>
       <c r="D79" s="7">
-        <f>B79/C79</f>
+        <f t="shared" si="2"/>
         <v>3.5377358490566039E-3</v>
       </c>
       <c r="E79" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2071,11 +2075,20 @@
         <v>616</v>
       </c>
       <c r="D80" s="7">
-        <f>B80/C80</f>
+        <f t="shared" si="2"/>
         <v>3.246753246753247E-3</v>
       </c>
       <c r="E80" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D81" s="7" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -2085,5 +2098,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added dropdown and added read selection
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$218</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="132">
   <si>
     <t>Book Ranking</t>
   </si>
@@ -407,6 +408,12 @@
   </si>
   <si>
     <t>The Ransom of Russian Art</t>
+  </si>
+  <si>
+    <t>Book Read</t>
+  </si>
+  <si>
+    <t>Yes (Reading Again)</t>
   </si>
 </sst>
 </file>
@@ -771,11 +778,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E124"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,6 +791,7 @@
     <col min="1" max="1" width="125.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -810,7 +819,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
@@ -2354,6 +2363,9 @@
         <f t="shared" si="2"/>
         <v>5.3619302949061663E-3</v>
       </c>
+      <c r="E88" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
@@ -2405,6 +2417,9 @@
         <f t="shared" si="2"/>
         <v>5.208333333333333E-3</v>
       </c>
+      <c r="E91" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
@@ -2420,6 +2435,9 @@
         <f t="shared" si="2"/>
         <v>5.208333333333333E-3</v>
       </c>
+      <c r="E92" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
@@ -2435,6 +2453,9 @@
         <f t="shared" si="2"/>
         <v>5.0000000000000001E-3</v>
       </c>
+      <c r="E93" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
@@ -2450,6 +2471,9 @@
         <f t="shared" si="2"/>
         <v>5.0000000000000001E-3</v>
       </c>
+      <c r="E94" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
@@ -2465,6 +2489,9 @@
         <f t="shared" si="2"/>
         <v>4.807692307692308E-3</v>
       </c>
+      <c r="E95" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
@@ -2480,8 +2507,11 @@
         <f t="shared" si="2"/>
         <v>4.807692307692308E-3</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>100</v>
       </c>
@@ -2495,8 +2525,11 @@
         <f t="shared" si="2"/>
         <v>4.7169811320754715E-3</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>106</v>
       </c>
@@ -2510,8 +2543,11 @@
         <f t="shared" si="2"/>
         <v>4.3859649122807015E-3</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>47</v>
       </c>
@@ -2525,8 +2561,11 @@
         <f t="shared" ref="D99:D124" si="3">B99/C99</f>
         <v>3.787878787878788E-3</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>62</v>
       </c>
@@ -2540,8 +2579,11 @@
         <f t="shared" si="3"/>
         <v>3.6764705882352941E-3</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>23</v>
       </c>
@@ -2555,8 +2597,11 @@
         <f t="shared" si="3"/>
         <v>3.5377358490566039E-3</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>102</v>
       </c>
@@ -2570,8 +2615,11 @@
         <f t="shared" si="3"/>
         <v>3.472222222222222E-3</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>6</v>
       </c>
@@ -2585,8 +2633,11 @@
         <f t="shared" si="3"/>
         <v>3.246753246753247E-3</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>99</v>
       </c>
@@ -2600,8 +2651,11 @@
         <f t="shared" si="3"/>
         <v>3.1250000000000002E-3</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>91</v>
       </c>
@@ -2612,188 +2666,861 @@
         <v>1280</v>
       </c>
       <c r="D105" s="7">
-        <f t="shared" si="3"/>
+        <f>IFERROR(B105/C105," ")</f>
         <v>2.3437499999999999E-3</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D106" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="7" t="str">
+        <f>IFERROR(B106/C106," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E106" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D107" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="7" t="str">
+        <f t="shared" ref="D107:D170" si="4">IFERROR(B107/C107," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E107" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D108" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E108" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D109" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E109" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D110" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E110" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D111" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E111" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D112" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E112" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D113" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E113" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D114" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E114" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D115" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E115" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D116" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E116" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D117" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E117" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D118" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E118" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D119" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E119" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D120" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D120" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E120" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D121" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D121" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E121" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D122" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E122" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D123" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E123" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D124" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="D124" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E124" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D125" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D126" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D127" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D128" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D130" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D131" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D132" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D133" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D134" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D135" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D136" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D137" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D138" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D139" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D140" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D141" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D142" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D143" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D144" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D148" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D149" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D150" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D151" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D152" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D153" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D154" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D155" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D156" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D157" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D158" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D159" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D160" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D161" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D162" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D163" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D164" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D165" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D166" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D167" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D168" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D169" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D170" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D171" s="7" t="str">
+        <f t="shared" ref="D171:D218" si="5">IFERROR(B171/C171," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D172" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D173" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D174" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D175" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D176" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D177" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D178" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D179" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D180" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D181" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D182" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D183" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D184" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D185" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D186" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D187" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D188" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D189" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D190" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D191" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D192" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D193" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D194" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D195" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D196" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D197" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D198" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D199" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D200" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D201" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D202" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D203" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D204" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D205" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D206" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D207" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D208" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D209" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D210" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D211" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D212" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D213" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D214" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D215" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D216" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D217" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D218" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D70">
-    <sortState ref="A3:D105">
-      <sortCondition descending="1" ref="D2:D70"/>
-    </sortState>
+  <autoFilter ref="A2:E218">
+    <filterColumn colId="4">
+      <filters blank="1">
+        <filter val="No"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E138</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added elements of journalism
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="133">
   <si>
     <t>Book Ranking</t>
   </si>
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>Yes (Reading Again)</t>
+  </si>
+  <si>
+    <t>The Elements of Journalism</t>
   </si>
 </sst>
 </file>
@@ -779,11 +782,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E218"/>
+  <dimension ref="A1:E219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="2" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,7 +2561,7 @@
         <v>528</v>
       </c>
       <c r="D99" s="7">
-        <f t="shared" ref="D99:D124" si="3">B99/C99</f>
+        <f t="shared" ref="D99:D104" si="3">B99/C99</f>
         <v>3.787878787878788E-3</v>
       </c>
       <c r="E99" t="s">
@@ -2902,9 +2905,15 @@
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D125" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
+      </c>
+      <c r="E125" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3179,7 +3188,7 @@
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D171" s="7" t="str">
-        <f t="shared" ref="D171:D218" si="5">IFERROR(B171/C171," ")</f>
+        <f t="shared" ref="D171:D219" si="5">IFERROR(B171/C171," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3461,6 +3470,12 @@
     </row>
     <row r="218" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D218" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D219" s="7" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
@@ -3468,7 +3483,7 @@
   </sheetData>
   <autoFilter ref="A2:E218">
     <filterColumn colId="4">
-      <filters blank="1">
+      <filters>
         <filter val="No"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Added Monk's guide to a clean house
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="134">
   <si>
     <t>Book Ranking</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>The Elements of Journalism</t>
+  </si>
+  <si>
+    <t>A Monk's Guide to a Clean House</t>
   </si>
 </sst>
 </file>
@@ -785,8 +788,8 @@
   <dimension ref="A1:E219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E125" sqref="E125"/>
+      <pane ySplit="2" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A126" sqref="A126:E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2917,9 +2920,15 @@
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>133</v>
+      </c>
       <c r="D126" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>IFERROR(B126/C126," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E126" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3188,7 +3197,7 @@
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D171" s="7" t="str">
-        <f t="shared" ref="D171:D219" si="5">IFERROR(B171/C171," ")</f>
+        <f t="shared" ref="D171:D220" si="5">IFERROR(B171/C171," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3497,7 +3506,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E138</xm:sqref>
+          <xm:sqref>E3:E125 E127:E138</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Spell check on book list
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -59,9 +59,6 @@
     <t>The Gnostic Gospels.</t>
   </si>
   <si>
-    <t>Empire of the Summer Moon: Quanah Parker and the Rise and Fall of the Comanches, the Most Powerful</t>
-  </si>
-  <si>
     <t>How Music Works</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t xml:space="preserve">Living Buddha, Living Christ 10th Anniversary Edition  </t>
   </si>
   <si>
-    <t xml:space="preserve">The Gnôsis of the Light  </t>
-  </si>
-  <si>
     <t xml:space="preserve">On the Decay of the Art of Lying  </t>
   </si>
   <si>
@@ -245,9 +239,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Bringin up Bebe</t>
-  </si>
-  <si>
     <t>Fiasco</t>
   </si>
   <si>
@@ -284,9 +275,6 @@
     <t>The Elements of Zen</t>
   </si>
   <si>
-    <t>Dr. Suess: American Icon</t>
-  </si>
-  <si>
     <t>Myths to Live By</t>
   </si>
   <si>
@@ -329,9 +317,6 @@
     <t>A Global History of Architecture</t>
   </si>
   <si>
-    <t>A Pictoral History of the Great Lakes</t>
-  </si>
-  <si>
     <t>Mooney</t>
   </si>
   <si>
@@ -398,9 +383,6 @@
     <t>The First World War (Strachan)</t>
   </si>
   <si>
-    <t>Solderi from the Wars Returning (Carrington)</t>
-  </si>
-  <si>
     <t>The New Knighthood</t>
   </si>
   <si>
@@ -420,6 +402,24 @@
   </si>
   <si>
     <t>A Monk's Guide to a Clean House</t>
+  </si>
+  <si>
+    <t>Soldier from the Wars Returning (Carrington)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Gnosis of the Light  </t>
+  </si>
+  <si>
+    <t>Dr. Seuss: American Icon</t>
+  </si>
+  <si>
+    <t>Bringing up Bebe</t>
+  </si>
+  <si>
+    <t>Empire of the Summer Moon: Quanah Parker and the Rise and Fall of the Comanche's, the Most Powerful</t>
+  </si>
+  <si>
+    <t>A Pictorial History of the Great Lakes</t>
   </si>
 </sst>
 </file>
@@ -788,8 +788,8 @@
   <dimension ref="A1:E219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A126" sqref="A126:E126"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,12 +822,12 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -840,12 +840,12 @@
         <v>8.6956521739130432E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B4" s="3">
         <v>5</v>
@@ -858,12 +858,12 @@
         <v>6.8493150684931503E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -876,12 +876,12 @@
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3">
         <v>4</v>
@@ -894,12 +894,12 @@
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3">
         <v>5</v>
@@ -912,12 +912,12 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -930,12 +930,12 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B9" s="3">
         <v>5</v>
@@ -948,12 +948,12 @@
         <v>3.7593984962406013E-2</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3">
         <v>4</v>
@@ -966,12 +966,12 @@
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
@@ -984,12 +984,12 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -1002,12 +1002,12 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -1020,12 +1020,12 @@
         <v>2.4193548387096774E-2</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3">
         <v>3</v>
@@ -1038,12 +1038,12 @@
         <v>2.34375E-2</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -1056,12 +1056,12 @@
         <v>2.1929824561403508E-2</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B16" s="3">
         <v>4</v>
@@ -1074,12 +1074,12 @@
         <v>2.0942408376963352E-2</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="3">
         <v>4</v>
@@ -1092,12 +1092,12 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>88</v>
+        <v>130</v>
       </c>
       <c r="B18" s="3">
         <v>4</v>
@@ -1110,12 +1110,12 @@
         <v>2.0202020202020204E-2</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B19" s="3">
         <v>5</v>
@@ -1128,12 +1128,12 @@
         <v>1.937984496124031E-2</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B20" s="3">
         <v>3</v>
@@ -1146,12 +1146,12 @@
         <v>1.9108280254777069E-2</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="3">
         <v>3</v>
@@ -1164,12 +1164,12 @@
         <v>1.8749999999999999E-2</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B22" s="3">
         <v>4</v>
@@ -1182,12 +1182,12 @@
         <v>1.7857142857142856E-2</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B23" s="3">
         <v>4</v>
@@ -1200,12 +1200,12 @@
         <v>1.7699115044247787E-2</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24" s="3">
         <v>5</v>
@@ -1218,12 +1218,12 @@
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B25" s="3">
         <v>4</v>
@@ -1236,7 +1236,7 @@
         <v>1.7316017316017316E-2</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1254,12 +1254,12 @@
         <v>1.6483516483516484E-2</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="3">
         <v>4</v>
@@ -1272,12 +1272,12 @@
         <v>1.6E-2</v>
       </c>
       <c r="E27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B28" s="3">
         <v>4</v>
@@ -1290,12 +1290,12 @@
         <v>1.5037593984962405E-2</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="3">
         <v>5</v>
@@ -1308,12 +1308,12 @@
         <v>1.488095238095238E-2</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B30" s="3">
         <v>2</v>
@@ -1326,12 +1326,12 @@
         <v>1.4598540145985401E-2</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B31" s="3">
         <v>4</v>
@@ -1344,12 +1344,12 @@
         <v>1.4492753623188406E-2</v>
       </c>
       <c r="E31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="3">
         <v>3</v>
@@ -1362,12 +1362,12 @@
         <v>1.4423076923076924E-2</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B33" s="3">
         <v>3</v>
@@ -1380,12 +1380,12 @@
         <v>1.4084507042253521E-2</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" s="3">
         <v>5</v>
@@ -1398,12 +1398,12 @@
         <v>1.358695652173913E-2</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" s="3">
         <v>4</v>
@@ -1416,12 +1416,12 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B36" s="3">
         <v>2</v>
@@ -1434,12 +1434,12 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B37" s="3">
         <v>4</v>
@@ -1452,12 +1452,12 @@
         <v>1.1904761904761904E-2</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B38" s="3">
         <v>3</v>
@@ -1470,12 +1470,12 @@
         <v>1.171875E-2</v>
       </c>
       <c r="E38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B39" s="3">
         <v>5</v>
@@ -1488,12 +1488,12 @@
         <v>1.1574074074074073E-2</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="3">
         <v>3</v>
@@ -1506,12 +1506,12 @@
         <v>1.1363636363636364E-2</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B41" s="3">
         <v>3</v>
@@ -1524,12 +1524,12 @@
         <v>1.1278195488721804E-2</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B42" s="3">
         <v>3</v>
@@ -1542,12 +1542,12 @@
         <v>1.0830324909747292E-2</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B43" s="3">
         <v>4</v>
@@ -1560,12 +1560,12 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B44" s="3">
         <v>4</v>
@@ -1578,12 +1578,12 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="3">
         <v>3</v>
@@ -1596,12 +1596,12 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B46" s="3">
         <v>4</v>
@@ -1614,12 +1614,12 @@
         <v>0.01</v>
       </c>
       <c r="E46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B47" s="3">
         <v>2</v>
@@ -1632,12 +1632,12 @@
         <v>0.01</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B48" s="3">
         <v>4</v>
@@ -1650,12 +1650,12 @@
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B49" s="8">
         <v>2</v>
@@ -1668,12 +1668,12 @@
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B50" s="3">
         <v>2</v>
@@ -1686,12 +1686,12 @@
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E50" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B51" s="3">
         <v>3</v>
@@ -1704,12 +1704,12 @@
         <v>9.4936708860759497E-3</v>
       </c>
       <c r="E51" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="B52" s="3">
         <v>4</v>
@@ -1722,12 +1722,12 @@
         <v>9.2592592592592587E-3</v>
       </c>
       <c r="E52" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" s="3">
         <v>4</v>
@@ -1740,7 +1740,7 @@
         <v>9.1743119266055051E-3</v>
       </c>
       <c r="E53" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1758,12 +1758,12 @@
         <v>9.0090090090090089E-3</v>
       </c>
       <c r="E54" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" s="3">
         <v>3</v>
@@ -1776,12 +1776,12 @@
         <v>8.9285714285714281E-3</v>
       </c>
       <c r="E55" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B56" s="3">
         <v>2</v>
@@ -1794,12 +1794,12 @@
         <v>8.8888888888888889E-3</v>
       </c>
       <c r="E56" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B57" s="3">
         <v>3</v>
@@ -1812,7 +1812,7 @@
         <v>8.7209302325581394E-3</v>
       </c>
       <c r="E57" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1830,12 +1830,12 @@
         <v>8.6206896551724137E-3</v>
       </c>
       <c r="E58" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B59" s="3">
         <v>4</v>
@@ -1848,12 +1848,12 @@
         <v>8.6206896551724137E-3</v>
       </c>
       <c r="E59" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B60" s="3">
         <v>3</v>
@@ -1866,12 +1866,12 @@
         <v>8.5227272727272721E-3</v>
       </c>
       <c r="E60" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B61" s="3">
         <v>4</v>
@@ -1884,12 +1884,12 @@
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="E61" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B62" s="3">
         <v>3</v>
@@ -1902,7 +1902,7 @@
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="E62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1920,7 +1920,7 @@
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="E63" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1938,12 +1938,12 @@
         <v>8.152173913043478E-3</v>
       </c>
       <c r="E64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B65" s="3">
         <v>3</v>
@@ -1956,12 +1956,12 @@
         <v>8.152173913043478E-3</v>
       </c>
       <c r="E65" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="B66" s="3">
         <v>3</v>
@@ -1974,7 +1974,7 @@
         <v>8.0862533692722376E-3</v>
       </c>
       <c r="E66" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1992,12 +1992,12 @@
         <v>8.0160320641282558E-3</v>
       </c>
       <c r="E67" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B68" s="3">
         <v>2</v>
@@ -2010,12 +2010,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="E68" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B69" s="3">
         <v>4</v>
@@ -2028,12 +2028,12 @@
         <v>7.8125E-3</v>
       </c>
       <c r="E69" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B70" s="3">
         <v>4</v>
@@ -2046,12 +2046,12 @@
         <v>7.8125E-3</v>
       </c>
       <c r="E70" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B71" s="3">
         <v>2</v>
@@ -2064,12 +2064,12 @@
         <v>7.575757575757576E-3</v>
       </c>
       <c r="E71" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B72" s="3">
         <v>3</v>
@@ -2082,12 +2082,12 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="E72" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B73" s="3">
         <v>4</v>
@@ -2100,12 +2100,12 @@
         <v>7.3529411764705881E-3</v>
       </c>
       <c r="E73" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B74" s="3">
         <v>4</v>
@@ -2118,7 +2118,7 @@
         <v>7.1428571428571426E-3</v>
       </c>
       <c r="E74" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2136,12 +2136,12 @@
         <v>7.0422535211267607E-3</v>
       </c>
       <c r="E75" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B76" s="3">
         <v>2</v>
@@ -2154,12 +2154,12 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E76" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B77" s="3">
         <v>1</v>
@@ -2172,12 +2172,12 @@
         <v>6.7567567567567571E-3</v>
       </c>
       <c r="E77" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B78" s="3">
         <v>3</v>
@@ -2190,12 +2190,12 @@
         <v>6.6666666666666671E-3</v>
       </c>
       <c r="E78" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B79" s="3">
         <v>3</v>
@@ -2208,12 +2208,12 @@
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="E79" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B80" s="3">
         <v>3</v>
@@ -2226,12 +2226,12 @@
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="E80" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B81" s="3">
         <v>3</v>
@@ -2244,12 +2244,12 @@
         <v>6.1475409836065573E-3</v>
       </c>
       <c r="E81" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B82" s="3">
         <v>2</v>
@@ -2262,12 +2262,12 @@
         <v>6.024096385542169E-3</v>
       </c>
       <c r="E82" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B83" s="3">
         <v>2</v>
@@ -2280,12 +2280,12 @@
         <v>6.024096385542169E-3</v>
       </c>
       <c r="E83" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="B84" s="3">
         <v>2</v>
@@ -2298,12 +2298,12 @@
         <v>5.8139534883720929E-3</v>
       </c>
       <c r="E84" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B85" s="3">
         <v>4</v>
@@ -2316,12 +2316,12 @@
         <v>5.681818181818182E-3</v>
       </c>
       <c r="E85" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B86" s="3">
         <v>2</v>
@@ -2334,12 +2334,12 @@
         <v>5.4644808743169399E-3</v>
       </c>
       <c r="E86" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B87" s="3">
         <v>4</v>
@@ -2352,12 +2352,12 @@
         <v>5.434782608695652E-3</v>
       </c>
       <c r="E87" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B88" s="3">
         <v>2</v>
@@ -2370,12 +2370,12 @@
         <v>5.3619302949061663E-3</v>
       </c>
       <c r="E88" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B89" s="3">
         <v>3</v>
@@ -2388,12 +2388,12 @@
         <v>5.3571428571428572E-3</v>
       </c>
       <c r="E89" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B90" s="3">
         <v>3</v>
@@ -2406,12 +2406,12 @@
         <v>5.3571428571428572E-3</v>
       </c>
       <c r="E90" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B91" s="3">
         <v>3</v>
@@ -2424,12 +2424,12 @@
         <v>5.208333333333333E-3</v>
       </c>
       <c r="E91" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B92" s="3">
         <v>2</v>
@@ -2442,12 +2442,12 @@
         <v>5.208333333333333E-3</v>
       </c>
       <c r="E92" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B93" s="3">
         <v>1</v>
@@ -2460,12 +2460,12 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E93" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B94" s="3">
         <v>2</v>
@@ -2478,12 +2478,12 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E94" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B95" s="3">
         <v>2</v>
@@ -2496,12 +2496,12 @@
         <v>4.807692307692308E-3</v>
       </c>
       <c r="E95" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B96" s="3">
         <v>2</v>
@@ -2514,12 +2514,12 @@
         <v>4.807692307692308E-3</v>
       </c>
       <c r="E96" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B97" s="3">
         <v>4</v>
@@ -2532,12 +2532,12 @@
         <v>4.7169811320754715E-3</v>
       </c>
       <c r="E97" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B98" s="3">
         <v>2</v>
@@ -2550,12 +2550,12 @@
         <v>4.3859649122807015E-3</v>
       </c>
       <c r="E98" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B99" s="3">
         <v>2</v>
@@ -2568,12 +2568,12 @@
         <v>3.787878787878788E-3</v>
       </c>
       <c r="E99" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B100" s="3">
         <v>2</v>
@@ -2586,12 +2586,12 @@
         <v>3.6764705882352941E-3</v>
       </c>
       <c r="E100" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B101" s="3">
         <v>3</v>
@@ -2604,12 +2604,12 @@
         <v>3.5377358490566039E-3</v>
       </c>
       <c r="E101" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B102" s="3">
         <v>3</v>
@@ -2622,7 +2622,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="E102" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2640,12 +2640,12 @@
         <v>3.246753246753247E-3</v>
       </c>
       <c r="E103" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B104" s="3">
         <v>1</v>
@@ -2658,12 +2658,12 @@
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="E104" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B105" s="3">
         <v>3</v>
@@ -2676,259 +2676,259 @@
         <v>2.3437499999999999E-3</v>
       </c>
       <c r="E105" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D106" s="7" t="str">
         <f>IFERROR(B106/C106," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E106" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D107" s="7" t="str">
         <f t="shared" ref="D107:D170" si="4">IFERROR(B107/C107," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E107" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D108" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E108" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D109" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E109" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D110" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E110" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D111" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E111" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D112" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E112" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D113" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E113" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D114" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E114" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D115" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E115" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D116" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E116" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D117" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E117" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D118" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E118" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D119" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E119" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D120" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E120" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D121" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E121" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D122" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E122" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D123" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E123" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D124" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E124" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D125" s="7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E125" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D126" s="7" t="str">
         <f>IFERROR(B126/C126," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E126" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3197,7 +3197,7 @@
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D171" s="7" t="str">
-        <f t="shared" ref="D171:D220" si="5">IFERROR(B171/C171," ")</f>
+        <f t="shared" ref="D171:D219" si="5">IFERROR(B171/C171," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3526,22 +3526,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added page numbers and values to book ranking
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -797,8 +797,8 @@
   <dimension ref="A1:E219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E129" sqref="E129"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,181 +852,151 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="B4" s="3">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3">
-        <v>73</v>
-      </c>
-      <c r="D4" s="7">
-        <f t="shared" si="0"/>
-        <v>6.8493150684931503E-2</v>
+        <v>2</v>
+      </c>
+      <c r="D4" s="7" t="str">
+        <f>IFERROR(B4/C4," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="3">
-        <v>30</v>
-      </c>
-      <c r="D5" s="7">
-        <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
+      <c r="D5" s="7" t="str">
+        <f>IFERROR(B5/C5," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="B6" s="3">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3">
-        <v>74</v>
-      </c>
-      <c r="D6" s="7">
-        <f t="shared" si="0"/>
-        <v>5.4054054054054057E-2</v>
+        <v>2</v>
+      </c>
+      <c r="D6" s="7" t="str">
+        <f>IFERROR(B6/C6," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="B7" s="3">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f>IFERROR(B7/C7," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7" t="str">
+        <f>IFERROR(B8/C8," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7" t="str">
+        <f>IFERROR(B9/C9," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7" t="str">
+        <f>IFERROR(B10/C10," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7" t="str">
+        <f>IFERROR(B11/C11," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="7">
-        <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="3">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3">
-        <v>72</v>
-      </c>
-      <c r="D8" s="7">
-        <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="3">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3">
-        <v>133</v>
-      </c>
-      <c r="D9" s="7">
-        <f t="shared" si="0"/>
-        <v>3.7593984962406013E-2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="3">
-        <v>4</v>
-      </c>
-      <c r="C10" s="3">
-        <v>132</v>
-      </c>
-      <c r="D10" s="7">
-        <f t="shared" si="0"/>
-        <v>3.0303030303030304E-2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="3">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3">
-        <v>160</v>
-      </c>
-      <c r="D11" s="7">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="3">
-        <v>80</v>
-      </c>
-      <c r="D12" s="7">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+      <c r="D12" s="7" t="str">
+        <f>IFERROR(B12/C12," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="B13" s="3">
-        <v>3</v>
-      </c>
-      <c r="C13" s="3">
-        <v>124</v>
-      </c>
-      <c r="D13" s="7">
-        <f t="shared" si="0"/>
-        <v>2.4193548387096774E-2</v>
+        <v>2</v>
+      </c>
+      <c r="D13" s="7" t="str">
+        <f>IFERROR(B13/C13," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E13" t="s">
         <v>72</v>
@@ -1034,17 +1004,17 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="B14" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C14" s="3">
-        <v>128</v>
+        <v>73</v>
       </c>
       <c r="D14" s="7">
-        <f t="shared" si="0"/>
-        <v>2.34375E-2</v>
+        <f>B14/C14</f>
+        <v>6.8493150684931503E-2</v>
       </c>
       <c r="E14" t="s">
         <v>72</v>
@@ -1052,17 +1022,17 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B15" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C15" s="3">
-        <v>228</v>
+        <v>30</v>
       </c>
       <c r="D15" s="7">
-        <f t="shared" si="0"/>
-        <v>2.1929824561403508E-2</v>
+        <f>B15/C15</f>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="E15" t="s">
         <v>72</v>
@@ -1070,17 +1040,17 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3">
         <v>4</v>
       </c>
       <c r="C16" s="3">
-        <v>191</v>
+        <v>74</v>
       </c>
       <c r="D16" s="7">
-        <f t="shared" si="0"/>
-        <v>2.0942408376963352E-2</v>
+        <f>B16/C16</f>
+        <v>5.4054054054054057E-2</v>
       </c>
       <c r="E16" t="s">
         <v>72</v>
@@ -1088,17 +1058,17 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" s="3">
-        <v>192</v>
+        <v>120</v>
       </c>
       <c r="D17" s="7">
-        <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <f>B17/C17</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E17" t="s">
         <v>72</v>
@@ -1106,17 +1076,17 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="B18" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="3">
-        <v>198</v>
+        <v>72</v>
       </c>
       <c r="D18" s="7">
-        <f t="shared" si="0"/>
-        <v>2.0202020202020204E-2</v>
+        <f>B18/C18</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E18" t="s">
         <v>72</v>
@@ -1124,17 +1094,17 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
       <c r="B19" s="3">
         <v>5</v>
       </c>
       <c r="C19" s="3">
-        <v>258</v>
+        <v>128</v>
       </c>
       <c r="D19" s="7">
-        <f t="shared" si="0"/>
-        <v>1.937984496124031E-2</v>
+        <f>IFERROR(B19/C19," ")</f>
+        <v>3.90625E-2</v>
       </c>
       <c r="E19" t="s">
         <v>72</v>
@@ -1142,17 +1112,17 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="B20" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C20" s="3">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="D20" s="7">
-        <f t="shared" si="0"/>
-        <v>1.9108280254777069E-2</v>
+        <f>B20/C20</f>
+        <v>3.7593984962406013E-2</v>
       </c>
       <c r="E20" t="s">
         <v>72</v>
@@ -1160,17 +1130,17 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21" s="3">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="D21" s="7">
-        <f t="shared" si="0"/>
-        <v>1.8749999999999999E-2</v>
+        <f>B21/C21</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="E21" t="s">
         <v>72</v>
@@ -1178,17 +1148,17 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B22" s="3">
         <v>4</v>
       </c>
       <c r="C22" s="3">
-        <v>224</v>
+        <v>160</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" si="0"/>
-        <v>1.7857142857142856E-2</v>
+        <f>B22/C22</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E22" t="s">
         <v>72</v>
@@ -1196,17 +1166,17 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="B23" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23" s="3">
-        <v>226</v>
+        <v>80</v>
       </c>
       <c r="D23" s="7">
-        <f t="shared" si="0"/>
-        <v>1.7699115044247787E-2</v>
+        <f>B23/C23</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E23" t="s">
         <v>72</v>
@@ -1214,17 +1184,17 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B24" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C24" s="3">
-        <v>288</v>
+        <v>124</v>
       </c>
       <c r="D24" s="7">
-        <f t="shared" si="0"/>
-        <v>1.7361111111111112E-2</v>
+        <f>B24/C24</f>
+        <v>2.4193548387096774E-2</v>
       </c>
       <c r="E24" t="s">
         <v>72</v>
@@ -1232,17 +1202,17 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="B25" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" s="3">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="D25" s="7">
-        <f t="shared" si="0"/>
-        <v>1.7316017316017316E-2</v>
+        <f>IFERROR(B25/C25," ")</f>
+        <v>2.403846153846154E-2</v>
       </c>
       <c r="E25" t="s">
         <v>72</v>
@@ -1250,17 +1220,17 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B26" s="3">
         <v>3</v>
       </c>
       <c r="C26" s="3">
-        <v>182</v>
+        <v>128</v>
       </c>
       <c r="D26" s="7">
-        <f t="shared" si="0"/>
-        <v>1.6483516483516484E-2</v>
+        <f>B26/C26</f>
+        <v>2.34375E-2</v>
       </c>
       <c r="E26" t="s">
         <v>72</v>
@@ -1268,17 +1238,17 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B27" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C27" s="3">
-        <v>250</v>
+        <v>228</v>
       </c>
       <c r="D27" s="7">
-        <f t="shared" si="0"/>
-        <v>1.6E-2</v>
+        <f>B27/C27</f>
+        <v>2.1929824561403508E-2</v>
       </c>
       <c r="E27" t="s">
         <v>72</v>
@@ -1286,17 +1256,17 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B28" s="3">
         <v>4</v>
       </c>
       <c r="C28" s="3">
-        <v>266</v>
+        <v>191</v>
       </c>
       <c r="D28" s="7">
-        <f t="shared" si="0"/>
-        <v>1.5037593984962405E-2</v>
+        <f>B28/C28</f>
+        <v>2.0942408376963352E-2</v>
       </c>
       <c r="E28" t="s">
         <v>72</v>
@@ -1304,17 +1274,17 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B29" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="3">
-        <v>336</v>
+        <v>192</v>
       </c>
       <c r="D29" s="7">
-        <f t="shared" si="0"/>
-        <v>1.488095238095238E-2</v>
+        <f>B29/C29</f>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="E29" t="s">
         <v>72</v>
@@ -1322,17 +1292,17 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="B30" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C30" s="3">
-        <v>137</v>
+        <v>198</v>
       </c>
       <c r="D30" s="7">
-        <f t="shared" si="0"/>
-        <v>1.4598540145985401E-2</v>
+        <f>B30/C30</f>
+        <v>2.0202020202020204E-2</v>
       </c>
       <c r="E30" t="s">
         <v>72</v>
@@ -1340,17 +1310,17 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B31" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" s="3">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="D31" s="7">
-        <f t="shared" si="0"/>
-        <v>1.4492753623188406E-2</v>
+        <f>B31/C31</f>
+        <v>1.937984496124031E-2</v>
       </c>
       <c r="E31" t="s">
         <v>72</v>
@@ -1358,17 +1328,17 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="B32" s="3">
         <v>3</v>
       </c>
       <c r="C32" s="3">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="D32" s="7">
-        <f t="shared" si="0"/>
-        <v>1.4423076923076924E-2</v>
+        <f>B32/C32</f>
+        <v>1.9108280254777069E-2</v>
       </c>
       <c r="E32" t="s">
         <v>72</v>
@@ -1376,17 +1346,17 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="B33" s="3">
         <v>3</v>
       </c>
       <c r="C33" s="3">
-        <v>213</v>
+        <v>160</v>
       </c>
       <c r="D33" s="7">
-        <f t="shared" si="0"/>
-        <v>1.4084507042253521E-2</v>
+        <f>B33/C33</f>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="E33" t="s">
         <v>72</v>
@@ -1394,17 +1364,17 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B34" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" s="3">
-        <v>368</v>
+        <v>224</v>
       </c>
       <c r="D34" s="7">
-        <f t="shared" si="0"/>
-        <v>1.358695652173913E-2</v>
+        <f>B34/C34</f>
+        <v>1.7857142857142856E-2</v>
       </c>
       <c r="E34" t="s">
         <v>72</v>
@@ -1412,17 +1382,17 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B35" s="3">
         <v>4</v>
       </c>
       <c r="C35" s="3">
-        <v>320</v>
+        <v>226</v>
       </c>
       <c r="D35" s="7">
-        <f t="shared" ref="D35:D66" si="1">B35/C35</f>
-        <v>1.2500000000000001E-2</v>
+        <f>B35/C35</f>
+        <v>1.7699115044247787E-2</v>
       </c>
       <c r="E35" t="s">
         <v>72</v>
@@ -1430,17 +1400,17 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="B36" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C36" s="3">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="D36" s="7">
-        <f t="shared" si="1"/>
-        <v>1.2500000000000001E-2</v>
+        <f>B36/C36</f>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="E36" t="s">
         <v>72</v>
@@ -1448,17 +1418,17 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B37" s="3">
         <v>4</v>
       </c>
       <c r="C37" s="3">
-        <v>336</v>
+        <v>231</v>
       </c>
       <c r="D37" s="7">
-        <f t="shared" si="1"/>
-        <v>1.1904761904761904E-2</v>
+        <f>B37/C37</f>
+        <v>1.7316017316017316E-2</v>
       </c>
       <c r="E37" t="s">
         <v>72</v>
@@ -1466,17 +1436,17 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="B38" s="3">
         <v>3</v>
       </c>
       <c r="C38" s="3">
-        <v>256</v>
+        <v>181</v>
       </c>
       <c r="D38" s="7">
-        <f t="shared" si="1"/>
-        <v>1.171875E-2</v>
+        <f>IFERROR(B38/C38," ")</f>
+        <v>1.6574585635359115E-2</v>
       </c>
       <c r="E38" t="s">
         <v>72</v>
@@ -1484,17 +1454,17 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="B39" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C39" s="3">
-        <v>432</v>
+        <v>182</v>
       </c>
       <c r="D39" s="7">
-        <f t="shared" si="1"/>
-        <v>1.1574074074074073E-2</v>
+        <f>B39/C39</f>
+        <v>1.6483516483516484E-2</v>
       </c>
       <c r="E39" t="s">
         <v>72</v>
@@ -1502,17 +1472,17 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B40" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C40" s="3">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" si="1"/>
-        <v>1.1363636363636364E-2</v>
+        <f>B40/C40</f>
+        <v>1.6E-2</v>
       </c>
       <c r="E40" t="s">
         <v>72</v>
@@ -1520,17 +1490,17 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B41" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C41" s="3">
         <v>266</v>
       </c>
       <c r="D41" s="7">
-        <f t="shared" si="1"/>
-        <v>1.1278195488721804E-2</v>
+        <f>B41/C41</f>
+        <v>1.5037593984962405E-2</v>
       </c>
       <c r="E41" t="s">
         <v>72</v>
@@ -1538,17 +1508,17 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="B42" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C42" s="3">
-        <v>277</v>
+        <v>336</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" si="1"/>
-        <v>1.0830324909747292E-2</v>
+        <f>B42/C42</f>
+        <v>1.488095238095238E-2</v>
       </c>
       <c r="E42" t="s">
         <v>72</v>
@@ -1556,17 +1526,17 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="B43" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C43" s="3">
-        <v>384</v>
+        <v>137</v>
       </c>
       <c r="D43" s="7">
-        <f t="shared" si="1"/>
-        <v>1.0416666666666666E-2</v>
+        <f>B43/C43</f>
+        <v>1.4598540145985401E-2</v>
       </c>
       <c r="E43" t="s">
         <v>72</v>
@@ -1574,17 +1544,17 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B44" s="3">
         <v>4</v>
       </c>
       <c r="C44" s="3">
-        <v>384</v>
+        <v>276</v>
       </c>
       <c r="D44" s="7">
-        <f t="shared" si="1"/>
-        <v>1.0416666666666666E-2</v>
+        <f>B44/C44</f>
+        <v>1.4492753623188406E-2</v>
       </c>
       <c r="E44" t="s">
         <v>72</v>
@@ -1592,17 +1562,17 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B45" s="3">
         <v>3</v>
       </c>
       <c r="C45" s="3">
-        <v>288</v>
+        <v>208</v>
       </c>
       <c r="D45" s="7">
-        <f t="shared" si="1"/>
-        <v>1.0416666666666666E-2</v>
+        <f>B45/C45</f>
+        <v>1.4423076923076924E-2</v>
       </c>
       <c r="E45" t="s">
         <v>72</v>
@@ -1610,17 +1580,17 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B46" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46" s="3">
-        <v>400</v>
+        <v>213</v>
       </c>
       <c r="D46" s="7">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
+        <f>B46/C46</f>
+        <v>1.4084507042253521E-2</v>
       </c>
       <c r="E46" t="s">
         <v>72</v>
@@ -1628,17 +1598,17 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B47" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" s="3">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D47" s="7">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
+        <f>IFERROR(B47/C47," ")</f>
+        <v>1.3636363636363636E-2</v>
       </c>
       <c r="E47" t="s">
         <v>72</v>
@@ -1646,17 +1616,17 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="B48" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C48" s="3">
-        <v>416</v>
+        <v>368</v>
       </c>
       <c r="D48" s="7">
-        <f t="shared" si="1"/>
-        <v>9.6153846153846159E-3</v>
+        <f>B48/C48</f>
+        <v>1.358695652173913E-2</v>
       </c>
       <c r="E48" t="s">
         <v>72</v>
@@ -1664,17 +1634,17 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B49" s="8">
-        <v>2</v>
+        <v>66</v>
+      </c>
+      <c r="B49" s="3">
+        <v>4</v>
       </c>
       <c r="C49" s="3">
-        <v>208</v>
+        <v>320</v>
       </c>
       <c r="D49" s="7">
-        <f t="shared" si="1"/>
-        <v>9.6153846153846159E-3</v>
+        <f>B49/C49</f>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="E49" t="s">
         <v>72</v>
@@ -1682,17 +1652,17 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="B50" s="3">
         <v>2</v>
       </c>
       <c r="C50" s="3">
-        <v>208</v>
+        <v>160</v>
       </c>
       <c r="D50" s="7">
-        <f t="shared" si="1"/>
-        <v>9.6153846153846159E-3</v>
+        <f>B50/C50</f>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="E50" t="s">
         <v>72</v>
@@ -1700,17 +1670,17 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="B51" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C51" s="3">
-        <v>316</v>
+        <v>336</v>
       </c>
       <c r="D51" s="7">
-        <f t="shared" si="1"/>
-        <v>9.4936708860759497E-3</v>
+        <f>B51/C51</f>
+        <v>1.1904761904761904E-2</v>
       </c>
       <c r="E51" t="s">
         <v>72</v>
@@ -1718,17 +1688,17 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>131</v>
+        <v>14</v>
       </c>
       <c r="B52" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52" s="3">
-        <v>432</v>
+        <v>256</v>
       </c>
       <c r="D52" s="7">
-        <f t="shared" si="1"/>
-        <v>9.2592592592592587E-3</v>
+        <f>B52/C52</f>
+        <v>1.171875E-2</v>
       </c>
       <c r="E52" t="s">
         <v>72</v>
@@ -1736,17 +1706,17 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="B53" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C53" s="3">
-        <v>436</v>
+        <v>256</v>
       </c>
       <c r="D53" s="7">
-        <f t="shared" si="1"/>
-        <v>9.1743119266055051E-3</v>
+        <f>IFERROR(B53/C53," ")</f>
+        <v>1.171875E-2</v>
       </c>
       <c r="E53" t="s">
         <v>72</v>
@@ -1754,17 +1724,17 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B54" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C54" s="3">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="D54" s="7">
-        <f t="shared" si="1"/>
-        <v>9.0090090090090089E-3</v>
+        <f>B54/C54</f>
+        <v>1.1574074074074073E-2</v>
       </c>
       <c r="E54" t="s">
         <v>72</v>
@@ -1772,17 +1742,17 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" s="3">
         <v>3</v>
       </c>
       <c r="C55" s="3">
-        <v>336</v>
+        <v>264</v>
       </c>
       <c r="D55" s="7">
-        <f t="shared" si="1"/>
-        <v>8.9285714285714281E-3</v>
+        <f>B55/C55</f>
+        <v>1.1363636363636364E-2</v>
       </c>
       <c r="E55" t="s">
         <v>72</v>
@@ -1790,17 +1760,17 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="B56" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C56" s="3">
-        <v>225</v>
+        <v>352</v>
       </c>
       <c r="D56" s="7">
-        <f t="shared" si="1"/>
-        <v>8.8888888888888889E-3</v>
+        <f>IFERROR(B56/C56," ")</f>
+        <v>1.1363636363636364E-2</v>
       </c>
       <c r="E56" t="s">
         <v>72</v>
@@ -1808,17 +1778,17 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B57" s="3">
         <v>3</v>
       </c>
       <c r="C57" s="3">
-        <v>344</v>
+        <v>266</v>
       </c>
       <c r="D57" s="7">
-        <f t="shared" si="1"/>
-        <v>8.7209302325581394E-3</v>
+        <f>B57/C57</f>
+        <v>1.1278195488721804E-2</v>
       </c>
       <c r="E57" t="s">
         <v>72</v>
@@ -1826,17 +1796,17 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="B58" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58" s="3">
-        <v>464</v>
+        <v>277</v>
       </c>
       <c r="D58" s="7">
-        <f t="shared" si="1"/>
-        <v>8.6206896551724137E-3</v>
+        <f>B58/C58</f>
+        <v>1.0830324909747292E-2</v>
       </c>
       <c r="E58" t="s">
         <v>72</v>
@@ -1844,17 +1814,17 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="B59" s="3">
         <v>4</v>
       </c>
       <c r="C59" s="3">
-        <v>464</v>
+        <v>384</v>
       </c>
       <c r="D59" s="7">
-        <f t="shared" si="1"/>
-        <v>8.6206896551724137E-3</v>
+        <f>B59/C59</f>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E59" t="s">
         <v>72</v>
@@ -1862,17 +1832,17 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B60" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C60" s="3">
-        <v>352</v>
+        <v>384</v>
       </c>
       <c r="D60" s="7">
-        <f t="shared" si="1"/>
-        <v>8.5227272727272721E-3</v>
+        <f>B60/C60</f>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E60" t="s">
         <v>72</v>
@@ -1880,17 +1850,17 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B61" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C61" s="3">
-        <v>480</v>
+        <v>288</v>
       </c>
       <c r="D61" s="7">
-        <f t="shared" si="1"/>
-        <v>8.3333333333333332E-3</v>
+        <f>B61/C61</f>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E61" t="s">
         <v>72</v>
@@ -1898,17 +1868,17 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="B62" s="3">
         <v>3</v>
       </c>
       <c r="C62" s="3">
-        <v>360</v>
+        <v>288</v>
       </c>
       <c r="D62" s="7">
-        <f t="shared" si="1"/>
-        <v>8.3333333333333332E-3</v>
+        <f>IFERROR(B62/C62," ")</f>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E62" t="s">
         <v>72</v>
@@ -1916,17 +1886,17 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B63" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C63" s="3">
-        <v>240</v>
+        <v>400</v>
       </c>
       <c r="D63" s="7">
-        <f t="shared" si="1"/>
-        <v>8.3333333333333332E-3</v>
+        <f>B63/C63</f>
+        <v>0.01</v>
       </c>
       <c r="E63" t="s">
         <v>72</v>
@@ -1934,17 +1904,17 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="B64" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C64" s="3">
-        <v>368</v>
+        <v>200</v>
       </c>
       <c r="D64" s="7">
-        <f t="shared" si="1"/>
-        <v>8.152173913043478E-3</v>
+        <f>B64/C64</f>
+        <v>0.01</v>
       </c>
       <c r="E64" t="s">
         <v>72</v>
@@ -1952,17 +1922,17 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B65" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C65" s="3">
-        <v>368</v>
+        <v>400</v>
       </c>
       <c r="D65" s="7">
-        <f t="shared" si="1"/>
-        <v>8.152173913043478E-3</v>
+        <f>IFERROR(B65/C65," ")</f>
+        <v>0.01</v>
       </c>
       <c r="E65" t="s">
         <v>72</v>
@@ -1970,17 +1940,17 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="B66" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C66" s="3">
-        <v>371</v>
+        <v>416</v>
       </c>
       <c r="D66" s="7">
-        <f t="shared" si="1"/>
-        <v>8.0862533692722376E-3</v>
+        <f>B66/C66</f>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E66" t="s">
         <v>72</v>
@@ -1988,17 +1958,17 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B67" s="3">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c r="B67" s="8">
+        <v>2</v>
       </c>
       <c r="C67" s="3">
-        <v>499</v>
+        <v>208</v>
       </c>
       <c r="D67" s="7">
-        <f t="shared" ref="D67:D98" si="2">B67/C67</f>
-        <v>8.0160320641282558E-3</v>
+        <f>B67/C67</f>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E67" t="s">
         <v>72</v>
@@ -2006,17 +1976,17 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B68" s="3">
         <v>2</v>
       </c>
       <c r="C68" s="3">
-        <v>250</v>
+        <v>208</v>
       </c>
       <c r="D68" s="7">
-        <f t="shared" si="2"/>
-        <v>8.0000000000000002E-3</v>
+        <f>B68/C68</f>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E68" t="s">
         <v>72</v>
@@ -2024,17 +1994,17 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="B69" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69" s="3">
-        <v>512</v>
+        <v>312</v>
       </c>
       <c r="D69" s="7">
-        <f t="shared" si="2"/>
-        <v>7.8125E-3</v>
+        <f>IFERROR(B69/C69," ")</f>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E69" t="s">
         <v>72</v>
@@ -2042,17 +2012,17 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="B70" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C70" s="3">
-        <v>512</v>
+        <v>316</v>
       </c>
       <c r="D70" s="7">
-        <f t="shared" si="2"/>
-        <v>7.8125E-3</v>
+        <f>B70/C70</f>
+        <v>9.4936708860759497E-3</v>
       </c>
       <c r="E70" t="s">
         <v>72</v>
@@ -2060,17 +2030,17 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="B71" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C71" s="3">
-        <v>264</v>
+        <v>432</v>
       </c>
       <c r="D71" s="7">
-        <f t="shared" si="2"/>
-        <v>7.575757575757576E-3</v>
+        <f>B71/C71</f>
+        <v>9.2592592592592587E-3</v>
       </c>
       <c r="E71" t="s">
         <v>72</v>
@@ -2078,17 +2048,17 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B72" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C72" s="3">
-        <v>400</v>
+        <v>436</v>
       </c>
       <c r="D72" s="7">
-        <f t="shared" si="2"/>
-        <v>7.4999999999999997E-3</v>
+        <f>B72/C72</f>
+        <v>9.1743119266055051E-3</v>
       </c>
       <c r="E72" t="s">
         <v>72</v>
@@ -2096,17 +2066,17 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="B73" s="3">
         <v>4</v>
       </c>
       <c r="C73" s="3">
-        <v>544</v>
+        <v>444</v>
       </c>
       <c r="D73" s="7">
-        <f t="shared" si="2"/>
-        <v>7.3529411764705881E-3</v>
+        <f>B73/C73</f>
+        <v>9.0090090090090089E-3</v>
       </c>
       <c r="E73" t="s">
         <v>72</v>
@@ -2114,17 +2084,17 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B74" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C74" s="3">
-        <v>560</v>
+        <v>336</v>
       </c>
       <c r="D74" s="7">
-        <f t="shared" si="2"/>
-        <v>7.1428571428571426E-3</v>
+        <f>B74/C74</f>
+        <v>8.9285714285714281E-3</v>
       </c>
       <c r="E74" t="s">
         <v>72</v>
@@ -2132,17 +2102,17 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B75" s="3">
         <v>2</v>
       </c>
       <c r="C75" s="3">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="D75" s="7">
-        <f t="shared" si="2"/>
-        <v>7.0422535211267607E-3</v>
+        <f>B75/C75</f>
+        <v>8.8888888888888889E-3</v>
       </c>
       <c r="E75" t="s">
         <v>72</v>
@@ -2150,17 +2120,17 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="B76" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C76" s="3">
-        <v>288</v>
+        <v>344</v>
       </c>
       <c r="D76" s="7">
-        <f t="shared" si="2"/>
-        <v>6.9444444444444441E-3</v>
+        <f>B76/C76</f>
+        <v>8.7209302325581394E-3</v>
       </c>
       <c r="E76" t="s">
         <v>72</v>
@@ -2168,17 +2138,17 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="B77" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C77" s="3">
-        <v>148</v>
+        <v>464</v>
       </c>
       <c r="D77" s="7">
-        <f t="shared" si="2"/>
-        <v>6.7567567567567571E-3</v>
+        <f>B77/C77</f>
+        <v>8.6206896551724137E-3</v>
       </c>
       <c r="E77" t="s">
         <v>72</v>
@@ -2186,17 +2156,17 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B78" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C78" s="3">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="D78" s="7">
-        <f t="shared" si="2"/>
-        <v>6.6666666666666671E-3</v>
+        <f>B78/C78</f>
+        <v>8.6206896551724137E-3</v>
       </c>
       <c r="E78" t="s">
         <v>72</v>
@@ -2204,17 +2174,17 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B79" s="3">
         <v>3</v>
       </c>
       <c r="C79" s="3">
-        <v>480</v>
+        <v>352</v>
       </c>
       <c r="D79" s="7">
-        <f t="shared" si="2"/>
-        <v>6.2500000000000003E-3</v>
+        <f>B79/C79</f>
+        <v>8.5227272727272721E-3</v>
       </c>
       <c r="E79" t="s">
         <v>72</v>
@@ -2222,17 +2192,17 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="B80" s="3">
         <v>3</v>
       </c>
       <c r="C80" s="3">
-        <v>480</v>
+        <v>352</v>
       </c>
       <c r="D80" s="7">
-        <f t="shared" si="2"/>
-        <v>6.2500000000000003E-3</v>
+        <f>IFERROR(B80/C80," ")</f>
+        <v>8.5227272727272721E-3</v>
       </c>
       <c r="E80" t="s">
         <v>72</v>
@@ -2240,17 +2210,17 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B81" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C81" s="3">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="D81" s="7">
-        <f t="shared" si="2"/>
-        <v>6.1475409836065573E-3</v>
+        <f>B81/C81</f>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E81" t="s">
         <v>72</v>
@@ -2258,17 +2228,17 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="B82" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C82" s="3">
-        <v>332</v>
+        <v>360</v>
       </c>
       <c r="D82" s="7">
-        <f t="shared" si="2"/>
-        <v>6.024096385542169E-3</v>
+        <f>B82/C82</f>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E82" t="s">
         <v>72</v>
@@ -2276,17 +2246,17 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="B83" s="3">
         <v>2</v>
       </c>
       <c r="C83" s="3">
-        <v>332</v>
+        <v>240</v>
       </c>
       <c r="D83" s="7">
-        <f t="shared" si="2"/>
-        <v>6.024096385542169E-3</v>
+        <f>B83/C83</f>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E83" t="s">
         <v>72</v>
@@ -2294,17 +2264,17 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
       <c r="B84" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C84" s="3">
-        <v>344</v>
+        <v>368</v>
       </c>
       <c r="D84" s="7">
-        <f t="shared" si="2"/>
-        <v>5.8139534883720929E-3</v>
+        <f>B84/C84</f>
+        <v>8.152173913043478E-3</v>
       </c>
       <c r="E84" t="s">
         <v>72</v>
@@ -2312,17 +2282,17 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B85" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C85" s="3">
-        <v>704</v>
+        <v>368</v>
       </c>
       <c r="D85" s="7">
-        <f t="shared" si="2"/>
-        <v>5.681818181818182E-3</v>
+        <f>B85/C85</f>
+        <v>8.152173913043478E-3</v>
       </c>
       <c r="E85" t="s">
         <v>72</v>
@@ -2330,17 +2300,17 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="B86" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C86" s="3">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D86" s="7">
-        <f t="shared" si="2"/>
-        <v>5.4644808743169399E-3</v>
+        <f>B86/C86</f>
+        <v>8.0862533692722376E-3</v>
       </c>
       <c r="E86" t="s">
         <v>72</v>
@@ -2348,17 +2318,17 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="B87" s="3">
         <v>4</v>
       </c>
       <c r="C87" s="3">
-        <v>736</v>
+        <v>499</v>
       </c>
       <c r="D87" s="7">
-        <f t="shared" si="2"/>
-        <v>5.434782608695652E-3</v>
+        <f>B87/C87</f>
+        <v>8.0160320641282558E-3</v>
       </c>
       <c r="E87" t="s">
         <v>72</v>
@@ -2366,17 +2336,17 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B88" s="3">
         <v>2</v>
       </c>
       <c r="C88" s="3">
-        <v>373</v>
+        <v>250</v>
       </c>
       <c r="D88" s="7">
-        <f t="shared" si="2"/>
-        <v>5.3619302949061663E-3</v>
+        <f>B88/C88</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E88" t="s">
         <v>72</v>
@@ -2384,17 +2354,17 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B89" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C89" s="3">
-        <v>560</v>
+        <v>512</v>
       </c>
       <c r="D89" s="7">
-        <f t="shared" si="2"/>
-        <v>5.3571428571428572E-3</v>
+        <f>B89/C89</f>
+        <v>7.8125E-3</v>
       </c>
       <c r="E89" t="s">
         <v>72</v>
@@ -2402,17 +2372,17 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="B90" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C90" s="3">
-        <v>560</v>
+        <v>512</v>
       </c>
       <c r="D90" s="7">
-        <f t="shared" si="2"/>
-        <v>5.3571428571428572E-3</v>
+        <f>B90/C90</f>
+        <v>7.8125E-3</v>
       </c>
       <c r="E90" t="s">
         <v>72</v>
@@ -2420,17 +2390,17 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B91" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C91" s="3">
-        <v>576</v>
+        <v>264</v>
       </c>
       <c r="D91" s="7">
-        <f t="shared" si="2"/>
-        <v>5.208333333333333E-3</v>
+        <f>B91/C91</f>
+        <v>7.575757575757576E-3</v>
       </c>
       <c r="E91" t="s">
         <v>72</v>
@@ -2438,17 +2408,17 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="B92" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C92" s="3">
-        <v>384</v>
+        <v>400</v>
       </c>
       <c r="D92" s="7">
-        <f t="shared" si="2"/>
-        <v>5.208333333333333E-3</v>
+        <f>B92/C92</f>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E92" t="s">
         <v>72</v>
@@ -2456,17 +2426,17 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B93" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C93" s="3">
-        <v>200</v>
+        <v>544</v>
       </c>
       <c r="D93" s="7">
-        <f t="shared" si="2"/>
-        <v>5.0000000000000001E-3</v>
+        <f>B93/C93</f>
+        <v>7.3529411764705881E-3</v>
       </c>
       <c r="E93" t="s">
         <v>72</v>
@@ -2474,17 +2444,17 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="B94" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C94" s="3">
-        <v>400</v>
+        <v>416</v>
       </c>
       <c r="D94" s="7">
-        <f t="shared" si="2"/>
-        <v>5.0000000000000001E-3</v>
+        <f>IFERROR(B94/C94," ")</f>
+        <v>7.2115384615384619E-3</v>
       </c>
       <c r="E94" t="s">
         <v>72</v>
@@ -2492,17 +2462,17 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B95" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C95" s="3">
-        <v>416</v>
+        <v>560</v>
       </c>
       <c r="D95" s="7">
-        <f t="shared" si="2"/>
-        <v>4.807692307692308E-3</v>
+        <f>B95/C95</f>
+        <v>7.1428571428571426E-3</v>
       </c>
       <c r="E95" t="s">
         <v>72</v>
@@ -2510,17 +2480,17 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B96" s="3">
         <v>2</v>
       </c>
       <c r="C96" s="3">
-        <v>416</v>
+        <v>284</v>
       </c>
       <c r="D96" s="7">
-        <f t="shared" si="2"/>
-        <v>4.807692307692308E-3</v>
+        <f>B96/C96</f>
+        <v>7.0422535211267607E-3</v>
       </c>
       <c r="E96" t="s">
         <v>72</v>
@@ -2528,17 +2498,17 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="B97" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C97" s="3">
-        <v>848</v>
+        <v>288</v>
       </c>
       <c r="D97" s="7">
-        <f t="shared" si="2"/>
-        <v>4.7169811320754715E-3</v>
+        <f>B97/C97</f>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="E97" t="s">
         <v>72</v>
@@ -2546,17 +2516,17 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="B98" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C98" s="3">
-        <v>456</v>
+        <v>736</v>
       </c>
       <c r="D98" s="7">
-        <f t="shared" si="2"/>
-        <v>4.3859649122807015E-3</v>
+        <f>IFERROR(B98/C98," ")</f>
+        <v>6.793478260869565E-3</v>
       </c>
       <c r="E98" t="s">
         <v>72</v>
@@ -2564,17 +2534,17 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B99" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C99" s="3">
-        <v>528</v>
+        <v>148</v>
       </c>
       <c r="D99" s="7">
-        <f t="shared" ref="D99:D104" si="3">B99/C99</f>
-        <v>3.787878787878788E-3</v>
+        <f>B99/C99</f>
+        <v>6.7567567567567571E-3</v>
       </c>
       <c r="E99" t="s">
         <v>72</v>
@@ -2582,17 +2552,17 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="B100" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C100" s="3">
-        <v>544</v>
+        <v>450</v>
       </c>
       <c r="D100" s="7">
-        <f t="shared" si="3"/>
-        <v>3.6764705882352941E-3</v>
+        <f>B100/C100</f>
+        <v>6.6666666666666671E-3</v>
       </c>
       <c r="E100" t="s">
         <v>72</v>
@@ -2600,17 +2570,17 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="B101" s="3">
         <v>3</v>
       </c>
       <c r="C101" s="3">
-        <v>848</v>
+        <v>464</v>
       </c>
       <c r="D101" s="7">
-        <f t="shared" si="3"/>
-        <v>3.5377358490566039E-3</v>
+        <f>IFERROR(B101/C101," ")</f>
+        <v>6.4655172413793103E-3</v>
       </c>
       <c r="E101" t="s">
         <v>72</v>
@@ -2618,17 +2588,17 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="B102" s="3">
         <v>3</v>
       </c>
       <c r="C102" s="3">
-        <v>864</v>
+        <v>480</v>
       </c>
       <c r="D102" s="7">
-        <f t="shared" si="3"/>
-        <v>3.472222222222222E-3</v>
+        <f>B102/C102</f>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E102" t="s">
         <v>72</v>
@@ -2636,17 +2606,17 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B103" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C103" s="3">
-        <v>616</v>
+        <v>480</v>
       </c>
       <c r="D103" s="7">
-        <f t="shared" si="3"/>
-        <v>3.246753246753247E-3</v>
+        <f>B103/C103</f>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E103" t="s">
         <v>72</v>
@@ -2654,17 +2624,17 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="B104" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C104" s="3">
-        <v>320</v>
+        <v>488</v>
       </c>
       <c r="D104" s="7">
-        <f t="shared" si="3"/>
-        <v>3.1250000000000002E-3</v>
+        <f>B104/C104</f>
+        <v>6.1475409836065573E-3</v>
       </c>
       <c r="E104" t="s">
         <v>72</v>
@@ -2672,17 +2642,17 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="B105" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C105" s="3">
-        <v>1280</v>
+        <v>332</v>
       </c>
       <c r="D105" s="7">
-        <f>IFERROR(B105/C105," ")</f>
-        <v>2.3437499999999999E-3</v>
+        <f>B105/C105</f>
+        <v>6.024096385542169E-3</v>
       </c>
       <c r="E105" t="s">
         <v>72</v>
@@ -2690,11 +2660,17 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D106" s="7" t="str">
-        <f>IFERROR(B106/C106," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>102</v>
+      </c>
+      <c r="B106" s="3">
+        <v>2</v>
+      </c>
+      <c r="C106" s="3">
+        <v>332</v>
+      </c>
+      <c r="D106" s="7">
+        <f>B106/C106</f>
+        <v>6.024096385542169E-3</v>
       </c>
       <c r="E106" t="s">
         <v>72</v>
@@ -2702,11 +2678,17 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D107" s="7" t="str">
-        <f t="shared" ref="D107:D170" si="4">IFERROR(B107/C107," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>133</v>
+      </c>
+      <c r="B107" s="3">
+        <v>2</v>
+      </c>
+      <c r="C107" s="3">
+        <v>344</v>
+      </c>
+      <c r="D107" s="7">
+        <f>B107/C107</f>
+        <v>5.8139534883720929E-3</v>
       </c>
       <c r="E107" t="s">
         <v>72</v>
@@ -2714,11 +2696,17 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D108" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>34</v>
+      </c>
+      <c r="B108" s="3">
+        <v>4</v>
+      </c>
+      <c r="C108" s="3">
+        <v>704</v>
+      </c>
+      <c r="D108" s="7">
+        <f>B108/C108</f>
+        <v>5.681818181818182E-3</v>
       </c>
       <c r="E108" t="s">
         <v>72</v>
@@ -2726,11 +2714,17 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D109" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>103</v>
+      </c>
+      <c r="B109" s="3">
+        <v>2</v>
+      </c>
+      <c r="C109" s="3">
+        <v>366</v>
+      </c>
+      <c r="D109" s="7">
+        <f>B109/C109</f>
+        <v>5.4644808743169399E-3</v>
       </c>
       <c r="E109" t="s">
         <v>72</v>
@@ -2738,11 +2732,17 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D110" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>70</v>
+      </c>
+      <c r="B110" s="3">
+        <v>4</v>
+      </c>
+      <c r="C110" s="3">
+        <v>736</v>
+      </c>
+      <c r="D110" s="7">
+        <f>B110/C110</f>
+        <v>5.434782608695652E-3</v>
       </c>
       <c r="E110" t="s">
         <v>72</v>
@@ -2750,11 +2750,17 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D111" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>36</v>
+      </c>
+      <c r="B111" s="3">
+        <v>2</v>
+      </c>
+      <c r="C111" s="3">
+        <v>373</v>
+      </c>
+      <c r="D111" s="7">
+        <f>B111/C111</f>
+        <v>5.3619302949061663E-3</v>
       </c>
       <c r="E111" t="s">
         <v>72</v>
@@ -2762,11 +2768,17 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D112" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>23</v>
+      </c>
+      <c r="B112" s="3">
+        <v>3</v>
+      </c>
+      <c r="C112" s="3">
+        <v>560</v>
+      </c>
+      <c r="D112" s="7">
+        <f>B112/C112</f>
+        <v>5.3571428571428572E-3</v>
       </c>
       <c r="E112" t="s">
         <v>72</v>
@@ -2774,11 +2786,17 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D113" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>26</v>
+      </c>
+      <c r="B113" s="3">
+        <v>3</v>
+      </c>
+      <c r="C113" s="3">
+        <v>560</v>
+      </c>
+      <c r="D113" s="7">
+        <f>B113/C113</f>
+        <v>5.3571428571428572E-3</v>
       </c>
       <c r="E113" t="s">
         <v>72</v>
@@ -2786,11 +2804,17 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D114" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>27</v>
+      </c>
+      <c r="B114" s="3">
+        <v>3</v>
+      </c>
+      <c r="C114" s="3">
+        <v>576</v>
+      </c>
+      <c r="D114" s="7">
+        <f>B114/C114</f>
+        <v>5.208333333333333E-3</v>
       </c>
       <c r="E114" t="s">
         <v>72</v>
@@ -2798,11 +2822,17 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D115" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>13</v>
+      </c>
+      <c r="B115" s="3">
+        <v>2</v>
+      </c>
+      <c r="C115" s="3">
+        <v>384</v>
+      </c>
+      <c r="D115" s="7">
+        <f>B115/C115</f>
+        <v>5.208333333333333E-3</v>
       </c>
       <c r="E115" t="s">
         <v>72</v>
@@ -2810,11 +2840,17 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D116" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>81</v>
+      </c>
+      <c r="B116" s="3">
+        <v>1</v>
+      </c>
+      <c r="C116" s="3">
+        <v>200</v>
+      </c>
+      <c r="D116" s="7">
+        <f>B116/C116</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E116" t="s">
         <v>72</v>
@@ -2822,11 +2858,17 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D117" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>16</v>
+      </c>
+      <c r="B117" s="3">
+        <v>2</v>
+      </c>
+      <c r="C117" s="3">
+        <v>400</v>
+      </c>
+      <c r="D117" s="7">
+        <f>B117/C117</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E117" t="s">
         <v>72</v>
@@ -2834,11 +2876,17 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D118" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>32</v>
+      </c>
+      <c r="B118" s="3">
+        <v>2</v>
+      </c>
+      <c r="C118" s="3">
+        <v>416</v>
+      </c>
+      <c r="D118" s="7">
+        <f>B118/C118</f>
+        <v>4.807692307692308E-3</v>
       </c>
       <c r="E118" t="s">
         <v>72</v>
@@ -2846,11 +2894,17 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D119" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>59</v>
+      </c>
+      <c r="B119" s="3">
+        <v>2</v>
+      </c>
+      <c r="C119" s="3">
+        <v>416</v>
+      </c>
+      <c r="D119" s="7">
+        <f>B119/C119</f>
+        <v>4.807692307692308E-3</v>
       </c>
       <c r="E119" t="s">
         <v>72</v>
@@ -2858,11 +2912,17 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D120" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>96</v>
+      </c>
+      <c r="B120" s="3">
+        <v>4</v>
+      </c>
+      <c r="C120" s="3">
+        <v>848</v>
+      </c>
+      <c r="D120" s="7">
+        <f>B120/C120</f>
+        <v>4.7169811320754715E-3</v>
       </c>
       <c r="E120" t="s">
         <v>72</v>
@@ -2870,11 +2930,17 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D121" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>107</v>
+      </c>
+      <c r="B121" s="3">
+        <v>2</v>
+      </c>
+      <c r="C121" s="3">
+        <v>440</v>
+      </c>
+      <c r="D121" s="7">
+        <f>IFERROR(B121/C121," ")</f>
+        <v>4.5454545454545452E-3</v>
       </c>
       <c r="E121" t="s">
         <v>72</v>
@@ -2882,11 +2948,17 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D122" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>101</v>
+      </c>
+      <c r="B122" s="3">
+        <v>2</v>
+      </c>
+      <c r="C122" s="3">
+        <v>456</v>
+      </c>
+      <c r="D122" s="7">
+        <f>B122/C122</f>
+        <v>4.3859649122807015E-3</v>
       </c>
       <c r="E122" t="s">
         <v>72</v>
@@ -2894,11 +2966,17 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D123" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>46</v>
+      </c>
+      <c r="B123" s="3">
+        <v>2</v>
+      </c>
+      <c r="C123" s="3">
+        <v>528</v>
+      </c>
+      <c r="D123" s="7">
+        <f>B123/C123</f>
+        <v>3.787878787878788E-3</v>
       </c>
       <c r="E123" t="s">
         <v>72</v>
@@ -2906,11 +2984,17 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D124" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>60</v>
+      </c>
+      <c r="B124" s="3">
+        <v>2</v>
+      </c>
+      <c r="C124" s="3">
+        <v>544</v>
+      </c>
+      <c r="D124" s="7">
+        <f>B124/C124</f>
+        <v>3.6764705882352941E-3</v>
       </c>
       <c r="E124" t="s">
         <v>72</v>
@@ -2918,11 +3002,17 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D125" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>22</v>
+      </c>
+      <c r="B125" s="3">
+        <v>3</v>
+      </c>
+      <c r="C125" s="3">
+        <v>848</v>
+      </c>
+      <c r="D125" s="7">
+        <f>B125/C125</f>
+        <v>3.5377358490566039E-3</v>
       </c>
       <c r="E125" t="s">
         <v>72</v>
@@ -2930,11 +3020,17 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D126" s="7" t="str">
-        <f>IFERROR(B126/C126," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>98</v>
+      </c>
+      <c r="B126" s="3">
+        <v>3</v>
+      </c>
+      <c r="C126" s="3">
+        <v>864</v>
+      </c>
+      <c r="D126" s="7">
+        <f>B126/C126</f>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="E126" t="s">
         <v>72</v>
@@ -2942,11 +3038,17 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D127" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>6</v>
+      </c>
+      <c r="B127" s="3">
+        <v>2</v>
+      </c>
+      <c r="C127" s="3">
+        <v>616</v>
+      </c>
+      <c r="D127" s="7">
+        <f>B127/C127</f>
+        <v>3.246753246753247E-3</v>
       </c>
       <c r="E127" t="s">
         <v>72</v>
@@ -2954,14 +3056,17 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="B128" s="3">
-        <v>3</v>
-      </c>
-      <c r="D128" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>1</v>
+      </c>
+      <c r="C128" s="3">
+        <v>320</v>
+      </c>
+      <c r="D128" s="7">
+        <f>B128/C128</f>
+        <v>3.1250000000000002E-3</v>
       </c>
       <c r="E128" t="s">
         <v>72</v>
@@ -2969,566 +3074,577 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="B129" s="3">
-        <v>4</v>
-      </c>
-      <c r="D129" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
+      </c>
+      <c r="C129" s="3">
+        <v>1280</v>
+      </c>
+      <c r="D129" s="7">
+        <f>IFERROR(B129/C129," ")</f>
+        <v>2.3437499999999999E-3</v>
       </c>
       <c r="E129" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D130" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D107:D170" si="1">IFERROR(B130/C130," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D131" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D132" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D133" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D134" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D135" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D136" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D137" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D138" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D139" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D140" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D141" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D142" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D143" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D144" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="145" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D145" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="146" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D146" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="147" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D147" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="148" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D148" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="149" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D149" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="150" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D150" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="151" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D151" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="152" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D152" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="153" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D153" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="154" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D154" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="155" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D155" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="156" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D156" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="157" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D157" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="158" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D158" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="159" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D159" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="160" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D160" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="161" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D161" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="162" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D162" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="163" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D163" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="164" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D164" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="165" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D165" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="166" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D166" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="167" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D167" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="168" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D168" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="169" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D169" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="170" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D170" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="171" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D171" s="7" t="str">
-        <f t="shared" ref="D171:D219" si="5">IFERROR(B171/C171," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D171:D219" si="2">IFERROR(B171/C171," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="172" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D172" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="173" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D173" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="174" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D174" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="175" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D175" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="176" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D176" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="177" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D177" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="178" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D178" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="179" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D179" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="180" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D180" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="181" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D181" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="182" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D182" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="183" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D183" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="184" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D184" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="185" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D185" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="186" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D186" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="187" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D187" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="188" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D188" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="189" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D189" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="190" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D190" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="191" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D191" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="192" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D192" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="193" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D193" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="194" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D194" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="195" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D195" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="196" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D196" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="197" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D197" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="198" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D198" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="199" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D199" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="200" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D200" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="201" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D201" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="202" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D202" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="203" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D203" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="204" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D204" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="205" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D205" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="206" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D206" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="207" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D207" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="208" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D208" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="209" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D209" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="210" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D210" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="211" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D211" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="212" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D212" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="213" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D213" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="214" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D214" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="215" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D215" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="216" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D216" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="217" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D217" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="218" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D218" s="7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="219" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D219" s="7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:E218">
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
     <filterColumn colId="4">
       <filters>
         <filter val="No"/>
       </filters>
     </filterColumn>
+    <sortState ref="A4:E129">
+      <sortCondition descending="1" ref="D2:D218"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added book to list
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="138">
   <si>
     <t>Book Ranking</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>Impeachment: A Citizen's Guide</t>
+  </si>
+  <si>
+    <t>Advice Not Given: A Guide for Getting Over Yourself</t>
   </si>
 </sst>
 </file>
@@ -798,7 +801,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +848,7 @@
         <v>46</v>
       </c>
       <c r="D3" s="7">
-        <f t="shared" ref="D3:D34" si="0">B3/C3</f>
+        <f t="shared" ref="D3" si="0">B3/C3</f>
         <v>8.6956521739130432E-2</v>
       </c>
       <c r="E3" t="s">
@@ -860,7 +863,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="7" t="str">
-        <f>IFERROR(B4/C4," ")</f>
+        <f t="shared" ref="D4:D13" si="1">IFERROR(B4/C4," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E4" t="s">
@@ -875,7 +878,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="7" t="str">
-        <f>IFERROR(B5/C5," ")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E5" t="s">
@@ -890,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="7" t="str">
-        <f>IFERROR(B6/C6," ")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E6" t="s">
@@ -905,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="7" t="str">
-        <f>IFERROR(B7/C7," ")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E7" t="s">
@@ -920,7 +923,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="str">
-        <f>IFERROR(B8/C8," ")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E8" t="s">
@@ -935,7 +938,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="7" t="str">
-        <f>IFERROR(B9/C9," ")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E9" t="s">
@@ -950,7 +953,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="7" t="str">
-        <f>IFERROR(B10/C10," ")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E10" t="s">
@@ -965,7 +968,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="7" t="str">
-        <f>IFERROR(B11/C11," ")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E11" t="s">
@@ -980,7 +983,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="7" t="str">
-        <f>IFERROR(B12/C12," ")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E12" t="s">
@@ -995,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="7" t="str">
-        <f>IFERROR(B13/C13," ")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E13" t="s">
@@ -1049,7 +1052,7 @@
         <v>74</v>
       </c>
       <c r="D16" s="7">
-        <f>B16/C16</f>
+        <f t="shared" ref="D16:D79" si="2">IFERROR(B16/C16," ")</f>
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="E16" t="s">
@@ -1067,7 +1070,7 @@
         <v>120</v>
       </c>
       <c r="D17" s="7">
-        <f>B17/C17</f>
+        <f t="shared" si="2"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E17" t="s">
@@ -1085,7 +1088,7 @@
         <v>72</v>
       </c>
       <c r="D18" s="7">
-        <f>B18/C18</f>
+        <f t="shared" si="2"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E18" t="s">
@@ -1103,7 +1106,7 @@
         <v>128</v>
       </c>
       <c r="D19" s="7">
-        <f>IFERROR(B19/C19," ")</f>
+        <f t="shared" si="2"/>
         <v>3.90625E-2</v>
       </c>
       <c r="E19" t="s">
@@ -1121,7 +1124,7 @@
         <v>133</v>
       </c>
       <c r="D20" s="7">
-        <f>B20/C20</f>
+        <f t="shared" si="2"/>
         <v>3.7593984962406013E-2</v>
       </c>
       <c r="E20" t="s">
@@ -1139,7 +1142,7 @@
         <v>132</v>
       </c>
       <c r="D21" s="7">
-        <f>B21/C21</f>
+        <f t="shared" si="2"/>
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="E21" t="s">
@@ -1157,7 +1160,7 @@
         <v>160</v>
       </c>
       <c r="D22" s="7">
-        <f>B22/C22</f>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E22" t="s">
@@ -1175,7 +1178,7 @@
         <v>80</v>
       </c>
       <c r="D23" s="7">
-        <f>B23/C23</f>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E23" t="s">
@@ -1193,7 +1196,7 @@
         <v>124</v>
       </c>
       <c r="D24" s="7">
-        <f>B24/C24</f>
+        <f t="shared" si="2"/>
         <v>2.4193548387096774E-2</v>
       </c>
       <c r="E24" t="s">
@@ -1211,7 +1214,7 @@
         <v>208</v>
       </c>
       <c r="D25" s="7">
-        <f>IFERROR(B25/C25," ")</f>
+        <f t="shared" si="2"/>
         <v>2.403846153846154E-2</v>
       </c>
       <c r="E25" t="s">
@@ -1229,7 +1232,7 @@
         <v>128</v>
       </c>
       <c r="D26" s="7">
-        <f>B26/C26</f>
+        <f t="shared" si="2"/>
         <v>2.34375E-2</v>
       </c>
       <c r="E26" t="s">
@@ -1238,17 +1241,17 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="B27" s="3">
         <v>5</v>
       </c>
       <c r="C27" s="3">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D27" s="7">
-        <f>B27/C27</f>
-        <v>2.1929824561403508E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2321428571428572E-2</v>
       </c>
       <c r="E27" t="s">
         <v>72</v>
@@ -1256,17 +1259,17 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="B28" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28" s="3">
-        <v>191</v>
+        <v>228</v>
       </c>
       <c r="D28" s="7">
-        <f>B28/C28</f>
-        <v>2.0942408376963352E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.1929824561403508E-2</v>
       </c>
       <c r="E28" t="s">
         <v>72</v>
@@ -1274,17 +1277,17 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="B29" s="3">
         <v>4</v>
       </c>
       <c r="C29" s="3">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D29" s="7">
-        <f>B29/C29</f>
-        <v>2.0833333333333332E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.0942408376963352E-2</v>
       </c>
       <c r="E29" t="s">
         <v>72</v>
@@ -1292,17 +1295,17 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>130</v>
+        <v>38</v>
       </c>
       <c r="B30" s="3">
         <v>4</v>
       </c>
       <c r="C30" s="3">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D30" s="7">
-        <f>B30/C30</f>
-        <v>2.0202020202020204E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="E30" t="s">
         <v>72</v>
@@ -1310,17 +1313,17 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="B31" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="3">
-        <v>258</v>
+        <v>198</v>
       </c>
       <c r="D31" s="7">
-        <f>B31/C31</f>
-        <v>1.937984496124031E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.0202020202020204E-2</v>
       </c>
       <c r="E31" t="s">
         <v>72</v>
@@ -1328,17 +1331,17 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B32" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C32" s="3">
-        <v>157</v>
+        <v>258</v>
       </c>
       <c r="D32" s="7">
-        <f>B32/C32</f>
-        <v>1.9108280254777069E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.937984496124031E-2</v>
       </c>
       <c r="E32" t="s">
         <v>72</v>
@@ -1346,17 +1349,17 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="B33" s="3">
         <v>3</v>
       </c>
       <c r="C33" s="3">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D33" s="7">
-        <f>B33/C33</f>
-        <v>1.8749999999999999E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.9108280254777069E-2</v>
       </c>
       <c r="E33" t="s">
         <v>72</v>
@@ -1364,17 +1367,17 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B34" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C34" s="3">
-        <v>224</v>
+        <v>160</v>
       </c>
       <c r="D34" s="7">
-        <f>B34/C34</f>
-        <v>1.7857142857142856E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="E34" t="s">
         <v>72</v>
@@ -1382,17 +1385,17 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="B35" s="3">
         <v>4</v>
       </c>
       <c r="C35" s="3">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D35" s="7">
-        <f>B35/C35</f>
-        <v>1.7699115044247787E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.7857142857142856E-2</v>
       </c>
       <c r="E35" t="s">
         <v>72</v>
@@ -1400,17 +1403,17 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B36" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36" s="3">
-        <v>288</v>
+        <v>226</v>
       </c>
       <c r="D36" s="7">
-        <f>B36/C36</f>
-        <v>1.7361111111111112E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.7699115044247787E-2</v>
       </c>
       <c r="E36" t="s">
         <v>72</v>
@@ -1418,17 +1421,17 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B37" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C37" s="3">
-        <v>231</v>
+        <v>288</v>
       </c>
       <c r="D37" s="7">
-        <f>B37/C37</f>
-        <v>1.7316017316017316E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="E37" t="s">
         <v>72</v>
@@ -1436,17 +1439,17 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="B38" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C38" s="3">
-        <v>181</v>
+        <v>231</v>
       </c>
       <c r="D38" s="7">
-        <f>IFERROR(B38/C38," ")</f>
-        <v>1.6574585635359115E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.7316017316017316E-2</v>
       </c>
       <c r="E38" t="s">
         <v>72</v>
@@ -1454,17 +1457,17 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="B39" s="3">
         <v>3</v>
       </c>
       <c r="C39" s="3">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D39" s="7">
-        <f>B39/C39</f>
-        <v>1.6483516483516484E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.6574585635359115E-2</v>
       </c>
       <c r="E39" t="s">
         <v>72</v>
@@ -1472,17 +1475,17 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B40" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40" s="3">
-        <v>250</v>
+        <v>182</v>
       </c>
       <c r="D40" s="7">
-        <f>B40/C40</f>
-        <v>1.6E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.6483516483516484E-2</v>
       </c>
       <c r="E40" t="s">
         <v>72</v>
@@ -1490,17 +1493,17 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="B41" s="3">
         <v>4</v>
       </c>
       <c r="C41" s="3">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="D41" s="7">
-        <f>B41/C41</f>
-        <v>1.5037593984962405E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.6E-2</v>
       </c>
       <c r="E41" t="s">
         <v>72</v>
@@ -1508,17 +1511,17 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="B42" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="3">
-        <v>336</v>
+        <v>266</v>
       </c>
       <c r="D42" s="7">
-        <f>B42/C42</f>
-        <v>1.488095238095238E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.5037593984962405E-2</v>
       </c>
       <c r="E42" t="s">
         <v>72</v>
@@ -1526,17 +1529,17 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="B43" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C43" s="3">
-        <v>137</v>
+        <v>336</v>
       </c>
       <c r="D43" s="7">
-        <f>B43/C43</f>
-        <v>1.4598540145985401E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.488095238095238E-2</v>
       </c>
       <c r="E43" t="s">
         <v>72</v>
@@ -1544,17 +1547,17 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B44" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C44" s="3">
-        <v>276</v>
+        <v>137</v>
       </c>
       <c r="D44" s="7">
-        <f>B44/C44</f>
-        <v>1.4492753623188406E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.4598540145985401E-2</v>
       </c>
       <c r="E44" t="s">
         <v>72</v>
@@ -1562,17 +1565,17 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="B45" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C45" s="3">
-        <v>208</v>
+        <v>276</v>
       </c>
       <c r="D45" s="7">
-        <f>B45/C45</f>
-        <v>1.4423076923076924E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.4492753623188406E-2</v>
       </c>
       <c r="E45" t="s">
         <v>72</v>
@@ -1580,17 +1583,17 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="B46" s="3">
         <v>3</v>
       </c>
       <c r="C46" s="3">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D46" s="7">
-        <f>B46/C46</f>
-        <v>1.4084507042253521E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.4423076923076924E-2</v>
       </c>
       <c r="E46" t="s">
         <v>72</v>
@@ -1598,17 +1601,17 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="B47" s="3">
         <v>3</v>
       </c>
       <c r="C47" s="3">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D47" s="7">
-        <f>IFERROR(B47/C47," ")</f>
-        <v>1.3636363636363636E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.4084507042253521E-2</v>
       </c>
       <c r="E47" t="s">
         <v>72</v>
@@ -1616,17 +1619,17 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="B48" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C48" s="3">
-        <v>368</v>
+        <v>220</v>
       </c>
       <c r="D48" s="7">
-        <f>B48/C48</f>
-        <v>1.358695652173913E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.3636363636363636E-2</v>
       </c>
       <c r="E48" t="s">
         <v>72</v>
@@ -1634,17 +1637,17 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B49" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C49" s="3">
-        <v>320</v>
+        <v>368</v>
       </c>
       <c r="D49" s="7">
-        <f>B49/C49</f>
-        <v>1.2500000000000001E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.358695652173913E-2</v>
       </c>
       <c r="E49" t="s">
         <v>72</v>
@@ -1652,16 +1655,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="B50" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C50" s="3">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D50" s="7">
-        <f>B50/C50</f>
+        <f t="shared" si="2"/>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="E50" t="s">
@@ -1670,17 +1673,17 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="B51" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C51" s="3">
-        <v>336</v>
+        <v>160</v>
       </c>
       <c r="D51" s="7">
-        <f>B51/C51</f>
-        <v>1.1904761904761904E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="E51" t="s">
         <v>72</v>
@@ -1688,17 +1691,17 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="B52" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C52" s="3">
-        <v>256</v>
+        <v>336</v>
       </c>
       <c r="D52" s="7">
-        <f>B52/C52</f>
-        <v>1.171875E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.1904761904761904E-2</v>
       </c>
       <c r="E52" t="s">
         <v>72</v>
@@ -1706,7 +1709,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="B53" s="3">
         <v>3</v>
@@ -1715,7 +1718,7 @@
         <v>256</v>
       </c>
       <c r="D53" s="7">
-        <f>IFERROR(B53/C53," ")</f>
+        <f t="shared" si="2"/>
         <v>1.171875E-2</v>
       </c>
       <c r="E53" t="s">
@@ -1724,17 +1727,17 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="B54" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C54" s="3">
-        <v>432</v>
+        <v>256</v>
       </c>
       <c r="D54" s="7">
-        <f>B54/C54</f>
-        <v>1.1574074074074073E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.171875E-2</v>
       </c>
       <c r="E54" t="s">
         <v>72</v>
@@ -1742,17 +1745,17 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B55" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C55" s="3">
-        <v>264</v>
+        <v>432</v>
       </c>
       <c r="D55" s="7">
-        <f>B55/C55</f>
-        <v>1.1363636363636364E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.1574074074074073E-2</v>
       </c>
       <c r="E55" t="s">
         <v>72</v>
@@ -1760,16 +1763,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>126</v>
+        <v>55</v>
       </c>
       <c r="B56" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C56" s="3">
-        <v>352</v>
+        <v>264</v>
       </c>
       <c r="D56" s="7">
-        <f>IFERROR(B56/C56," ")</f>
+        <f t="shared" si="2"/>
         <v>1.1363636363636364E-2</v>
       </c>
       <c r="E56" t="s">
@@ -1778,17 +1781,17 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="B57" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C57" s="3">
-        <v>266</v>
+        <v>352</v>
       </c>
       <c r="D57" s="7">
-        <f>B57/C57</f>
-        <v>1.1278195488721804E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.1363636363636364E-2</v>
       </c>
       <c r="E57" t="s">
         <v>72</v>
@@ -1796,17 +1799,17 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B58" s="3">
         <v>3</v>
       </c>
       <c r="C58" s="3">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="D58" s="7">
-        <f>B58/C58</f>
-        <v>1.0830324909747292E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.1278195488721804E-2</v>
       </c>
       <c r="E58" t="s">
         <v>72</v>
@@ -1814,17 +1817,17 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="B59" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C59" s="3">
-        <v>384</v>
+        <v>277</v>
       </c>
       <c r="D59" s="7">
-        <f>B59/C59</f>
-        <v>1.0416666666666666E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.0830324909747292E-2</v>
       </c>
       <c r="E59" t="s">
         <v>72</v>
@@ -1832,7 +1835,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="B60" s="3">
         <v>4</v>
@@ -1841,7 +1844,7 @@
         <v>384</v>
       </c>
       <c r="D60" s="7">
-        <f>B60/C60</f>
+        <f t="shared" si="2"/>
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E60" t="s">
@@ -1850,16 +1853,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="B61" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C61" s="3">
-        <v>288</v>
+        <v>384</v>
       </c>
       <c r="D61" s="7">
-        <f>B61/C61</f>
+        <f t="shared" si="2"/>
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E61" t="s">
@@ -1868,7 +1871,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="B62" s="3">
         <v>3</v>
@@ -1877,7 +1880,7 @@
         <v>288</v>
       </c>
       <c r="D62" s="7">
-        <f>IFERROR(B62/C62," ")</f>
+        <f t="shared" si="2"/>
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E62" t="s">
@@ -1886,17 +1889,17 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="B63" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C63" s="3">
-        <v>400</v>
+        <v>288</v>
       </c>
       <c r="D63" s="7">
-        <f>B63/C63</f>
-        <v>0.01</v>
+        <f t="shared" si="2"/>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E63" t="s">
         <v>72</v>
@@ -1904,16 +1907,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>104</v>
+        <v>24</v>
       </c>
       <c r="B64" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C64" s="3">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D64" s="7">
-        <f>B64/C64</f>
+        <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
       <c r="E64" t="s">
@@ -1922,16 +1925,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B65" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C65" s="3">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D65" s="7">
-        <f>IFERROR(B65/C65," ")</f>
+        <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
       <c r="E65" t="s">
@@ -1940,17 +1943,17 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="B66" s="3">
         <v>4</v>
       </c>
       <c r="C66" s="3">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="D66" s="7">
-        <f>B66/C66</f>
-        <v>9.6153846153846159E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.01</v>
       </c>
       <c r="E66" t="s">
         <v>72</v>
@@ -1958,16 +1961,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B67" s="8">
-        <v>2</v>
+        <v>82</v>
+      </c>
+      <c r="B67" s="3">
+        <v>4</v>
       </c>
       <c r="C67" s="3">
-        <v>208</v>
+        <v>416</v>
       </c>
       <c r="D67" s="7">
-        <f>B67/C67</f>
+        <f t="shared" si="2"/>
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E67" t="s">
@@ -1976,16 +1979,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B68" s="3">
+        <v>15</v>
+      </c>
+      <c r="B68" s="8">
         <v>2</v>
       </c>
       <c r="C68" s="3">
         <v>208</v>
       </c>
       <c r="D68" s="7">
-        <f>B68/C68</f>
+        <f t="shared" si="2"/>
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E68" t="s">
@@ -1994,16 +1997,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>135</v>
+        <v>58</v>
       </c>
       <c r="B69" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C69" s="3">
-        <v>312</v>
+        <v>208</v>
       </c>
       <c r="D69" s="7">
-        <f>IFERROR(B69/C69," ")</f>
+        <f t="shared" si="2"/>
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E69" t="s">
@@ -2012,17 +2015,17 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="B70" s="3">
         <v>3</v>
       </c>
       <c r="C70" s="3">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D70" s="7">
-        <f>B70/C70</f>
-        <v>9.4936708860759497E-3</v>
+        <f t="shared" si="2"/>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E70" t="s">
         <v>72</v>
@@ -2030,17 +2033,17 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="B71" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C71" s="3">
-        <v>432</v>
+        <v>316</v>
       </c>
       <c r="D71" s="7">
-        <f>B71/C71</f>
-        <v>9.2592592592592587E-3</v>
+        <f t="shared" si="2"/>
+        <v>9.4936708860759497E-3</v>
       </c>
       <c r="E71" t="s">
         <v>72</v>
@@ -2048,17 +2051,17 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
       <c r="B72" s="3">
         <v>4</v>
       </c>
       <c r="C72" s="3">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D72" s="7">
-        <f>B72/C72</f>
-        <v>9.1743119266055051E-3</v>
+        <f t="shared" si="2"/>
+        <v>9.2592592592592587E-3</v>
       </c>
       <c r="E72" t="s">
         <v>72</v>
@@ -2066,17 +2069,17 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="B73" s="3">
         <v>4</v>
       </c>
       <c r="C73" s="3">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="D73" s="7">
-        <f>B73/C73</f>
-        <v>9.0090090090090089E-3</v>
+        <f t="shared" si="2"/>
+        <v>9.1743119266055051E-3</v>
       </c>
       <c r="E73" t="s">
         <v>72</v>
@@ -2084,17 +2087,17 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="B74" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C74" s="3">
-        <v>336</v>
+        <v>444</v>
       </c>
       <c r="D74" s="7">
-        <f>B74/C74</f>
-        <v>8.9285714285714281E-3</v>
+        <f t="shared" si="2"/>
+        <v>9.0090090090090089E-3</v>
       </c>
       <c r="E74" t="s">
         <v>72</v>
@@ -2102,17 +2105,17 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B75" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C75" s="3">
-        <v>225</v>
+        <v>336</v>
       </c>
       <c r="D75" s="7">
-        <f>B75/C75</f>
-        <v>8.8888888888888889E-3</v>
+        <f t="shared" si="2"/>
+        <v>8.9285714285714281E-3</v>
       </c>
       <c r="E75" t="s">
         <v>72</v>
@@ -2120,17 +2123,17 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B76" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C76" s="3">
-        <v>344</v>
+        <v>225</v>
       </c>
       <c r="D76" s="7">
-        <f>B76/C76</f>
-        <v>8.7209302325581394E-3</v>
+        <f t="shared" si="2"/>
+        <v>8.8888888888888889E-3</v>
       </c>
       <c r="E76" t="s">
         <v>72</v>
@@ -2138,17 +2141,17 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="B77" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C77" s="3">
-        <v>464</v>
+        <v>344</v>
       </c>
       <c r="D77" s="7">
-        <f>B77/C77</f>
-        <v>8.6206896551724137E-3</v>
+        <f t="shared" si="2"/>
+        <v>8.7209302325581394E-3</v>
       </c>
       <c r="E77" t="s">
         <v>72</v>
@@ -2156,7 +2159,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="B78" s="3">
         <v>4</v>
@@ -2165,7 +2168,7 @@
         <v>464</v>
       </c>
       <c r="D78" s="7">
-        <f>B78/C78</f>
+        <f t="shared" si="2"/>
         <v>8.6206896551724137E-3</v>
       </c>
       <c r="E78" t="s">
@@ -2174,17 +2177,17 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="B79" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C79" s="3">
-        <v>352</v>
+        <v>464</v>
       </c>
       <c r="D79" s="7">
-        <f>B79/C79</f>
-        <v>8.5227272727272721E-3</v>
+        <f t="shared" si="2"/>
+        <v>8.6206896551724137E-3</v>
       </c>
       <c r="E79" t="s">
         <v>72</v>
@@ -2192,7 +2195,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="B80" s="3">
         <v>3</v>
@@ -2201,7 +2204,7 @@
         <v>352</v>
       </c>
       <c r="D80" s="7">
-        <f>IFERROR(B80/C80," ")</f>
+        <f t="shared" ref="D80:D129" si="3">IFERROR(B80/C80," ")</f>
         <v>8.5227272727272721E-3</v>
       </c>
       <c r="E80" t="s">
@@ -2210,17 +2213,17 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>21</v>
+        <v>110</v>
       </c>
       <c r="B81" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C81" s="3">
-        <v>480</v>
+        <v>352</v>
       </c>
       <c r="D81" s="7">
-        <f>B81/C81</f>
-        <v>8.3333333333333332E-3</v>
+        <f t="shared" si="3"/>
+        <v>8.5227272727272721E-3</v>
       </c>
       <c r="E81" t="s">
         <v>72</v>
@@ -2228,16 +2231,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B82" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C82" s="3">
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="D82" s="7">
-        <f>B82/C82</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="E82" t="s">
@@ -2246,16 +2249,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B83" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C83" s="3">
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="D83" s="7">
-        <f>B83/C83</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="E83" t="s">
@@ -2264,17 +2267,17 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B84" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C84" s="3">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="D84" s="7">
-        <f>B84/C84</f>
-        <v>8.152173913043478E-3</v>
+        <f t="shared" si="3"/>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E84" t="s">
         <v>72</v>
@@ -2282,7 +2285,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B85" s="3">
         <v>3</v>
@@ -2291,7 +2294,7 @@
         <v>368</v>
       </c>
       <c r="D85" s="7">
-        <f>B85/C85</f>
+        <f t="shared" si="3"/>
         <v>8.152173913043478E-3</v>
       </c>
       <c r="E85" t="s">
@@ -2300,17 +2303,17 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="B86" s="3">
         <v>3</v>
       </c>
       <c r="C86" s="3">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D86" s="7">
-        <f>B86/C86</f>
-        <v>8.0862533692722376E-3</v>
+        <f t="shared" si="3"/>
+        <v>8.152173913043478E-3</v>
       </c>
       <c r="E86" t="s">
         <v>72</v>
@@ -2318,17 +2321,17 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>5</v>
+        <v>132</v>
       </c>
       <c r="B87" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C87" s="3">
-        <v>499</v>
+        <v>371</v>
       </c>
       <c r="D87" s="7">
-        <f>B87/C87</f>
-        <v>8.0160320641282558E-3</v>
+        <f t="shared" si="3"/>
+        <v>8.0862533692722376E-3</v>
       </c>
       <c r="E87" t="s">
         <v>72</v>
@@ -2336,17 +2339,17 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="B88" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C88" s="3">
-        <v>250</v>
+        <v>499</v>
       </c>
       <c r="D88" s="7">
-        <f>B88/C88</f>
-        <v>8.0000000000000002E-3</v>
+        <f t="shared" si="3"/>
+        <v>8.0160320641282558E-3</v>
       </c>
       <c r="E88" t="s">
         <v>72</v>
@@ -2354,17 +2357,17 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B89" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C89" s="3">
-        <v>512</v>
+        <v>250</v>
       </c>
       <c r="D89" s="7">
-        <f>B89/C89</f>
-        <v>7.8125E-3</v>
+        <f t="shared" si="3"/>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E89" t="s">
         <v>72</v>
@@ -2372,7 +2375,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="B90" s="3">
         <v>4</v>
@@ -2381,7 +2384,7 @@
         <v>512</v>
       </c>
       <c r="D90" s="7">
-        <f>B90/C90</f>
+        <f t="shared" si="3"/>
         <v>7.8125E-3</v>
       </c>
       <c r="E90" t="s">
@@ -2390,17 +2393,17 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="B91" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C91" s="3">
-        <v>264</v>
+        <v>512</v>
       </c>
       <c r="D91" s="7">
-        <f>B91/C91</f>
-        <v>7.575757575757576E-3</v>
+        <f t="shared" si="3"/>
+        <v>7.8125E-3</v>
       </c>
       <c r="E91" t="s">
         <v>72</v>
@@ -2408,17 +2411,17 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B92" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C92" s="3">
-        <v>400</v>
+        <v>264</v>
       </c>
       <c r="D92" s="7">
-        <f>B92/C92</f>
-        <v>7.4999999999999997E-3</v>
+        <f t="shared" si="3"/>
+        <v>7.575757575757576E-3</v>
       </c>
       <c r="E92" t="s">
         <v>72</v>
@@ -2426,17 +2429,17 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B93" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C93" s="3">
-        <v>544</v>
+        <v>400</v>
       </c>
       <c r="D93" s="7">
-        <f>B93/C93</f>
-        <v>7.3529411764705881E-3</v>
+        <f t="shared" si="3"/>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E93" t="s">
         <v>72</v>
@@ -2444,17 +2447,17 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="B94" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C94" s="3">
-        <v>416</v>
+        <v>544</v>
       </c>
       <c r="D94" s="7">
-        <f>IFERROR(B94/C94," ")</f>
-        <v>7.2115384615384619E-3</v>
+        <f t="shared" si="3"/>
+        <v>7.3529411764705881E-3</v>
       </c>
       <c r="E94" t="s">
         <v>72</v>
@@ -2462,17 +2465,17 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="B95" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C95" s="3">
-        <v>560</v>
+        <v>416</v>
       </c>
       <c r="D95" s="7">
-        <f>B95/C95</f>
-        <v>7.1428571428571426E-3</v>
+        <f t="shared" si="3"/>
+        <v>7.2115384615384619E-3</v>
       </c>
       <c r="E95" t="s">
         <v>72</v>
@@ -2480,17 +2483,17 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B96" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C96" s="3">
-        <v>284</v>
+        <v>560</v>
       </c>
       <c r="D96" s="7">
-        <f>B96/C96</f>
-        <v>7.0422535211267607E-3</v>
+        <f t="shared" si="3"/>
+        <v>7.1428571428571426E-3</v>
       </c>
       <c r="E96" t="s">
         <v>72</v>
@@ -2498,17 +2501,17 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="B97" s="3">
         <v>2</v>
       </c>
       <c r="C97" s="3">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D97" s="7">
-        <f>B97/C97</f>
-        <v>6.9444444444444441E-3</v>
+        <f t="shared" si="3"/>
+        <v>7.0422535211267607E-3</v>
       </c>
       <c r="E97" t="s">
         <v>72</v>
@@ -2516,17 +2519,17 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="B98" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C98" s="3">
-        <v>736</v>
+        <v>288</v>
       </c>
       <c r="D98" s="7">
-        <f>IFERROR(B98/C98," ")</f>
-        <v>6.793478260869565E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="E98" t="s">
         <v>72</v>
@@ -2534,17 +2537,17 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>61</v>
+        <v>134</v>
       </c>
       <c r="B99" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C99" s="3">
-        <v>148</v>
+        <v>736</v>
       </c>
       <c r="D99" s="7">
-        <f>B99/C99</f>
-        <v>6.7567567567567571E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.793478260869565E-3</v>
       </c>
       <c r="E99" t="s">
         <v>72</v>
@@ -2552,17 +2555,17 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="B100" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C100" s="3">
-        <v>450</v>
+        <v>148</v>
       </c>
       <c r="D100" s="7">
-        <f>B100/C100</f>
-        <v>6.6666666666666671E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.7567567567567571E-3</v>
       </c>
       <c r="E100" t="s">
         <v>72</v>
@@ -2570,17 +2573,17 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="B101" s="3">
         <v>3</v>
       </c>
       <c r="C101" s="3">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="D101" s="7">
-        <f>IFERROR(B101/C101," ")</f>
-        <v>6.4655172413793103E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.6666666666666671E-3</v>
       </c>
       <c r="E101" t="s">
         <v>72</v>
@@ -2588,17 +2591,17 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="B102" s="3">
         <v>3</v>
       </c>
       <c r="C102" s="3">
-        <v>480</v>
+        <v>464</v>
       </c>
       <c r="D102" s="7">
-        <f>B102/C102</f>
-        <v>6.2500000000000003E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.4655172413793103E-3</v>
       </c>
       <c r="E102" t="s">
         <v>72</v>
@@ -2606,7 +2609,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B103" s="3">
         <v>3</v>
@@ -2615,7 +2618,7 @@
         <v>480</v>
       </c>
       <c r="D103" s="7">
-        <f>B103/C103</f>
+        <f t="shared" si="3"/>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="E103" t="s">
@@ -2624,17 +2627,17 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B104" s="3">
         <v>3</v>
       </c>
       <c r="C104" s="3">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="D104" s="7">
-        <f>B104/C104</f>
-        <v>6.1475409836065573E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E104" t="s">
         <v>72</v>
@@ -2642,17 +2645,17 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B105" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C105" s="3">
-        <v>332</v>
+        <v>488</v>
       </c>
       <c r="D105" s="7">
-        <f>B105/C105</f>
-        <v>6.024096385542169E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.1475409836065573E-3</v>
       </c>
       <c r="E105" t="s">
         <v>72</v>
@@ -2660,7 +2663,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="B106" s="3">
         <v>2</v>
@@ -2669,7 +2672,7 @@
         <v>332</v>
       </c>
       <c r="D106" s="7">
-        <f>B106/C106</f>
+        <f t="shared" si="3"/>
         <v>6.024096385542169E-3</v>
       </c>
       <c r="E106" t="s">
@@ -2678,17 +2681,17 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="B107" s="3">
         <v>2</v>
       </c>
       <c r="C107" s="3">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="D107" s="7">
-        <f>B107/C107</f>
-        <v>5.8139534883720929E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.024096385542169E-3</v>
       </c>
       <c r="E107" t="s">
         <v>72</v>
@@ -2696,17 +2699,17 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="B108" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C108" s="3">
-        <v>704</v>
+        <v>344</v>
       </c>
       <c r="D108" s="7">
-        <f>B108/C108</f>
-        <v>5.681818181818182E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.8139534883720929E-3</v>
       </c>
       <c r="E108" t="s">
         <v>72</v>
@@ -2714,17 +2717,17 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
       <c r="B109" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C109" s="3">
-        <v>366</v>
+        <v>704</v>
       </c>
       <c r="D109" s="7">
-        <f>B109/C109</f>
-        <v>5.4644808743169399E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.681818181818182E-3</v>
       </c>
       <c r="E109" t="s">
         <v>72</v>
@@ -2732,17 +2735,17 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B110" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C110" s="3">
-        <v>736</v>
+        <v>366</v>
       </c>
       <c r="D110" s="7">
-        <f>B110/C110</f>
-        <v>5.434782608695652E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.4644808743169399E-3</v>
       </c>
       <c r="E110" t="s">
         <v>72</v>
@@ -2750,17 +2753,17 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B111" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C111" s="3">
-        <v>373</v>
+        <v>736</v>
       </c>
       <c r="D111" s="7">
-        <f>B111/C111</f>
-        <v>5.3619302949061663E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.434782608695652E-3</v>
       </c>
       <c r="E111" t="s">
         <v>72</v>
@@ -2768,17 +2771,17 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B112" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C112" s="3">
-        <v>560</v>
+        <v>373</v>
       </c>
       <c r="D112" s="7">
-        <f>B112/C112</f>
-        <v>5.3571428571428572E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.3619302949061663E-3</v>
       </c>
       <c r="E112" t="s">
         <v>72</v>
@@ -2786,7 +2789,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B113" s="3">
         <v>3</v>
@@ -2795,7 +2798,7 @@
         <v>560</v>
       </c>
       <c r="D113" s="7">
-        <f>B113/C113</f>
+        <f t="shared" si="3"/>
         <v>5.3571428571428572E-3</v>
       </c>
       <c r="E113" t="s">
@@ -2804,17 +2807,17 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B114" s="3">
         <v>3</v>
       </c>
       <c r="C114" s="3">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="D114" s="7">
-        <f>B114/C114</f>
-        <v>5.208333333333333E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.3571428571428572E-3</v>
       </c>
       <c r="E114" t="s">
         <v>72</v>
@@ -2822,16 +2825,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B115" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C115" s="3">
-        <v>384</v>
+        <v>576</v>
       </c>
       <c r="D115" s="7">
-        <f>B115/C115</f>
+        <f t="shared" si="3"/>
         <v>5.208333333333333E-3</v>
       </c>
       <c r="E115" t="s">
@@ -2840,17 +2843,17 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="B116" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C116" s="3">
-        <v>200</v>
+        <v>384</v>
       </c>
       <c r="D116" s="7">
-        <f>B116/C116</f>
-        <v>5.0000000000000001E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.208333333333333E-3</v>
       </c>
       <c r="E116" t="s">
         <v>72</v>
@@ -2858,16 +2861,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="B117" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C117" s="3">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D117" s="7">
-        <f>B117/C117</f>
+        <f t="shared" si="3"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E117" t="s">
@@ -2876,17 +2879,17 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B118" s="3">
         <v>2</v>
       </c>
       <c r="C118" s="3">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="D118" s="7">
-        <f>B118/C118</f>
-        <v>4.807692307692308E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E118" t="s">
         <v>72</v>
@@ -2894,7 +2897,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B119" s="3">
         <v>2</v>
@@ -2903,7 +2906,7 @@
         <v>416</v>
       </c>
       <c r="D119" s="7">
-        <f>B119/C119</f>
+        <f t="shared" si="3"/>
         <v>4.807692307692308E-3</v>
       </c>
       <c r="E119" t="s">
@@ -2912,17 +2915,17 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="B120" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C120" s="3">
-        <v>848</v>
+        <v>416</v>
       </c>
       <c r="D120" s="7">
-        <f>B120/C120</f>
-        <v>4.7169811320754715E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.807692307692308E-3</v>
       </c>
       <c r="E120" t="s">
         <v>72</v>
@@ -2930,17 +2933,17 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B121" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C121" s="3">
-        <v>440</v>
+        <v>848</v>
       </c>
       <c r="D121" s="7">
-        <f>IFERROR(B121/C121," ")</f>
-        <v>4.5454545454545452E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.7169811320754715E-3</v>
       </c>
       <c r="E121" t="s">
         <v>72</v>
@@ -2948,17 +2951,17 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B122" s="3">
         <v>2</v>
       </c>
       <c r="C122" s="3">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="D122" s="7">
-        <f>B122/C122</f>
-        <v>4.3859649122807015E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.5454545454545452E-3</v>
       </c>
       <c r="E122" t="s">
         <v>72</v>
@@ -2966,17 +2969,17 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="B123" s="3">
         <v>2</v>
       </c>
       <c r="C123" s="3">
-        <v>528</v>
+        <v>456</v>
       </c>
       <c r="D123" s="7">
-        <f>B123/C123</f>
-        <v>3.787878787878788E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.3859649122807015E-3</v>
       </c>
       <c r="E123" t="s">
         <v>72</v>
@@ -2984,17 +2987,17 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B124" s="3">
         <v>2</v>
       </c>
       <c r="C124" s="3">
-        <v>544</v>
+        <v>528</v>
       </c>
       <c r="D124" s="7">
-        <f>B124/C124</f>
-        <v>3.6764705882352941E-3</v>
+        <f t="shared" si="3"/>
+        <v>3.787878787878788E-3</v>
       </c>
       <c r="E124" t="s">
         <v>72</v>
@@ -3002,17 +3005,17 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="B125" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C125" s="3">
-        <v>848</v>
+        <v>544</v>
       </c>
       <c r="D125" s="7">
-        <f>B125/C125</f>
-        <v>3.5377358490566039E-3</v>
+        <f t="shared" si="3"/>
+        <v>3.6764705882352941E-3</v>
       </c>
       <c r="E125" t="s">
         <v>72</v>
@@ -3020,17 +3023,17 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="B126" s="3">
         <v>3</v>
       </c>
       <c r="C126" s="3">
-        <v>864</v>
+        <v>848</v>
       </c>
       <c r="D126" s="7">
-        <f>B126/C126</f>
-        <v>3.472222222222222E-3</v>
+        <f t="shared" si="3"/>
+        <v>3.5377358490566039E-3</v>
       </c>
       <c r="E126" t="s">
         <v>72</v>
@@ -3038,17 +3041,17 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B127" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C127" s="3">
-        <v>616</v>
+        <v>864</v>
       </c>
       <c r="D127" s="7">
-        <f>B127/C127</f>
-        <v>3.246753246753247E-3</v>
+        <f t="shared" si="3"/>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="E127" t="s">
         <v>72</v>
@@ -3056,17 +3059,17 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>95</v>
+        <v>6</v>
       </c>
       <c r="B128" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C128" s="3">
-        <v>320</v>
+        <v>616</v>
       </c>
       <c r="D128" s="7">
-        <f>B128/C128</f>
-        <v>3.1250000000000002E-3</v>
+        <f t="shared" si="3"/>
+        <v>3.246753246753247E-3</v>
       </c>
       <c r="E128" t="s">
         <v>72</v>
@@ -3074,17 +3077,17 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B129" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C129" s="3">
-        <v>1280</v>
+        <v>320</v>
       </c>
       <c r="D129" s="7">
-        <f>IFERROR(B129/C129," ")</f>
-        <v>2.3437499999999999E-3</v>
+        <f t="shared" si="3"/>
+        <v>3.1250000000000002E-3</v>
       </c>
       <c r="E129" t="s">
         <v>72</v>
@@ -3092,542 +3095,554 @@
     </row>
     <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D130" s="7" t="str">
-        <f t="shared" ref="D107:D170" si="1">IFERROR(B130/C130," ")</f>
+        <f>IFERROR(B130/C130," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D131" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B131/C131," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D132" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B132/C132," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D133" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B133/C133," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D134" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B134/C134," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D135" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B135/C135," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D136" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B136/C136," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D137" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B137/C137," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D138" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B138/C138," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D139" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B139/C139," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D140" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B140/C140," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D141" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B141/C141," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D142" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B142/C142," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D143" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B143/C143," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D144" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B144/C144," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="145" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D145" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B145/C145," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="146" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D146" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B146/C146," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="147" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D147" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B147/C147," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="148" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D148" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B148/C148," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="149" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D149" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B149/C149," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="150" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D150" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B150/C150," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="151" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D151" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B151/C151," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="152" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D152" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B152/C152," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="153" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D153" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B153/C153," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="154" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D154" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B154/C154," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="155" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D155" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B155/C155," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="156" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D156" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B156/C156," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="157" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D157" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B157/C157," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="158" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D158" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B158/C158," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="159" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D159" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B159/C159," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="160" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D160" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B160/C160," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="161" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D161" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B161/C161," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="162" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D162" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B162/C162," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="163" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D163" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B163/C163," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="164" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D164" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B164/C164," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="165" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D165" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B165/C165," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="166" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D166" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B166/C166," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="167" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D167" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B167/C167," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="168" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D168" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B168/C168," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="169" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D169" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B169/C169," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="170" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D170" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR(B170/C170," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="171" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D171" s="7" t="str">
-        <f t="shared" ref="D171:D219" si="2">IFERROR(B171/C171," ")</f>
+        <f>IFERROR(B171/C171," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="172" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D172" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B172/C172," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="173" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D173" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B173/C173," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="174" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D174" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B174/C174," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="175" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D175" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B175/C175," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="176" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D176" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B176/C176," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="177" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D177" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B177/C177," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="178" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D178" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B178/C178," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="179" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D179" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B179/C179," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="180" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D180" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B180/C180," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="181" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D181" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B181/C181," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="182" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D182" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B182/C182," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="183" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D183" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B183/C183," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="184" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D184" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B184/C184," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="185" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D185" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B185/C185," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="186" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D186" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B186/C186," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="187" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D187" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B187/C187," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="188" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D188" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B188/C188," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="189" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D189" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B189/C189," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="190" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D190" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B190/C190," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="191" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D191" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B191/C191," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="192" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D192" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B192/C192," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="193" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D193" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B193/C193," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="194" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D194" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B194/C194," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="195" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D195" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B195/C195," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="196" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D196" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B196/C196," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="197" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D197" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B197/C197," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="198" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D198" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B198/C198," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="199" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D199" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B199/C199," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="200" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D200" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B200/C200," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="201" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D201" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B201/C201," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="202" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D202" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B202/C202," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="203" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D203" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B203/C203," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="204" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D204" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B204/C204," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="205" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D205" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B205/C205," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="206" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D206" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B206/C206," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="207" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D207" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>IFERROR(B207/C207," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="208" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D208" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="209" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(B208/C208," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D209" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="210" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(B209/C209," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D210" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="211" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(B210/C210," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D211" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="212" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(B211/C211," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D212" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="213" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(B212/C212," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D213" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="214" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(B213/C213," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D214" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="215" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(B214/C214," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D215" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="216" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(B215/C215," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D216" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="217" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(B216/C216," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D217" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="218" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(B217/C217," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D218" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D219" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <f>IFERROR(B218/C218," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B219" s="3">
+        <v>3</v>
+      </c>
+      <c r="C219" s="3">
+        <v>1280</v>
+      </c>
+      <c r="D219" s="7">
+        <f t="shared" ref="D219" si="4">IFERROR(B219/C219," ")</f>
+        <v>2.3437499999999999E-3</v>
+      </c>
+      <c r="E219" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3642,7 +3657,7 @@
         <filter val="No"/>
       </filters>
     </filterColumn>
-    <sortState ref="A4:E129">
+    <sortState ref="A14:E219">
       <sortCondition descending="1" ref="D2:D218"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Added already printed reports to list
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="144">
   <si>
     <t>Book Ranking</t>
   </si>
@@ -432,6 +432,24 @@
   </si>
   <si>
     <t>Advice Not Given: A Guide for Getting Over Yourself</t>
+  </si>
+  <si>
+    <t>Wisdom and the Context of Knowledge: Knowing that One Doesn't Know: Meacham (Report)</t>
+  </si>
+  <si>
+    <t>A Mathematica Theory of Communication: CE Shannon (Report)</t>
+  </si>
+  <si>
+    <t>The Waste Land: Poem</t>
+  </si>
+  <si>
+    <t>Randomness and Mathematical Proof (Report)</t>
+  </si>
+  <si>
+    <t>Power laws, Pareto distributinos and Zipf's Law (Report)</t>
+  </si>
+  <si>
+    <t>Self-organised criticality-what it is and what it isn't (Report)</t>
   </si>
 </sst>
 </file>
@@ -441,7 +459,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,13 +475,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -475,10 +505,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -492,8 +523,12 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -797,11 +832,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E219"/>
+  <dimension ref="A1:E225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,17 +1042,17 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>88</v>
+        <v>141</v>
       </c>
       <c r="B14" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="3">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="D14" s="7">
-        <f>B14/C14</f>
-        <v>6.8493150684931503E-2</v>
+        <f>IFERROR(B14/C14," ")</f>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E14" t="s">
         <v>72</v>
@@ -1025,17 +1060,17 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>57</v>
+        <v>140</v>
       </c>
       <c r="B15" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="3">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D15" s="7">
-        <f>B15/C15</f>
-        <v>6.6666666666666666E-2</v>
+        <f>IFERROR(B15/C15," ")</f>
+        <v>0.21428571428571427</v>
       </c>
       <c r="E15" t="s">
         <v>72</v>
@@ -1043,17 +1078,17 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="B16" s="3">
         <v>4</v>
       </c>
       <c r="C16" s="3">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="D16" s="7">
-        <f t="shared" ref="D16:D79" si="2">IFERROR(B16/C16," ")</f>
-        <v>5.4054054054054057E-2</v>
+        <f>IFERROR(B16/C16," ")</f>
+        <v>0.2</v>
       </c>
       <c r="E16" t="s">
         <v>72</v>
@@ -1061,17 +1096,17 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="B17" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" s="3">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="D17" s="7">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <f>IFERROR(B17/C17," ")</f>
+        <v>0.15</v>
       </c>
       <c r="E17" t="s">
         <v>72</v>
@@ -1079,35 +1114,35 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
       <c r="B18" s="3">
         <v>3</v>
       </c>
       <c r="C18" s="3">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="D18" s="7">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <f>IFERROR(B18/C18," ")</f>
+        <v>0.12</v>
       </c>
       <c r="E18" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>127</v>
+      <c r="A19" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="B19" s="3">
         <v>5</v>
       </c>
       <c r="C19" s="3">
-        <v>128</v>
+        <v>73</v>
       </c>
       <c r="D19" s="7">
-        <f t="shared" si="2"/>
-        <v>3.90625E-2</v>
+        <f>B19/C19</f>
+        <v>6.8493150684931503E-2</v>
       </c>
       <c r="E19" t="s">
         <v>72</v>
@@ -1115,17 +1150,17 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B20" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C20" s="3">
-        <v>133</v>
+        <v>30</v>
       </c>
       <c r="D20" s="7">
-        <f t="shared" si="2"/>
-        <v>3.7593984962406013E-2</v>
+        <f>B20/C20</f>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="E20" t="s">
         <v>72</v>
@@ -1133,17 +1168,17 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>51</v>
+        <v>139</v>
       </c>
       <c r="B21" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="3">
-        <v>132</v>
+        <v>55</v>
       </c>
       <c r="D21" s="7">
-        <f t="shared" si="2"/>
-        <v>3.0303030303030304E-2</v>
+        <f>IFERROR(B21/C21," ")</f>
+        <v>5.4545454545454543E-2</v>
       </c>
       <c r="E21" t="s">
         <v>72</v>
@@ -1151,17 +1186,17 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B22" s="3">
         <v>4</v>
       </c>
       <c r="C22" s="3">
-        <v>160</v>
+        <v>74</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" si="2"/>
-        <v>2.5000000000000001E-2</v>
+        <f>IFERROR(B22/C22," ")</f>
+        <v>5.4054054054054057E-2</v>
       </c>
       <c r="E22" t="s">
         <v>72</v>
@@ -1169,17 +1204,17 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>129</v>
+        <v>39</v>
       </c>
       <c r="B23" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C23" s="3">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="D23" s="7">
-        <f t="shared" si="2"/>
-        <v>2.5000000000000001E-2</v>
+        <f>IFERROR(B23/C23," ")</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E23" t="s">
         <v>72</v>
@@ -1187,17 +1222,17 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B24" s="3">
         <v>3</v>
       </c>
       <c r="C24" s="3">
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="D24" s="7">
-        <f t="shared" si="2"/>
-        <v>2.4193548387096774E-2</v>
+        <f>IFERROR(B24/C24," ")</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E24" t="s">
         <v>72</v>
@@ -1205,17 +1240,17 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B25" s="3">
         <v>5</v>
       </c>
       <c r="C25" s="3">
-        <v>208</v>
+        <v>128</v>
       </c>
       <c r="D25" s="7">
-        <f t="shared" si="2"/>
-        <v>2.403846153846154E-2</v>
+        <f>IFERROR(B25/C25," ")</f>
+        <v>3.90625E-2</v>
       </c>
       <c r="E25" t="s">
         <v>72</v>
@@ -1223,17 +1258,17 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B26" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C26" s="3">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D26" s="7">
-        <f t="shared" si="2"/>
-        <v>2.34375E-2</v>
+        <f>IFERROR(B26/C26," ")</f>
+        <v>3.7593984962406013E-2</v>
       </c>
       <c r="E26" t="s">
         <v>72</v>
@@ -1241,17 +1276,17 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="B27" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="3">
-        <v>224</v>
+        <v>132</v>
       </c>
       <c r="D27" s="7">
-        <f t="shared" si="2"/>
-        <v>2.2321428571428572E-2</v>
+        <f>IFERROR(B27/C27," ")</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="E27" t="s">
         <v>72</v>
@@ -1259,17 +1294,17 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B28" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="3">
-        <v>228</v>
+        <v>160</v>
       </c>
       <c r="D28" s="7">
-        <f t="shared" si="2"/>
-        <v>2.1929824561403508E-2</v>
+        <f>IFERROR(B28/C28," ")</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E28" t="s">
         <v>72</v>
@@ -1277,17 +1312,17 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="B29" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C29" s="3">
-        <v>191</v>
+        <v>80</v>
       </c>
       <c r="D29" s="7">
-        <f t="shared" si="2"/>
-        <v>2.0942408376963352E-2</v>
+        <f>IFERROR(B29/C29," ")</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E29" t="s">
         <v>72</v>
@@ -1295,17 +1330,17 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="B30" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3">
-        <v>192</v>
+        <v>124</v>
       </c>
       <c r="D30" s="7">
-        <f t="shared" si="2"/>
-        <v>2.0833333333333332E-2</v>
+        <f>IFERROR(B30/C30," ")</f>
+        <v>2.4193548387096774E-2</v>
       </c>
       <c r="E30" t="s">
         <v>72</v>
@@ -1313,17 +1348,17 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B31" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" s="3">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="D31" s="7">
-        <f t="shared" si="2"/>
-        <v>2.0202020202020204E-2</v>
+        <f>IFERROR(B31/C31," ")</f>
+        <v>2.403846153846154E-2</v>
       </c>
       <c r="E31" t="s">
         <v>72</v>
@@ -1331,17 +1366,17 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="B32" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C32" s="3">
-        <v>258</v>
+        <v>128</v>
       </c>
       <c r="D32" s="7">
-        <f t="shared" si="2"/>
-        <v>1.937984496124031E-2</v>
+        <f>IFERROR(B32/C32," ")</f>
+        <v>2.34375E-2</v>
       </c>
       <c r="E32" t="s">
         <v>72</v>
@@ -1349,17 +1384,17 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="B33" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C33" s="3">
-        <v>157</v>
+        <v>224</v>
       </c>
       <c r="D33" s="7">
-        <f t="shared" si="2"/>
-        <v>1.9108280254777069E-2</v>
+        <f>IFERROR(B33/C33," ")</f>
+        <v>2.2321428571428572E-2</v>
       </c>
       <c r="E33" t="s">
         <v>72</v>
@@ -1367,17 +1402,17 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B34" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C34" s="3">
-        <v>160</v>
+        <v>228</v>
       </c>
       <c r="D34" s="7">
-        <f t="shared" si="2"/>
-        <v>1.8749999999999999E-2</v>
+        <f>IFERROR(B34/C34," ")</f>
+        <v>2.1929824561403508E-2</v>
       </c>
       <c r="E34" t="s">
         <v>72</v>
@@ -1385,17 +1420,17 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B35" s="3">
         <v>4</v>
       </c>
       <c r="C35" s="3">
-        <v>224</v>
+        <v>191</v>
       </c>
       <c r="D35" s="7">
-        <f t="shared" si="2"/>
-        <v>1.7857142857142856E-2</v>
+        <f>IFERROR(B35/C35," ")</f>
+        <v>2.0942408376963352E-2</v>
       </c>
       <c r="E35" t="s">
         <v>72</v>
@@ -1403,17 +1438,17 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="B36" s="3">
         <v>4</v>
       </c>
       <c r="C36" s="3">
-        <v>226</v>
+        <v>192</v>
       </c>
       <c r="D36" s="7">
-        <f t="shared" si="2"/>
-        <v>1.7699115044247787E-2</v>
+        <f>IFERROR(B36/C36," ")</f>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="E36" t="s">
         <v>72</v>
@@ -1421,17 +1456,17 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
       <c r="B37" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" s="3">
-        <v>288</v>
+        <v>198</v>
       </c>
       <c r="D37" s="7">
-        <f t="shared" si="2"/>
-        <v>1.7361111111111112E-2</v>
+        <f>IFERROR(B37/C37," ")</f>
+        <v>2.0202020202020204E-2</v>
       </c>
       <c r="E37" t="s">
         <v>72</v>
@@ -1439,17 +1474,17 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B38" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C38" s="3">
-        <v>231</v>
+        <v>258</v>
       </c>
       <c r="D38" s="7">
-        <f t="shared" si="2"/>
-        <v>1.7316017316017316E-2</v>
+        <f>IFERROR(B38/C38," ")</f>
+        <v>1.937984496124031E-2</v>
       </c>
       <c r="E38" t="s">
         <v>72</v>
@@ -1457,17 +1492,17 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="B39" s="3">
         <v>3</v>
       </c>
       <c r="C39" s="3">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D39" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6574585635359115E-2</v>
+        <f>IFERROR(B39/C39," ")</f>
+        <v>1.9108280254777069E-2</v>
       </c>
       <c r="E39" t="s">
         <v>72</v>
@@ -1475,17 +1510,17 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="B40" s="3">
         <v>3</v>
       </c>
       <c r="C40" s="3">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6483516483516484E-2</v>
+        <f>IFERROR(B40/C40," ")</f>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="E40" t="s">
         <v>72</v>
@@ -1493,17 +1528,17 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B41" s="3">
         <v>4</v>
       </c>
       <c r="C41" s="3">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="D41" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6E-2</v>
+        <f>IFERROR(B41/C41," ")</f>
+        <v>1.7857142857142856E-2</v>
       </c>
       <c r="E41" t="s">
         <v>72</v>
@@ -1511,17 +1546,17 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B42" s="3">
         <v>4</v>
       </c>
       <c r="C42" s="3">
-        <v>266</v>
+        <v>226</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5037593984962405E-2</v>
+        <f>IFERROR(B42/C42," ")</f>
+        <v>1.7699115044247787E-2</v>
       </c>
       <c r="E42" t="s">
         <v>72</v>
@@ -1529,17 +1564,17 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B43" s="3">
         <v>5</v>
       </c>
       <c r="C43" s="3">
-        <v>336</v>
+        <v>288</v>
       </c>
       <c r="D43" s="7">
-        <f t="shared" si="2"/>
-        <v>1.488095238095238E-2</v>
+        <f>IFERROR(B43/C43," ")</f>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="E43" t="s">
         <v>72</v>
@@ -1547,17 +1582,17 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B44" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C44" s="3">
-        <v>137</v>
+        <v>231</v>
       </c>
       <c r="D44" s="7">
-        <f t="shared" si="2"/>
-        <v>1.4598540145985401E-2</v>
+        <f>IFERROR(B44/C44," ")</f>
+        <v>1.7316017316017316E-2</v>
       </c>
       <c r="E44" t="s">
         <v>72</v>
@@ -1565,17 +1600,17 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="B45" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C45" s="3">
-        <v>276</v>
+        <v>181</v>
       </c>
       <c r="D45" s="7">
-        <f t="shared" si="2"/>
-        <v>1.4492753623188406E-2</v>
+        <f>IFERROR(B45/C45," ")</f>
+        <v>1.6574585635359115E-2</v>
       </c>
       <c r="E45" t="s">
         <v>72</v>
@@ -1583,17 +1618,17 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B46" s="3">
         <v>3</v>
       </c>
       <c r="C46" s="3">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="D46" s="7">
-        <f t="shared" si="2"/>
-        <v>1.4423076923076924E-2</v>
+        <f>IFERROR(B46/C46," ")</f>
+        <v>1.6483516483516484E-2</v>
       </c>
       <c r="E46" t="s">
         <v>72</v>
@@ -1601,17 +1636,17 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="B47" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C47" s="3">
-        <v>213</v>
+        <v>250</v>
       </c>
       <c r="D47" s="7">
-        <f t="shared" si="2"/>
-        <v>1.4084507042253521E-2</v>
+        <f>IFERROR(B47/C47," ")</f>
+        <v>1.6E-2</v>
       </c>
       <c r="E47" t="s">
         <v>72</v>
@@ -1619,17 +1654,17 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B48" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C48" s="3">
-        <v>220</v>
+        <v>266</v>
       </c>
       <c r="D48" s="7">
-        <f t="shared" si="2"/>
-        <v>1.3636363636363636E-2</v>
+        <f>IFERROR(B48/C48," ")</f>
+        <v>1.5037593984962405E-2</v>
       </c>
       <c r="E48" t="s">
         <v>72</v>
@@ -1637,17 +1672,17 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B49" s="3">
         <v>5</v>
       </c>
       <c r="C49" s="3">
-        <v>368</v>
+        <v>336</v>
       </c>
       <c r="D49" s="7">
-        <f t="shared" si="2"/>
-        <v>1.358695652173913E-2</v>
+        <f>IFERROR(B49/C49," ")</f>
+        <v>1.488095238095238E-2</v>
       </c>
       <c r="E49" t="s">
         <v>72</v>
@@ -1655,17 +1690,17 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="B50" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C50" s="3">
-        <v>320</v>
+        <v>137</v>
       </c>
       <c r="D50" s="7">
-        <f t="shared" si="2"/>
-        <v>1.2500000000000001E-2</v>
+        <f>IFERROR(B50/C50," ")</f>
+        <v>1.4598540145985401E-2</v>
       </c>
       <c r="E50" t="s">
         <v>72</v>
@@ -1673,17 +1708,17 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B51" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C51" s="3">
-        <v>160</v>
+        <v>276</v>
       </c>
       <c r="D51" s="7">
-        <f t="shared" si="2"/>
-        <v>1.2500000000000001E-2</v>
+        <f>IFERROR(B51/C51," ")</f>
+        <v>1.4492753623188406E-2</v>
       </c>
       <c r="E51" t="s">
         <v>72</v>
@@ -1691,17 +1726,17 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="B52" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52" s="3">
-        <v>336</v>
+        <v>208</v>
       </c>
       <c r="D52" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1904761904761904E-2</v>
+        <f>IFERROR(B52/C52," ")</f>
+        <v>1.4423076923076924E-2</v>
       </c>
       <c r="E52" t="s">
         <v>72</v>
@@ -1709,17 +1744,17 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="B53" s="3">
         <v>3</v>
       </c>
       <c r="C53" s="3">
-        <v>256</v>
+        <v>213</v>
       </c>
       <c r="D53" s="7">
-        <f t="shared" si="2"/>
-        <v>1.171875E-2</v>
+        <f>IFERROR(B53/C53," ")</f>
+        <v>1.4084507042253521E-2</v>
       </c>
       <c r="E53" t="s">
         <v>72</v>
@@ -1727,17 +1762,17 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B54" s="3">
         <v>3</v>
       </c>
       <c r="C54" s="3">
-        <v>256</v>
+        <v>220</v>
       </c>
       <c r="D54" s="7">
-        <f t="shared" si="2"/>
-        <v>1.171875E-2</v>
+        <f>IFERROR(B54/C54," ")</f>
+        <v>1.3636363636363636E-2</v>
       </c>
       <c r="E54" t="s">
         <v>72</v>
@@ -1745,17 +1780,17 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="B55" s="3">
         <v>5</v>
       </c>
       <c r="C55" s="3">
-        <v>432</v>
+        <v>368</v>
       </c>
       <c r="D55" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1574074074074073E-2</v>
+        <f>IFERROR(B55/C55," ")</f>
+        <v>1.358695652173913E-2</v>
       </c>
       <c r="E55" t="s">
         <v>72</v>
@@ -1763,17 +1798,17 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B56" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C56" s="3">
-        <v>264</v>
+        <v>320</v>
       </c>
       <c r="D56" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1363636363636364E-2</v>
+        <f>IFERROR(B56/C56," ")</f>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="E56" t="s">
         <v>72</v>
@@ -1781,17 +1816,17 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="B57" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C57" s="3">
-        <v>352</v>
+        <v>160</v>
       </c>
       <c r="D57" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1363636363636364E-2</v>
+        <f>IFERROR(B57/C57," ")</f>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="E57" t="s">
         <v>72</v>
@@ -1799,17 +1834,17 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B58" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C58" s="3">
-        <v>266</v>
+        <v>336</v>
       </c>
       <c r="D58" s="7">
-        <f t="shared" si="2"/>
-        <v>1.1278195488721804E-2</v>
+        <f>IFERROR(B58/C58," ")</f>
+        <v>1.1904761904761904E-2</v>
       </c>
       <c r="E58" t="s">
         <v>72</v>
@@ -1817,17 +1852,17 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="B59" s="3">
         <v>3</v>
       </c>
       <c r="C59" s="3">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="D59" s="7">
-        <f t="shared" si="2"/>
-        <v>1.0830324909747292E-2</v>
+        <f>IFERROR(B59/C59," ")</f>
+        <v>1.171875E-2</v>
       </c>
       <c r="E59" t="s">
         <v>72</v>
@@ -1835,17 +1870,17 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="B60" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C60" s="3">
-        <v>384</v>
+        <v>256</v>
       </c>
       <c r="D60" s="7">
-        <f t="shared" si="2"/>
-        <v>1.0416666666666666E-2</v>
+        <f>IFERROR(B60/C60," ")</f>
+        <v>1.171875E-2</v>
       </c>
       <c r="E60" t="s">
         <v>72</v>
@@ -1853,17 +1888,17 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B61" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C61" s="3">
-        <v>384</v>
+        <v>432</v>
       </c>
       <c r="D61" s="7">
-        <f t="shared" si="2"/>
-        <v>1.0416666666666666E-2</v>
+        <f>IFERROR(B61/C61," ")</f>
+        <v>1.1574074074074073E-2</v>
       </c>
       <c r="E61" t="s">
         <v>72</v>
@@ -1871,17 +1906,17 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B62" s="3">
         <v>3</v>
       </c>
       <c r="C62" s="3">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="D62" s="7">
-        <f t="shared" si="2"/>
-        <v>1.0416666666666666E-2</v>
+        <f>IFERROR(B62/C62," ")</f>
+        <v>1.1363636363636364E-2</v>
       </c>
       <c r="E62" t="s">
         <v>72</v>
@@ -1889,17 +1924,17 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="B63" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C63" s="3">
-        <v>288</v>
+        <v>352</v>
       </c>
       <c r="D63" s="7">
-        <f t="shared" si="2"/>
-        <v>1.0416666666666666E-2</v>
+        <f>IFERROR(B63/C63," ")</f>
+        <v>1.1363636363636364E-2</v>
       </c>
       <c r="E63" t="s">
         <v>72</v>
@@ -1907,17 +1942,17 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B64" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C64" s="3">
-        <v>400</v>
+        <v>266</v>
       </c>
       <c r="D64" s="7">
-        <f t="shared" si="2"/>
-        <v>0.01</v>
+        <f>IFERROR(B64/C64," ")</f>
+        <v>1.1278195488721804E-2</v>
       </c>
       <c r="E64" t="s">
         <v>72</v>
@@ -1925,17 +1960,17 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B65" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C65" s="3">
-        <v>200</v>
+        <v>277</v>
       </c>
       <c r="D65" s="7">
-        <f t="shared" si="2"/>
-        <v>0.01</v>
+        <f>IFERROR(B65/C65," ")</f>
+        <v>1.0830324909747292E-2</v>
       </c>
       <c r="E65" t="s">
         <v>72</v>
@@ -1943,17 +1978,17 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="B66" s="3">
         <v>4</v>
       </c>
       <c r="C66" s="3">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="D66" s="7">
-        <f t="shared" si="2"/>
-        <v>0.01</v>
+        <f>IFERROR(B66/C66," ")</f>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E66" t="s">
         <v>72</v>
@@ -1961,17 +1996,17 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B67" s="3">
         <v>4</v>
       </c>
       <c r="C67" s="3">
-        <v>416</v>
+        <v>384</v>
       </c>
       <c r="D67" s="7">
-        <f t="shared" si="2"/>
-        <v>9.6153846153846159E-3</v>
+        <f>IFERROR(B67/C67," ")</f>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E67" t="s">
         <v>72</v>
@@ -1979,17 +2014,17 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B68" s="8">
-        <v>2</v>
+        <v>42</v>
+      </c>
+      <c r="B68" s="3">
+        <v>3</v>
       </c>
       <c r="C68" s="3">
-        <v>208</v>
+        <v>288</v>
       </c>
       <c r="D68" s="7">
-        <f t="shared" si="2"/>
-        <v>9.6153846153846159E-3</v>
+        <f>IFERROR(B68/C68," ")</f>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E68" t="s">
         <v>72</v>
@@ -1997,17 +2032,17 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B69" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C69" s="3">
-        <v>208</v>
+        <v>288</v>
       </c>
       <c r="D69" s="7">
-        <f t="shared" si="2"/>
-        <v>9.6153846153846159E-3</v>
+        <f>IFERROR(B69/C69," ")</f>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E69" t="s">
         <v>72</v>
@@ -2015,17 +2050,17 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>135</v>
+        <v>24</v>
       </c>
       <c r="B70" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C70" s="3">
-        <v>312</v>
+        <v>400</v>
       </c>
       <c r="D70" s="7">
-        <f t="shared" si="2"/>
-        <v>9.6153846153846159E-3</v>
+        <f>IFERROR(B70/C70," ")</f>
+        <v>0.01</v>
       </c>
       <c r="E70" t="s">
         <v>72</v>
@@ -2033,17 +2068,17 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B71" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" s="3">
-        <v>316</v>
+        <v>200</v>
       </c>
       <c r="D71" s="7">
-        <f t="shared" si="2"/>
-        <v>9.4936708860759497E-3</v>
+        <f>IFERROR(B71/C71," ")</f>
+        <v>0.01</v>
       </c>
       <c r="E71" t="s">
         <v>72</v>
@@ -2051,17 +2086,17 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="B72" s="3">
         <v>4</v>
       </c>
       <c r="C72" s="3">
-        <v>432</v>
+        <v>400</v>
       </c>
       <c r="D72" s="7">
-        <f t="shared" si="2"/>
-        <v>9.2592592592592587E-3</v>
+        <f>IFERROR(B72/C72," ")</f>
+        <v>0.01</v>
       </c>
       <c r="E72" t="s">
         <v>72</v>
@@ -2069,17 +2104,17 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B73" s="3">
         <v>4</v>
       </c>
       <c r="C73" s="3">
-        <v>436</v>
+        <v>416</v>
       </c>
       <c r="D73" s="7">
-        <f t="shared" si="2"/>
-        <v>9.1743119266055051E-3</v>
+        <f>IFERROR(B73/C73," ")</f>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E73" t="s">
         <v>72</v>
@@ -2087,17 +2122,17 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B74" s="3">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c r="B74" s="8">
+        <v>2</v>
       </c>
       <c r="C74" s="3">
-        <v>444</v>
+        <v>208</v>
       </c>
       <c r="D74" s="7">
-        <f t="shared" si="2"/>
-        <v>9.0090090090090089E-3</v>
+        <f>IFERROR(B74/C74," ")</f>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E74" t="s">
         <v>72</v>
@@ -2105,17 +2140,17 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B75" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75" s="3">
-        <v>336</v>
+        <v>208</v>
       </c>
       <c r="D75" s="7">
-        <f t="shared" si="2"/>
-        <v>8.9285714285714281E-3</v>
+        <f>IFERROR(B75/C75," ")</f>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E75" t="s">
         <v>72</v>
@@ -2123,17 +2158,17 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>74</v>
+        <v>135</v>
       </c>
       <c r="B76" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C76" s="3">
-        <v>225</v>
+        <v>312</v>
       </c>
       <c r="D76" s="7">
-        <f t="shared" si="2"/>
-        <v>8.8888888888888889E-3</v>
+        <f>IFERROR(B76/C76," ")</f>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="E76" t="s">
         <v>72</v>
@@ -2141,17 +2176,17 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B77" s="3">
         <v>3</v>
       </c>
       <c r="C77" s="3">
-        <v>344</v>
+        <v>316</v>
       </c>
       <c r="D77" s="7">
-        <f t="shared" si="2"/>
-        <v>8.7209302325581394E-3</v>
+        <f>IFERROR(B77/C77," ")</f>
+        <v>9.4936708860759497E-3</v>
       </c>
       <c r="E77" t="s">
         <v>72</v>
@@ -2159,17 +2194,17 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="B78" s="3">
         <v>4</v>
       </c>
       <c r="C78" s="3">
-        <v>464</v>
+        <v>432</v>
       </c>
       <c r="D78" s="7">
-        <f t="shared" si="2"/>
-        <v>8.6206896551724137E-3</v>
+        <f>IFERROR(B78/C78," ")</f>
+        <v>9.2592592592592587E-3</v>
       </c>
       <c r="E78" t="s">
         <v>72</v>
@@ -2177,17 +2212,17 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B79" s="3">
         <v>4</v>
       </c>
       <c r="C79" s="3">
-        <v>464</v>
+        <v>436</v>
       </c>
       <c r="D79" s="7">
-        <f t="shared" si="2"/>
-        <v>8.6206896551724137E-3</v>
+        <f>IFERROR(B79/C79," ")</f>
+        <v>9.1743119266055051E-3</v>
       </c>
       <c r="E79" t="s">
         <v>72</v>
@@ -2195,17 +2230,17 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B80" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C80" s="3">
-        <v>352</v>
+        <v>444</v>
       </c>
       <c r="D80" s="7">
-        <f t="shared" ref="D80:D129" si="3">IFERROR(B80/C80," ")</f>
-        <v>8.5227272727272721E-3</v>
+        <f>IFERROR(B80/C80," ")</f>
+        <v>9.0090090090090089E-3</v>
       </c>
       <c r="E80" t="s">
         <v>72</v>
@@ -2213,17 +2248,17 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="B81" s="3">
         <v>3</v>
       </c>
       <c r="C81" s="3">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="D81" s="7">
-        <f t="shared" si="3"/>
-        <v>8.5227272727272721E-3</v>
+        <f>IFERROR(B81/C81," ")</f>
+        <v>8.9285714285714281E-3</v>
       </c>
       <c r="E81" t="s">
         <v>72</v>
@@ -2231,17 +2266,17 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="B82" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C82" s="3">
-        <v>480</v>
+        <v>225</v>
       </c>
       <c r="D82" s="7">
-        <f t="shared" si="3"/>
-        <v>8.3333333333333332E-3</v>
+        <f>IFERROR(B82/C82," ")</f>
+        <v>8.8888888888888889E-3</v>
       </c>
       <c r="E82" t="s">
         <v>72</v>
@@ -2249,17 +2284,17 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="B83" s="3">
         <v>3</v>
       </c>
       <c r="C83" s="3">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="D83" s="7">
-        <f t="shared" si="3"/>
-        <v>8.3333333333333332E-3</v>
+        <f>IFERROR(B83/C83," ")</f>
+        <v>8.7209302325581394E-3</v>
       </c>
       <c r="E83" t="s">
         <v>72</v>
@@ -2267,17 +2302,17 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B84" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C84" s="3">
-        <v>240</v>
+        <v>464</v>
       </c>
       <c r="D84" s="7">
-        <f t="shared" si="3"/>
-        <v>8.3333333333333332E-3</v>
+        <f>IFERROR(B84/C84," ")</f>
+        <v>8.6206896551724137E-3</v>
       </c>
       <c r="E84" t="s">
         <v>72</v>
@@ -2285,17 +2320,17 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="B85" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C85" s="3">
-        <v>368</v>
+        <v>464</v>
       </c>
       <c r="D85" s="7">
-        <f t="shared" si="3"/>
-        <v>8.152173913043478E-3</v>
+        <f>IFERROR(B85/C85," ")</f>
+        <v>8.6206896551724137E-3</v>
       </c>
       <c r="E85" t="s">
         <v>72</v>
@@ -2303,17 +2338,17 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B86" s="3">
         <v>3</v>
       </c>
       <c r="C86" s="3">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="D86" s="7">
-        <f t="shared" si="3"/>
-        <v>8.152173913043478E-3</v>
+        <f>IFERROR(B86/C86," ")</f>
+        <v>8.5227272727272721E-3</v>
       </c>
       <c r="E86" t="s">
         <v>72</v>
@@ -2321,17 +2356,17 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B87" s="3">
         <v>3</v>
       </c>
       <c r="C87" s="3">
-        <v>371</v>
+        <v>352</v>
       </c>
       <c r="D87" s="7">
-        <f t="shared" si="3"/>
-        <v>8.0862533692722376E-3</v>
+        <f>IFERROR(B87/C87," ")</f>
+        <v>8.5227272727272721E-3</v>
       </c>
       <c r="E87" t="s">
         <v>72</v>
@@ -2339,17 +2374,17 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B88" s="3">
         <v>4</v>
       </c>
       <c r="C88" s="3">
-        <v>499</v>
+        <v>480</v>
       </c>
       <c r="D88" s="7">
-        <f t="shared" si="3"/>
-        <v>8.0160320641282558E-3</v>
+        <f>IFERROR(B88/C88," ")</f>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E88" t="s">
         <v>72</v>
@@ -2357,17 +2392,17 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="B89" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C89" s="3">
-        <v>250</v>
+        <v>360</v>
       </c>
       <c r="D89" s="7">
-        <f t="shared" si="3"/>
-        <v>8.0000000000000002E-3</v>
+        <f>IFERROR(B89/C89," ")</f>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E89" t="s">
         <v>72</v>
@@ -2375,17 +2410,17 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B90" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C90" s="3">
-        <v>512</v>
+        <v>240</v>
       </c>
       <c r="D90" s="7">
-        <f t="shared" si="3"/>
-        <v>7.8125E-3</v>
+        <f>IFERROR(B90/C90," ")</f>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E90" t="s">
         <v>72</v>
@@ -2393,17 +2428,17 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="B91" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C91" s="3">
-        <v>512</v>
+        <v>368</v>
       </c>
       <c r="D91" s="7">
-        <f t="shared" si="3"/>
-        <v>7.8125E-3</v>
+        <f>IFERROR(B91/C91," ")</f>
+        <v>8.152173913043478E-3</v>
       </c>
       <c r="E91" t="s">
         <v>72</v>
@@ -2411,17 +2446,17 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B92" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C92" s="3">
-        <v>264</v>
+        <v>368</v>
       </c>
       <c r="D92" s="7">
-        <f t="shared" si="3"/>
-        <v>7.575757575757576E-3</v>
+        <f>IFERROR(B92/C92," ")</f>
+        <v>8.152173913043478E-3</v>
       </c>
       <c r="E92" t="s">
         <v>72</v>
@@ -2429,17 +2464,17 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="B93" s="3">
         <v>3</v>
       </c>
       <c r="C93" s="3">
-        <v>400</v>
+        <v>371</v>
       </c>
       <c r="D93" s="7">
-        <f t="shared" si="3"/>
-        <v>7.4999999999999997E-3</v>
+        <f>IFERROR(B93/C93," ")</f>
+        <v>8.0862533692722376E-3</v>
       </c>
       <c r="E93" t="s">
         <v>72</v>
@@ -2447,17 +2482,17 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="B94" s="3">
         <v>4</v>
       </c>
       <c r="C94" s="3">
-        <v>544</v>
+        <v>499</v>
       </c>
       <c r="D94" s="7">
-        <f t="shared" si="3"/>
-        <v>7.3529411764705881E-3</v>
+        <f>IFERROR(B94/C94," ")</f>
+        <v>8.0160320641282558E-3</v>
       </c>
       <c r="E94" t="s">
         <v>72</v>
@@ -2465,17 +2500,17 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="B95" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C95" s="3">
-        <v>416</v>
+        <v>250</v>
       </c>
       <c r="D95" s="7">
-        <f t="shared" si="3"/>
-        <v>7.2115384615384619E-3</v>
+        <f>IFERROR(B95/C95," ")</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E95" t="s">
         <v>72</v>
@@ -2483,17 +2518,17 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B96" s="3">
         <v>4</v>
       </c>
       <c r="C96" s="3">
-        <v>560</v>
+        <v>512</v>
       </c>
       <c r="D96" s="7">
-        <f t="shared" si="3"/>
-        <v>7.1428571428571426E-3</v>
+        <f>IFERROR(B96/C96," ")</f>
+        <v>7.8125E-3</v>
       </c>
       <c r="E96" t="s">
         <v>72</v>
@@ -2501,17 +2536,17 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="B97" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C97" s="3">
-        <v>284</v>
+        <v>512</v>
       </c>
       <c r="D97" s="7">
-        <f t="shared" si="3"/>
-        <v>7.0422535211267607E-3</v>
+        <f>IFERROR(B97/C97," ")</f>
+        <v>7.8125E-3</v>
       </c>
       <c r="E97" t="s">
         <v>72</v>
@@ -2519,17 +2554,17 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B98" s="3">
         <v>2</v>
       </c>
       <c r="C98" s="3">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="D98" s="7">
-        <f t="shared" si="3"/>
-        <v>6.9444444444444441E-3</v>
+        <f>IFERROR(B98/C98," ")</f>
+        <v>7.575757575757576E-3</v>
       </c>
       <c r="E98" t="s">
         <v>72</v>
@@ -2537,17 +2572,17 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>134</v>
+        <v>53</v>
       </c>
       <c r="B99" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C99" s="3">
-        <v>736</v>
+        <v>400</v>
       </c>
       <c r="D99" s="7">
-        <f t="shared" si="3"/>
-        <v>6.793478260869565E-3</v>
+        <f>IFERROR(B99/C99," ")</f>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E99" t="s">
         <v>72</v>
@@ -2555,17 +2590,17 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B100" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C100" s="3">
-        <v>148</v>
+        <v>544</v>
       </c>
       <c r="D100" s="7">
-        <f t="shared" si="3"/>
-        <v>6.7567567567567571E-3</v>
+        <f>IFERROR(B100/C100," ")</f>
+        <v>7.3529411764705881E-3</v>
       </c>
       <c r="E100" t="s">
         <v>72</v>
@@ -2573,17 +2608,17 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="B101" s="3">
         <v>3</v>
       </c>
       <c r="C101" s="3">
-        <v>450</v>
+        <v>416</v>
       </c>
       <c r="D101" s="7">
-        <f t="shared" si="3"/>
-        <v>6.6666666666666671E-3</v>
+        <f>IFERROR(B101/C101," ")</f>
+        <v>7.2115384615384619E-3</v>
       </c>
       <c r="E101" t="s">
         <v>72</v>
@@ -2591,17 +2626,17 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="B102" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C102" s="3">
-        <v>464</v>
+        <v>560</v>
       </c>
       <c r="D102" s="7">
-        <f t="shared" si="3"/>
-        <v>6.4655172413793103E-3</v>
+        <f>IFERROR(B102/C102," ")</f>
+        <v>7.1428571428571426E-3</v>
       </c>
       <c r="E102" t="s">
         <v>72</v>
@@ -2609,17 +2644,17 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B103" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C103" s="3">
-        <v>480</v>
+        <v>284</v>
       </c>
       <c r="D103" s="7">
-        <f t="shared" si="3"/>
-        <v>6.2500000000000003E-3</v>
+        <f>IFERROR(B103/C103," ")</f>
+        <v>7.0422535211267607E-3</v>
       </c>
       <c r="E103" t="s">
         <v>72</v>
@@ -2627,17 +2662,17 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B104" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C104" s="3">
-        <v>480</v>
+        <v>288</v>
       </c>
       <c r="D104" s="7">
-        <f t="shared" si="3"/>
-        <v>6.2500000000000003E-3</v>
+        <f>IFERROR(B104/C104," ")</f>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="E104" t="s">
         <v>72</v>
@@ -2645,17 +2680,17 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
       <c r="B105" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C105" s="3">
-        <v>488</v>
+        <v>736</v>
       </c>
       <c r="D105" s="7">
-        <f t="shared" si="3"/>
-        <v>6.1475409836065573E-3</v>
+        <f>IFERROR(B105/C105," ")</f>
+        <v>6.793478260869565E-3</v>
       </c>
       <c r="E105" t="s">
         <v>72</v>
@@ -2663,17 +2698,17 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B106" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C106" s="3">
-        <v>332</v>
+        <v>148</v>
       </c>
       <c r="D106" s="7">
-        <f t="shared" si="3"/>
-        <v>6.024096385542169E-3</v>
+        <f>IFERROR(B106/C106," ")</f>
+        <v>6.7567567567567571E-3</v>
       </c>
       <c r="E106" t="s">
         <v>72</v>
@@ -2681,17 +2716,17 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B107" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C107" s="3">
-        <v>332</v>
+        <v>450</v>
       </c>
       <c r="D107" s="7">
-        <f t="shared" si="3"/>
-        <v>6.024096385542169E-3</v>
+        <f>IFERROR(B107/C107," ")</f>
+        <v>6.6666666666666671E-3</v>
       </c>
       <c r="E107" t="s">
         <v>72</v>
@@ -2699,17 +2734,17 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B108" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C108" s="3">
-        <v>344</v>
+        <v>464</v>
       </c>
       <c r="D108" s="7">
-        <f t="shared" si="3"/>
-        <v>5.8139534883720929E-3</v>
+        <f>IFERROR(B108/C108," ")</f>
+        <v>6.4655172413793103E-3</v>
       </c>
       <c r="E108" t="s">
         <v>72</v>
@@ -2717,17 +2752,17 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B109" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C109" s="3">
-        <v>704</v>
+        <v>480</v>
       </c>
       <c r="D109" s="7">
-        <f t="shared" si="3"/>
-        <v>5.681818181818182E-3</v>
+        <f>IFERROR(B109/C109," ")</f>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E109" t="s">
         <v>72</v>
@@ -2735,17 +2770,17 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="B110" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C110" s="3">
-        <v>366</v>
+        <v>480</v>
       </c>
       <c r="D110" s="7">
-        <f t="shared" si="3"/>
-        <v>5.4644808743169399E-3</v>
+        <f>IFERROR(B110/C110," ")</f>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E110" t="s">
         <v>72</v>
@@ -2753,17 +2788,17 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="B111" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C111" s="3">
-        <v>736</v>
+        <v>488</v>
       </c>
       <c r="D111" s="7">
-        <f t="shared" si="3"/>
-        <v>5.434782608695652E-3</v>
+        <f>IFERROR(B111/C111," ")</f>
+        <v>6.1475409836065573E-3</v>
       </c>
       <c r="E111" t="s">
         <v>72</v>
@@ -2771,17 +2806,17 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="B112" s="3">
         <v>2</v>
       </c>
       <c r="C112" s="3">
-        <v>373</v>
+        <v>332</v>
       </c>
       <c r="D112" s="7">
-        <f t="shared" si="3"/>
-        <v>5.3619302949061663E-3</v>
+        <f>IFERROR(B112/C112," ")</f>
+        <v>6.024096385542169E-3</v>
       </c>
       <c r="E112" t="s">
         <v>72</v>
@@ -2789,17 +2824,17 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="B113" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C113" s="3">
-        <v>560</v>
+        <v>332</v>
       </c>
       <c r="D113" s="7">
-        <f t="shared" si="3"/>
-        <v>5.3571428571428572E-3</v>
+        <f>IFERROR(B113/C113," ")</f>
+        <v>6.024096385542169E-3</v>
       </c>
       <c r="E113" t="s">
         <v>72</v>
@@ -2807,17 +2842,17 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="B114" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C114" s="3">
-        <v>560</v>
+        <v>344</v>
       </c>
       <c r="D114" s="7">
-        <f t="shared" si="3"/>
-        <v>5.3571428571428572E-3</v>
+        <f>IFERROR(B114/C114," ")</f>
+        <v>5.8139534883720929E-3</v>
       </c>
       <c r="E114" t="s">
         <v>72</v>
@@ -2825,17 +2860,17 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B115" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C115" s="3">
-        <v>576</v>
+        <v>704</v>
       </c>
       <c r="D115" s="7">
-        <f t="shared" si="3"/>
-        <v>5.208333333333333E-3</v>
+        <f>IFERROR(B115/C115," ")</f>
+        <v>5.681818181818182E-3</v>
       </c>
       <c r="E115" t="s">
         <v>72</v>
@@ -2843,17 +2878,17 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="B116" s="3">
         <v>2</v>
       </c>
       <c r="C116" s="3">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="D116" s="7">
-        <f t="shared" si="3"/>
-        <v>5.208333333333333E-3</v>
+        <f>IFERROR(B116/C116," ")</f>
+        <v>5.4644808743169399E-3</v>
       </c>
       <c r="E116" t="s">
         <v>72</v>
@@ -2861,17 +2896,17 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B117" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C117" s="3">
-        <v>200</v>
+        <v>736</v>
       </c>
       <c r="D117" s="7">
-        <f t="shared" si="3"/>
-        <v>5.0000000000000001E-3</v>
+        <f>IFERROR(B117/C117," ")</f>
+        <v>5.434782608695652E-3</v>
       </c>
       <c r="E117" t="s">
         <v>72</v>
@@ -2879,17 +2914,17 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B118" s="3">
         <v>2</v>
       </c>
       <c r="C118" s="3">
-        <v>400</v>
+        <v>373</v>
       </c>
       <c r="D118" s="7">
-        <f t="shared" si="3"/>
-        <v>5.0000000000000001E-3</v>
+        <f>IFERROR(B118/C118," ")</f>
+        <v>5.3619302949061663E-3</v>
       </c>
       <c r="E118" t="s">
         <v>72</v>
@@ -2897,17 +2932,17 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B119" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C119" s="3">
-        <v>416</v>
+        <v>560</v>
       </c>
       <c r="D119" s="7">
-        <f t="shared" si="3"/>
-        <v>4.807692307692308E-3</v>
+        <f>IFERROR(B119/C119," ")</f>
+        <v>5.3571428571428572E-3</v>
       </c>
       <c r="E119" t="s">
         <v>72</v>
@@ -2915,17 +2950,17 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B120" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C120" s="3">
-        <v>416</v>
+        <v>560</v>
       </c>
       <c r="D120" s="7">
-        <f t="shared" si="3"/>
-        <v>4.807692307692308E-3</v>
+        <f>IFERROR(B120/C120," ")</f>
+        <v>5.3571428571428572E-3</v>
       </c>
       <c r="E120" t="s">
         <v>72</v>
@@ -2933,17 +2968,17 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="B121" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C121" s="3">
-        <v>848</v>
+        <v>576</v>
       </c>
       <c r="D121" s="7">
-        <f t="shared" si="3"/>
-        <v>4.7169811320754715E-3</v>
+        <f>IFERROR(B121/C121," ")</f>
+        <v>5.208333333333333E-3</v>
       </c>
       <c r="E121" t="s">
         <v>72</v>
@@ -2951,17 +2986,17 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="B122" s="3">
         <v>2</v>
       </c>
       <c r="C122" s="3">
-        <v>440</v>
+        <v>384</v>
       </c>
       <c r="D122" s="7">
-        <f t="shared" si="3"/>
-        <v>4.5454545454545452E-3</v>
+        <f>IFERROR(B122/C122," ")</f>
+        <v>5.208333333333333E-3</v>
       </c>
       <c r="E122" t="s">
         <v>72</v>
@@ -2969,17 +3004,17 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B123" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C123" s="3">
-        <v>456</v>
+        <v>200</v>
       </c>
       <c r="D123" s="7">
-        <f t="shared" si="3"/>
-        <v>4.3859649122807015E-3</v>
+        <f>IFERROR(B123/C123," ")</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E123" t="s">
         <v>72</v>
@@ -2987,17 +3022,17 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B124" s="3">
         <v>2</v>
       </c>
       <c r="C124" s="3">
-        <v>528</v>
+        <v>400</v>
       </c>
       <c r="D124" s="7">
-        <f t="shared" si="3"/>
-        <v>3.787878787878788E-3</v>
+        <f>IFERROR(B124/C124," ")</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E124" t="s">
         <v>72</v>
@@ -3005,17 +3040,17 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="B125" s="3">
         <v>2</v>
       </c>
       <c r="C125" s="3">
-        <v>544</v>
+        <v>416</v>
       </c>
       <c r="D125" s="7">
-        <f t="shared" si="3"/>
-        <v>3.6764705882352941E-3</v>
+        <f>IFERROR(B125/C125," ")</f>
+        <v>4.807692307692308E-3</v>
       </c>
       <c r="E125" t="s">
         <v>72</v>
@@ -3023,17 +3058,17 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B126" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C126" s="3">
-        <v>848</v>
+        <v>416</v>
       </c>
       <c r="D126" s="7">
-        <f t="shared" si="3"/>
-        <v>3.5377358490566039E-3</v>
+        <f>IFERROR(B126/C126," ")</f>
+        <v>4.807692307692308E-3</v>
       </c>
       <c r="E126" t="s">
         <v>72</v>
@@ -3041,17 +3076,17 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B127" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C127" s="3">
-        <v>864</v>
+        <v>848</v>
       </c>
       <c r="D127" s="7">
-        <f t="shared" si="3"/>
-        <v>3.472222222222222E-3</v>
+        <f>IFERROR(B127/C127," ")</f>
+        <v>4.7169811320754715E-3</v>
       </c>
       <c r="E127" t="s">
         <v>72</v>
@@ -3059,17 +3094,17 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B128" s="3">
         <v>2</v>
       </c>
       <c r="C128" s="3">
-        <v>616</v>
+        <v>440</v>
       </c>
       <c r="D128" s="7">
-        <f t="shared" si="3"/>
-        <v>3.246753246753247E-3</v>
+        <f>IFERROR(B128/C128," ")</f>
+        <v>4.5454545454545452E-3</v>
       </c>
       <c r="E128" t="s">
         <v>72</v>
@@ -3077,17 +3112,17 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B129" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C129" s="3">
-        <v>320</v>
+        <v>456</v>
       </c>
       <c r="D129" s="7">
-        <f t="shared" si="3"/>
-        <v>3.1250000000000002E-3</v>
+        <f>IFERROR(B129/C129," ")</f>
+        <v>4.3859649122807015E-3</v>
       </c>
       <c r="E129" t="s">
         <v>72</v>
@@ -3629,19 +3664,127 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B219" s="3">
+        <v>2</v>
+      </c>
+      <c r="C219" s="3">
+        <v>528</v>
+      </c>
+      <c r="D219" s="7">
+        <f>IFERROR(B219/C219," ")</f>
+        <v>3.787878787878788E-3</v>
+      </c>
+      <c r="E219" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B220" s="3">
+        <v>2</v>
+      </c>
+      <c r="C220" s="3">
+        <v>544</v>
+      </c>
+      <c r="D220" s="7">
+        <f>IFERROR(B220/C220," ")</f>
+        <v>3.6764705882352941E-3</v>
+      </c>
+      <c r="E220" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B221" s="3">
+        <v>3</v>
+      </c>
+      <c r="C221" s="3">
+        <v>848</v>
+      </c>
+      <c r="D221" s="7">
+        <f>IFERROR(B221/C221," ")</f>
+        <v>3.5377358490566039E-3</v>
+      </c>
+      <c r="E221" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B222" s="3">
+        <v>3</v>
+      </c>
+      <c r="C222" s="3">
+        <v>864</v>
+      </c>
+      <c r="D222" s="7">
+        <f>IFERROR(B222/C222," ")</f>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="E222" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B223" s="3">
+        <v>2</v>
+      </c>
+      <c r="C223" s="3">
+        <v>616</v>
+      </c>
+      <c r="D223" s="7">
+        <f>IFERROR(B223/C223," ")</f>
+        <v>3.246753246753247E-3</v>
+      </c>
+      <c r="E223" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B224" s="3">
+        <v>1</v>
+      </c>
+      <c r="C224" s="3">
+        <v>320</v>
+      </c>
+      <c r="D224" s="7">
+        <f>IFERROR(B224/C224," ")</f>
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="E224" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B219" s="3">
-        <v>3</v>
-      </c>
-      <c r="C219" s="3">
+      <c r="B225" s="3">
+        <v>3</v>
+      </c>
+      <c r="C225" s="3">
         <v>1280</v>
       </c>
-      <c r="D219" s="7">
-        <f t="shared" ref="D219" si="4">IFERROR(B219/C219," ")</f>
+      <c r="D225" s="7">
+        <f>IFERROR(B225/C225," ")</f>
         <v>2.3437499999999999E-3</v>
       </c>
-      <c r="E219" t="s">
+      <c r="E225" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3657,7 +3800,7 @@
         <filter val="No"/>
       </filters>
     </filterColumn>
-    <sortState ref="A14:E219">
+    <sortState ref="A14:E225">
       <sortCondition descending="1" ref="D2:D218"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Marked Zoar as read
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -459,7 +459,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,25 +475,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -505,11 +493,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -523,12 +510,8 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1131,7 +1114,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" t="s">
         <v>88</v>
       </c>
       <c r="B19" s="3">
@@ -1145,7 +1128,7 @@
         <v>6.8493150684931503E-2</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,7 +1160,7 @@
         <v>55</v>
       </c>
       <c r="D21" s="7">
-        <f>IFERROR(B21/C21," ")</f>
+        <f t="shared" ref="D21:D84" si="2">IFERROR(B21/C21," ")</f>
         <v>5.4545454545454543E-2</v>
       </c>
       <c r="E21" t="s">
@@ -1195,7 +1178,7 @@
         <v>74</v>
       </c>
       <c r="D22" s="7">
-        <f>IFERROR(B22/C22," ")</f>
+        <f t="shared" si="2"/>
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="E22" t="s">
@@ -1213,7 +1196,7 @@
         <v>120</v>
       </c>
       <c r="D23" s="7">
-        <f>IFERROR(B23/C23," ")</f>
+        <f t="shared" si="2"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E23" t="s">
@@ -1231,7 +1214,7 @@
         <v>72</v>
       </c>
       <c r="D24" s="7">
-        <f>IFERROR(B24/C24," ")</f>
+        <f t="shared" si="2"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E24" t="s">
@@ -1249,7 +1232,7 @@
         <v>128</v>
       </c>
       <c r="D25" s="7">
-        <f>IFERROR(B25/C25," ")</f>
+        <f t="shared" si="2"/>
         <v>3.90625E-2</v>
       </c>
       <c r="E25" t="s">
@@ -1267,7 +1250,7 @@
         <v>133</v>
       </c>
       <c r="D26" s="7">
-        <f>IFERROR(B26/C26," ")</f>
+        <f t="shared" si="2"/>
         <v>3.7593984962406013E-2</v>
       </c>
       <c r="E26" t="s">
@@ -1285,7 +1268,7 @@
         <v>132</v>
       </c>
       <c r="D27" s="7">
-        <f>IFERROR(B27/C27," ")</f>
+        <f t="shared" si="2"/>
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="E27" t="s">
@@ -1303,7 +1286,7 @@
         <v>160</v>
       </c>
       <c r="D28" s="7">
-        <f>IFERROR(B28/C28," ")</f>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E28" t="s">
@@ -1321,7 +1304,7 @@
         <v>80</v>
       </c>
       <c r="D29" s="7">
-        <f>IFERROR(B29/C29," ")</f>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E29" t="s">
@@ -1339,7 +1322,7 @@
         <v>124</v>
       </c>
       <c r="D30" s="7">
-        <f>IFERROR(B30/C30," ")</f>
+        <f t="shared" si="2"/>
         <v>2.4193548387096774E-2</v>
       </c>
       <c r="E30" t="s">
@@ -1357,7 +1340,7 @@
         <v>208</v>
       </c>
       <c r="D31" s="7">
-        <f>IFERROR(B31/C31," ")</f>
+        <f t="shared" si="2"/>
         <v>2.403846153846154E-2</v>
       </c>
       <c r="E31" t="s">
@@ -1375,7 +1358,7 @@
         <v>128</v>
       </c>
       <c r="D32" s="7">
-        <f>IFERROR(B32/C32," ")</f>
+        <f t="shared" si="2"/>
         <v>2.34375E-2</v>
       </c>
       <c r="E32" t="s">
@@ -1393,7 +1376,7 @@
         <v>224</v>
       </c>
       <c r="D33" s="7">
-        <f>IFERROR(B33/C33," ")</f>
+        <f t="shared" si="2"/>
         <v>2.2321428571428572E-2</v>
       </c>
       <c r="E33" t="s">
@@ -1411,7 +1394,7 @@
         <v>228</v>
       </c>
       <c r="D34" s="7">
-        <f>IFERROR(B34/C34," ")</f>
+        <f t="shared" si="2"/>
         <v>2.1929824561403508E-2</v>
       </c>
       <c r="E34" t="s">
@@ -1429,7 +1412,7 @@
         <v>191</v>
       </c>
       <c r="D35" s="7">
-        <f>IFERROR(B35/C35," ")</f>
+        <f t="shared" si="2"/>
         <v>2.0942408376963352E-2</v>
       </c>
       <c r="E35" t="s">
@@ -1447,7 +1430,7 @@
         <v>192</v>
       </c>
       <c r="D36" s="7">
-        <f>IFERROR(B36/C36," ")</f>
+        <f t="shared" si="2"/>
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E36" t="s">
@@ -1465,7 +1448,7 @@
         <v>198</v>
       </c>
       <c r="D37" s="7">
-        <f>IFERROR(B37/C37," ")</f>
+        <f t="shared" si="2"/>
         <v>2.0202020202020204E-2</v>
       </c>
       <c r="E37" t="s">
@@ -1483,7 +1466,7 @@
         <v>258</v>
       </c>
       <c r="D38" s="7">
-        <f>IFERROR(B38/C38," ")</f>
+        <f t="shared" si="2"/>
         <v>1.937984496124031E-2</v>
       </c>
       <c r="E38" t="s">
@@ -1501,7 +1484,7 @@
         <v>157</v>
       </c>
       <c r="D39" s="7">
-        <f>IFERROR(B39/C39," ")</f>
+        <f t="shared" si="2"/>
         <v>1.9108280254777069E-2</v>
       </c>
       <c r="E39" t="s">
@@ -1519,7 +1502,7 @@
         <v>160</v>
       </c>
       <c r="D40" s="7">
-        <f>IFERROR(B40/C40," ")</f>
+        <f t="shared" si="2"/>
         <v>1.8749999999999999E-2</v>
       </c>
       <c r="E40" t="s">
@@ -1537,7 +1520,7 @@
         <v>224</v>
       </c>
       <c r="D41" s="7">
-        <f>IFERROR(B41/C41," ")</f>
+        <f t="shared" si="2"/>
         <v>1.7857142857142856E-2</v>
       </c>
       <c r="E41" t="s">
@@ -1555,7 +1538,7 @@
         <v>226</v>
       </c>
       <c r="D42" s="7">
-        <f>IFERROR(B42/C42," ")</f>
+        <f t="shared" si="2"/>
         <v>1.7699115044247787E-2</v>
       </c>
       <c r="E42" t="s">
@@ -1573,7 +1556,7 @@
         <v>288</v>
       </c>
       <c r="D43" s="7">
-        <f>IFERROR(B43/C43," ")</f>
+        <f t="shared" si="2"/>
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="E43" t="s">
@@ -1591,7 +1574,7 @@
         <v>231</v>
       </c>
       <c r="D44" s="7">
-        <f>IFERROR(B44/C44," ")</f>
+        <f t="shared" si="2"/>
         <v>1.7316017316017316E-2</v>
       </c>
       <c r="E44" t="s">
@@ -1609,7 +1592,7 @@
         <v>181</v>
       </c>
       <c r="D45" s="7">
-        <f>IFERROR(B45/C45," ")</f>
+        <f t="shared" si="2"/>
         <v>1.6574585635359115E-2</v>
       </c>
       <c r="E45" t="s">
@@ -1627,7 +1610,7 @@
         <v>182</v>
       </c>
       <c r="D46" s="7">
-        <f>IFERROR(B46/C46," ")</f>
+        <f t="shared" si="2"/>
         <v>1.6483516483516484E-2</v>
       </c>
       <c r="E46" t="s">
@@ -1645,7 +1628,7 @@
         <v>250</v>
       </c>
       <c r="D47" s="7">
-        <f>IFERROR(B47/C47," ")</f>
+        <f t="shared" si="2"/>
         <v>1.6E-2</v>
       </c>
       <c r="E47" t="s">
@@ -1663,7 +1646,7 @@
         <v>266</v>
       </c>
       <c r="D48" s="7">
-        <f>IFERROR(B48/C48," ")</f>
+        <f t="shared" si="2"/>
         <v>1.5037593984962405E-2</v>
       </c>
       <c r="E48" t="s">
@@ -1681,7 +1664,7 @@
         <v>336</v>
       </c>
       <c r="D49" s="7">
-        <f>IFERROR(B49/C49," ")</f>
+        <f t="shared" si="2"/>
         <v>1.488095238095238E-2</v>
       </c>
       <c r="E49" t="s">
@@ -1699,7 +1682,7 @@
         <v>137</v>
       </c>
       <c r="D50" s="7">
-        <f>IFERROR(B50/C50," ")</f>
+        <f t="shared" si="2"/>
         <v>1.4598540145985401E-2</v>
       </c>
       <c r="E50" t="s">
@@ -1717,7 +1700,7 @@
         <v>276</v>
       </c>
       <c r="D51" s="7">
-        <f>IFERROR(B51/C51," ")</f>
+        <f t="shared" si="2"/>
         <v>1.4492753623188406E-2</v>
       </c>
       <c r="E51" t="s">
@@ -1735,7 +1718,7 @@
         <v>208</v>
       </c>
       <c r="D52" s="7">
-        <f>IFERROR(B52/C52," ")</f>
+        <f t="shared" si="2"/>
         <v>1.4423076923076924E-2</v>
       </c>
       <c r="E52" t="s">
@@ -1753,7 +1736,7 @@
         <v>213</v>
       </c>
       <c r="D53" s="7">
-        <f>IFERROR(B53/C53," ")</f>
+        <f t="shared" si="2"/>
         <v>1.4084507042253521E-2</v>
       </c>
       <c r="E53" t="s">
@@ -1771,7 +1754,7 @@
         <v>220</v>
       </c>
       <c r="D54" s="7">
-        <f>IFERROR(B54/C54," ")</f>
+        <f t="shared" si="2"/>
         <v>1.3636363636363636E-2</v>
       </c>
       <c r="E54" t="s">
@@ -1789,7 +1772,7 @@
         <v>368</v>
       </c>
       <c r="D55" s="7">
-        <f>IFERROR(B55/C55," ")</f>
+        <f t="shared" si="2"/>
         <v>1.358695652173913E-2</v>
       </c>
       <c r="E55" t="s">
@@ -1807,7 +1790,7 @@
         <v>320</v>
       </c>
       <c r="D56" s="7">
-        <f>IFERROR(B56/C56," ")</f>
+        <f t="shared" si="2"/>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="E56" t="s">
@@ -1825,7 +1808,7 @@
         <v>160</v>
       </c>
       <c r="D57" s="7">
-        <f>IFERROR(B57/C57," ")</f>
+        <f t="shared" si="2"/>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="E57" t="s">
@@ -1843,7 +1826,7 @@
         <v>336</v>
       </c>
       <c r="D58" s="7">
-        <f>IFERROR(B58/C58," ")</f>
+        <f t="shared" si="2"/>
         <v>1.1904761904761904E-2</v>
       </c>
       <c r="E58" t="s">
@@ -1861,7 +1844,7 @@
         <v>256</v>
       </c>
       <c r="D59" s="7">
-        <f>IFERROR(B59/C59," ")</f>
+        <f t="shared" si="2"/>
         <v>1.171875E-2</v>
       </c>
       <c r="E59" t="s">
@@ -1879,7 +1862,7 @@
         <v>256</v>
       </c>
       <c r="D60" s="7">
-        <f>IFERROR(B60/C60," ")</f>
+        <f t="shared" si="2"/>
         <v>1.171875E-2</v>
       </c>
       <c r="E60" t="s">
@@ -1897,7 +1880,7 @@
         <v>432</v>
       </c>
       <c r="D61" s="7">
-        <f>IFERROR(B61/C61," ")</f>
+        <f t="shared" si="2"/>
         <v>1.1574074074074073E-2</v>
       </c>
       <c r="E61" t="s">
@@ -1915,7 +1898,7 @@
         <v>264</v>
       </c>
       <c r="D62" s="7">
-        <f>IFERROR(B62/C62," ")</f>
+        <f t="shared" si="2"/>
         <v>1.1363636363636364E-2</v>
       </c>
       <c r="E62" t="s">
@@ -1933,7 +1916,7 @@
         <v>352</v>
       </c>
       <c r="D63" s="7">
-        <f>IFERROR(B63/C63," ")</f>
+        <f t="shared" si="2"/>
         <v>1.1363636363636364E-2</v>
       </c>
       <c r="E63" t="s">
@@ -1951,7 +1934,7 @@
         <v>266</v>
       </c>
       <c r="D64" s="7">
-        <f>IFERROR(B64/C64," ")</f>
+        <f t="shared" si="2"/>
         <v>1.1278195488721804E-2</v>
       </c>
       <c r="E64" t="s">
@@ -1969,7 +1952,7 @@
         <v>277</v>
       </c>
       <c r="D65" s="7">
-        <f>IFERROR(B65/C65," ")</f>
+        <f t="shared" si="2"/>
         <v>1.0830324909747292E-2</v>
       </c>
       <c r="E65" t="s">
@@ -1987,7 +1970,7 @@
         <v>384</v>
       </c>
       <c r="D66" s="7">
-        <f>IFERROR(B66/C66," ")</f>
+        <f t="shared" si="2"/>
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E66" t="s">
@@ -2005,7 +1988,7 @@
         <v>384</v>
       </c>
       <c r="D67" s="7">
-        <f>IFERROR(B67/C67," ")</f>
+        <f t="shared" si="2"/>
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E67" t="s">
@@ -2023,7 +2006,7 @@
         <v>288</v>
       </c>
       <c r="D68" s="7">
-        <f>IFERROR(B68/C68," ")</f>
+        <f t="shared" si="2"/>
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E68" t="s">
@@ -2041,7 +2024,7 @@
         <v>288</v>
       </c>
       <c r="D69" s="7">
-        <f>IFERROR(B69/C69," ")</f>
+        <f t="shared" si="2"/>
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E69" t="s">
@@ -2059,7 +2042,7 @@
         <v>400</v>
       </c>
       <c r="D70" s="7">
-        <f>IFERROR(B70/C70," ")</f>
+        <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
       <c r="E70" t="s">
@@ -2077,7 +2060,7 @@
         <v>200</v>
       </c>
       <c r="D71" s="7">
-        <f>IFERROR(B71/C71," ")</f>
+        <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
       <c r="E71" t="s">
@@ -2095,7 +2078,7 @@
         <v>400</v>
       </c>
       <c r="D72" s="7">
-        <f>IFERROR(B72/C72," ")</f>
+        <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
       <c r="E72" t="s">
@@ -2113,7 +2096,7 @@
         <v>416</v>
       </c>
       <c r="D73" s="7">
-        <f>IFERROR(B73/C73," ")</f>
+        <f t="shared" si="2"/>
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E73" t="s">
@@ -2131,7 +2114,7 @@
         <v>208</v>
       </c>
       <c r="D74" s="7">
-        <f>IFERROR(B74/C74," ")</f>
+        <f t="shared" si="2"/>
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E74" t="s">
@@ -2149,7 +2132,7 @@
         <v>208</v>
       </c>
       <c r="D75" s="7">
-        <f>IFERROR(B75/C75," ")</f>
+        <f t="shared" si="2"/>
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E75" t="s">
@@ -2167,7 +2150,7 @@
         <v>312</v>
       </c>
       <c r="D76" s="7">
-        <f>IFERROR(B76/C76," ")</f>
+        <f t="shared" si="2"/>
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="E76" t="s">
@@ -2185,7 +2168,7 @@
         <v>316</v>
       </c>
       <c r="D77" s="7">
-        <f>IFERROR(B77/C77," ")</f>
+        <f t="shared" si="2"/>
         <v>9.4936708860759497E-3</v>
       </c>
       <c r="E77" t="s">
@@ -2203,7 +2186,7 @@
         <v>432</v>
       </c>
       <c r="D78" s="7">
-        <f>IFERROR(B78/C78," ")</f>
+        <f t="shared" si="2"/>
         <v>9.2592592592592587E-3</v>
       </c>
       <c r="E78" t="s">
@@ -2221,7 +2204,7 @@
         <v>436</v>
       </c>
       <c r="D79" s="7">
-        <f>IFERROR(B79/C79," ")</f>
+        <f t="shared" si="2"/>
         <v>9.1743119266055051E-3</v>
       </c>
       <c r="E79" t="s">
@@ -2239,7 +2222,7 @@
         <v>444</v>
       </c>
       <c r="D80" s="7">
-        <f>IFERROR(B80/C80," ")</f>
+        <f t="shared" si="2"/>
         <v>9.0090090090090089E-3</v>
       </c>
       <c r="E80" t="s">
@@ -2257,7 +2240,7 @@
         <v>336</v>
       </c>
       <c r="D81" s="7">
-        <f>IFERROR(B81/C81," ")</f>
+        <f t="shared" si="2"/>
         <v>8.9285714285714281E-3</v>
       </c>
       <c r="E81" t="s">
@@ -2275,7 +2258,7 @@
         <v>225</v>
       </c>
       <c r="D82" s="7">
-        <f>IFERROR(B82/C82," ")</f>
+        <f t="shared" si="2"/>
         <v>8.8888888888888889E-3</v>
       </c>
       <c r="E82" t="s">
@@ -2293,7 +2276,7 @@
         <v>344</v>
       </c>
       <c r="D83" s="7">
-        <f>IFERROR(B83/C83," ")</f>
+        <f t="shared" si="2"/>
         <v>8.7209302325581394E-3</v>
       </c>
       <c r="E83" t="s">
@@ -2311,7 +2294,7 @@
         <v>464</v>
       </c>
       <c r="D84" s="7">
-        <f>IFERROR(B84/C84," ")</f>
+        <f t="shared" si="2"/>
         <v>8.6206896551724137E-3</v>
       </c>
       <c r="E84" t="s">
@@ -2329,7 +2312,7 @@
         <v>464</v>
       </c>
       <c r="D85" s="7">
-        <f>IFERROR(B85/C85," ")</f>
+        <f t="shared" ref="D85:D148" si="3">IFERROR(B85/C85," ")</f>
         <v>8.6206896551724137E-3</v>
       </c>
       <c r="E85" t="s">
@@ -2347,7 +2330,7 @@
         <v>352</v>
       </c>
       <c r="D86" s="7">
-        <f>IFERROR(B86/C86," ")</f>
+        <f t="shared" si="3"/>
         <v>8.5227272727272721E-3</v>
       </c>
       <c r="E86" t="s">
@@ -2365,7 +2348,7 @@
         <v>352</v>
       </c>
       <c r="D87" s="7">
-        <f>IFERROR(B87/C87," ")</f>
+        <f t="shared" si="3"/>
         <v>8.5227272727272721E-3</v>
       </c>
       <c r="E87" t="s">
@@ -2383,7 +2366,7 @@
         <v>480</v>
       </c>
       <c r="D88" s="7">
-        <f>IFERROR(B88/C88," ")</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="E88" t="s">
@@ -2401,7 +2384,7 @@
         <v>360</v>
       </c>
       <c r="D89" s="7">
-        <f>IFERROR(B89/C89," ")</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="E89" t="s">
@@ -2419,7 +2402,7 @@
         <v>240</v>
       </c>
       <c r="D90" s="7">
-        <f>IFERROR(B90/C90," ")</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="E90" t="s">
@@ -2437,7 +2420,7 @@
         <v>368</v>
       </c>
       <c r="D91" s="7">
-        <f>IFERROR(B91/C91," ")</f>
+        <f t="shared" si="3"/>
         <v>8.152173913043478E-3</v>
       </c>
       <c r="E91" t="s">
@@ -2455,7 +2438,7 @@
         <v>368</v>
       </c>
       <c r="D92" s="7">
-        <f>IFERROR(B92/C92," ")</f>
+        <f t="shared" si="3"/>
         <v>8.152173913043478E-3</v>
       </c>
       <c r="E92" t="s">
@@ -2473,7 +2456,7 @@
         <v>371</v>
       </c>
       <c r="D93" s="7">
-        <f>IFERROR(B93/C93," ")</f>
+        <f t="shared" si="3"/>
         <v>8.0862533692722376E-3</v>
       </c>
       <c r="E93" t="s">
@@ -2491,7 +2474,7 @@
         <v>499</v>
       </c>
       <c r="D94" s="7">
-        <f>IFERROR(B94/C94," ")</f>
+        <f t="shared" si="3"/>
         <v>8.0160320641282558E-3</v>
       </c>
       <c r="E94" t="s">
@@ -2509,7 +2492,7 @@
         <v>250</v>
       </c>
       <c r="D95" s="7">
-        <f>IFERROR(B95/C95," ")</f>
+        <f t="shared" si="3"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="E95" t="s">
@@ -2527,7 +2510,7 @@
         <v>512</v>
       </c>
       <c r="D96" s="7">
-        <f>IFERROR(B96/C96," ")</f>
+        <f t="shared" si="3"/>
         <v>7.8125E-3</v>
       </c>
       <c r="E96" t="s">
@@ -2545,7 +2528,7 @@
         <v>512</v>
       </c>
       <c r="D97" s="7">
-        <f>IFERROR(B97/C97," ")</f>
+        <f t="shared" si="3"/>
         <v>7.8125E-3</v>
       </c>
       <c r="E97" t="s">
@@ -2563,7 +2546,7 @@
         <v>264</v>
       </c>
       <c r="D98" s="7">
-        <f>IFERROR(B98/C98," ")</f>
+        <f t="shared" si="3"/>
         <v>7.575757575757576E-3</v>
       </c>
       <c r="E98" t="s">
@@ -2581,7 +2564,7 @@
         <v>400</v>
       </c>
       <c r="D99" s="7">
-        <f>IFERROR(B99/C99," ")</f>
+        <f t="shared" si="3"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="E99" t="s">
@@ -2599,7 +2582,7 @@
         <v>544</v>
       </c>
       <c r="D100" s="7">
-        <f>IFERROR(B100/C100," ")</f>
+        <f t="shared" si="3"/>
         <v>7.3529411764705881E-3</v>
       </c>
       <c r="E100" t="s">
@@ -2617,7 +2600,7 @@
         <v>416</v>
       </c>
       <c r="D101" s="7">
-        <f>IFERROR(B101/C101," ")</f>
+        <f t="shared" si="3"/>
         <v>7.2115384615384619E-3</v>
       </c>
       <c r="E101" t="s">
@@ -2635,7 +2618,7 @@
         <v>560</v>
       </c>
       <c r="D102" s="7">
-        <f>IFERROR(B102/C102," ")</f>
+        <f t="shared" si="3"/>
         <v>7.1428571428571426E-3</v>
       </c>
       <c r="E102" t="s">
@@ -2653,7 +2636,7 @@
         <v>284</v>
       </c>
       <c r="D103" s="7">
-        <f>IFERROR(B103/C103," ")</f>
+        <f t="shared" si="3"/>
         <v>7.0422535211267607E-3</v>
       </c>
       <c r="E103" t="s">
@@ -2671,7 +2654,7 @@
         <v>288</v>
       </c>
       <c r="D104" s="7">
-        <f>IFERROR(B104/C104," ")</f>
+        <f t="shared" si="3"/>
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E104" t="s">
@@ -2689,7 +2672,7 @@
         <v>736</v>
       </c>
       <c r="D105" s="7">
-        <f>IFERROR(B105/C105," ")</f>
+        <f t="shared" si="3"/>
         <v>6.793478260869565E-3</v>
       </c>
       <c r="E105" t="s">
@@ -2707,7 +2690,7 @@
         <v>148</v>
       </c>
       <c r="D106" s="7">
-        <f>IFERROR(B106/C106," ")</f>
+        <f t="shared" si="3"/>
         <v>6.7567567567567571E-3</v>
       </c>
       <c r="E106" t="s">
@@ -2725,7 +2708,7 @@
         <v>450</v>
       </c>
       <c r="D107" s="7">
-        <f>IFERROR(B107/C107," ")</f>
+        <f t="shared" si="3"/>
         <v>6.6666666666666671E-3</v>
       </c>
       <c r="E107" t="s">
@@ -2743,7 +2726,7 @@
         <v>464</v>
       </c>
       <c r="D108" s="7">
-        <f>IFERROR(B108/C108," ")</f>
+        <f t="shared" si="3"/>
         <v>6.4655172413793103E-3</v>
       </c>
       <c r="E108" t="s">
@@ -2761,7 +2744,7 @@
         <v>480</v>
       </c>
       <c r="D109" s="7">
-        <f>IFERROR(B109/C109," ")</f>
+        <f t="shared" si="3"/>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="E109" t="s">
@@ -2779,7 +2762,7 @@
         <v>480</v>
       </c>
       <c r="D110" s="7">
-        <f>IFERROR(B110/C110," ")</f>
+        <f t="shared" si="3"/>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="E110" t="s">
@@ -2797,7 +2780,7 @@
         <v>488</v>
       </c>
       <c r="D111" s="7">
-        <f>IFERROR(B111/C111," ")</f>
+        <f t="shared" si="3"/>
         <v>6.1475409836065573E-3</v>
       </c>
       <c r="E111" t="s">
@@ -2815,7 +2798,7 @@
         <v>332</v>
       </c>
       <c r="D112" s="7">
-        <f>IFERROR(B112/C112," ")</f>
+        <f t="shared" si="3"/>
         <v>6.024096385542169E-3</v>
       </c>
       <c r="E112" t="s">
@@ -2833,7 +2816,7 @@
         <v>332</v>
       </c>
       <c r="D113" s="7">
-        <f>IFERROR(B113/C113," ")</f>
+        <f t="shared" si="3"/>
         <v>6.024096385542169E-3</v>
       </c>
       <c r="E113" t="s">
@@ -2851,7 +2834,7 @@
         <v>344</v>
       </c>
       <c r="D114" s="7">
-        <f>IFERROR(B114/C114," ")</f>
+        <f t="shared" si="3"/>
         <v>5.8139534883720929E-3</v>
       </c>
       <c r="E114" t="s">
@@ -2869,7 +2852,7 @@
         <v>704</v>
       </c>
       <c r="D115" s="7">
-        <f>IFERROR(B115/C115," ")</f>
+        <f t="shared" si="3"/>
         <v>5.681818181818182E-3</v>
       </c>
       <c r="E115" t="s">
@@ -2887,7 +2870,7 @@
         <v>366</v>
       </c>
       <c r="D116" s="7">
-        <f>IFERROR(B116/C116," ")</f>
+        <f t="shared" si="3"/>
         <v>5.4644808743169399E-3</v>
       </c>
       <c r="E116" t="s">
@@ -2905,7 +2888,7 @@
         <v>736</v>
       </c>
       <c r="D117" s="7">
-        <f>IFERROR(B117/C117," ")</f>
+        <f t="shared" si="3"/>
         <v>5.434782608695652E-3</v>
       </c>
       <c r="E117" t="s">
@@ -2923,7 +2906,7 @@
         <v>373</v>
       </c>
       <c r="D118" s="7">
-        <f>IFERROR(B118/C118," ")</f>
+        <f t="shared" si="3"/>
         <v>5.3619302949061663E-3</v>
       </c>
       <c r="E118" t="s">
@@ -2941,7 +2924,7 @@
         <v>560</v>
       </c>
       <c r="D119" s="7">
-        <f>IFERROR(B119/C119," ")</f>
+        <f t="shared" si="3"/>
         <v>5.3571428571428572E-3</v>
       </c>
       <c r="E119" t="s">
@@ -2959,7 +2942,7 @@
         <v>560</v>
       </c>
       <c r="D120" s="7">
-        <f>IFERROR(B120/C120," ")</f>
+        <f t="shared" si="3"/>
         <v>5.3571428571428572E-3</v>
       </c>
       <c r="E120" t="s">
@@ -2977,7 +2960,7 @@
         <v>576</v>
       </c>
       <c r="D121" s="7">
-        <f>IFERROR(B121/C121," ")</f>
+        <f t="shared" si="3"/>
         <v>5.208333333333333E-3</v>
       </c>
       <c r="E121" t="s">
@@ -2995,7 +2978,7 @@
         <v>384</v>
       </c>
       <c r="D122" s="7">
-        <f>IFERROR(B122/C122," ")</f>
+        <f t="shared" si="3"/>
         <v>5.208333333333333E-3</v>
       </c>
       <c r="E122" t="s">
@@ -3013,7 +2996,7 @@
         <v>200</v>
       </c>
       <c r="D123" s="7">
-        <f>IFERROR(B123/C123," ")</f>
+        <f t="shared" si="3"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E123" t="s">
@@ -3031,7 +3014,7 @@
         <v>400</v>
       </c>
       <c r="D124" s="7">
-        <f>IFERROR(B124/C124," ")</f>
+        <f t="shared" si="3"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E124" t="s">
@@ -3049,7 +3032,7 @@
         <v>416</v>
       </c>
       <c r="D125" s="7">
-        <f>IFERROR(B125/C125," ")</f>
+        <f t="shared" si="3"/>
         <v>4.807692307692308E-3</v>
       </c>
       <c r="E125" t="s">
@@ -3067,7 +3050,7 @@
         <v>416</v>
       </c>
       <c r="D126" s="7">
-        <f>IFERROR(B126/C126," ")</f>
+        <f t="shared" si="3"/>
         <v>4.807692307692308E-3</v>
       </c>
       <c r="E126" t="s">
@@ -3085,7 +3068,7 @@
         <v>848</v>
       </c>
       <c r="D127" s="7">
-        <f>IFERROR(B127/C127," ")</f>
+        <f t="shared" si="3"/>
         <v>4.7169811320754715E-3</v>
       </c>
       <c r="E127" t="s">
@@ -3103,7 +3086,7 @@
         <v>440</v>
       </c>
       <c r="D128" s="7">
-        <f>IFERROR(B128/C128," ")</f>
+        <f t="shared" si="3"/>
         <v>4.5454545454545452E-3</v>
       </c>
       <c r="E128" t="s">
@@ -3121,7 +3104,7 @@
         <v>456</v>
       </c>
       <c r="D129" s="7">
-        <f>IFERROR(B129/C129," ")</f>
+        <f t="shared" si="3"/>
         <v>4.3859649122807015E-3</v>
       </c>
       <c r="E129" t="s">
@@ -3130,535 +3113,535 @@
     </row>
     <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D130" s="7" t="str">
-        <f>IFERROR(B130/C130," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D131" s="7" t="str">
-        <f>IFERROR(B131/C131," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D132" s="7" t="str">
-        <f>IFERROR(B132/C132," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D133" s="7" t="str">
-        <f>IFERROR(B133/C133," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D134" s="7" t="str">
-        <f>IFERROR(B134/C134," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D135" s="7" t="str">
-        <f>IFERROR(B135/C135," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D136" s="7" t="str">
-        <f>IFERROR(B136/C136," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D137" s="7" t="str">
-        <f>IFERROR(B137/C137," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D138" s="7" t="str">
-        <f>IFERROR(B138/C138," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D139" s="7" t="str">
-        <f>IFERROR(B139/C139," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D140" s="7" t="str">
-        <f>IFERROR(B140/C140," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D141" s="7" t="str">
-        <f>IFERROR(B141/C141," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D142" s="7" t="str">
-        <f>IFERROR(B142/C142," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D143" s="7" t="str">
-        <f>IFERROR(B143/C143," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D144" s="7" t="str">
-        <f>IFERROR(B144/C144," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="145" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D145" s="7" t="str">
-        <f>IFERROR(B145/C145," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="146" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D146" s="7" t="str">
-        <f>IFERROR(B146/C146," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="147" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D147" s="7" t="str">
-        <f>IFERROR(B147/C147," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="148" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D148" s="7" t="str">
-        <f>IFERROR(B148/C148," ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="149" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D149" s="7" t="str">
-        <f>IFERROR(B149/C149," ")</f>
+        <f t="shared" ref="D149:D212" si="4">IFERROR(B149/C149," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="150" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D150" s="7" t="str">
-        <f>IFERROR(B150/C150," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="151" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D151" s="7" t="str">
-        <f>IFERROR(B151/C151," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="152" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D152" s="7" t="str">
-        <f>IFERROR(B152/C152," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="153" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D153" s="7" t="str">
-        <f>IFERROR(B153/C153," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="154" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D154" s="7" t="str">
-        <f>IFERROR(B154/C154," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="155" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D155" s="7" t="str">
-        <f>IFERROR(B155/C155," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="156" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D156" s="7" t="str">
-        <f>IFERROR(B156/C156," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="157" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D157" s="7" t="str">
-        <f>IFERROR(B157/C157," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="158" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D158" s="7" t="str">
-        <f>IFERROR(B158/C158," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="159" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D159" s="7" t="str">
-        <f>IFERROR(B159/C159," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="160" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D160" s="7" t="str">
-        <f>IFERROR(B160/C160," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="161" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D161" s="7" t="str">
-        <f>IFERROR(B161/C161," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="162" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D162" s="7" t="str">
-        <f>IFERROR(B162/C162," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="163" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D163" s="7" t="str">
-        <f>IFERROR(B163/C163," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="164" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D164" s="7" t="str">
-        <f>IFERROR(B164/C164," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="165" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D165" s="7" t="str">
-        <f>IFERROR(B165/C165," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="166" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D166" s="7" t="str">
-        <f>IFERROR(B166/C166," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="167" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D167" s="7" t="str">
-        <f>IFERROR(B167/C167," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="168" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D168" s="7" t="str">
-        <f>IFERROR(B168/C168," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="169" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D169" s="7" t="str">
-        <f>IFERROR(B169/C169," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="170" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D170" s="7" t="str">
-        <f>IFERROR(B170/C170," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="171" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D171" s="7" t="str">
-        <f>IFERROR(B171/C171," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="172" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D172" s="7" t="str">
-        <f>IFERROR(B172/C172," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="173" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D173" s="7" t="str">
-        <f>IFERROR(B173/C173," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="174" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D174" s="7" t="str">
-        <f>IFERROR(B174/C174," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="175" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D175" s="7" t="str">
-        <f>IFERROR(B175/C175," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="176" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D176" s="7" t="str">
-        <f>IFERROR(B176/C176," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="177" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D177" s="7" t="str">
-        <f>IFERROR(B177/C177," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="178" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D178" s="7" t="str">
-        <f>IFERROR(B178/C178," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="179" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D179" s="7" t="str">
-        <f>IFERROR(B179/C179," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="180" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D180" s="7" t="str">
-        <f>IFERROR(B180/C180," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="181" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D181" s="7" t="str">
-        <f>IFERROR(B181/C181," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="182" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D182" s="7" t="str">
-        <f>IFERROR(B182/C182," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="183" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D183" s="7" t="str">
-        <f>IFERROR(B183/C183," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="184" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D184" s="7" t="str">
-        <f>IFERROR(B184/C184," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="185" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D185" s="7" t="str">
-        <f>IFERROR(B185/C185," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="186" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D186" s="7" t="str">
-        <f>IFERROR(B186/C186," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="187" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D187" s="7" t="str">
-        <f>IFERROR(B187/C187," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="188" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D188" s="7" t="str">
-        <f>IFERROR(B188/C188," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="189" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D189" s="7" t="str">
-        <f>IFERROR(B189/C189," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="190" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D190" s="7" t="str">
-        <f>IFERROR(B190/C190," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="191" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D191" s="7" t="str">
-        <f>IFERROR(B191/C191," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="192" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D192" s="7" t="str">
-        <f>IFERROR(B192/C192," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="193" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D193" s="7" t="str">
-        <f>IFERROR(B193/C193," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="194" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D194" s="7" t="str">
-        <f>IFERROR(B194/C194," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="195" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D195" s="7" t="str">
-        <f>IFERROR(B195/C195," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="196" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D196" s="7" t="str">
-        <f>IFERROR(B196/C196," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="197" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D197" s="7" t="str">
-        <f>IFERROR(B197/C197," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="198" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D198" s="7" t="str">
-        <f>IFERROR(B198/C198," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="199" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D199" s="7" t="str">
-        <f>IFERROR(B199/C199," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="200" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D200" s="7" t="str">
-        <f>IFERROR(B200/C200," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="201" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D201" s="7" t="str">
-        <f>IFERROR(B201/C201," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="202" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D202" s="7" t="str">
-        <f>IFERROR(B202/C202," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="203" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D203" s="7" t="str">
-        <f>IFERROR(B203/C203," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="204" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D204" s="7" t="str">
-        <f>IFERROR(B204/C204," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="205" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D205" s="7" t="str">
-        <f>IFERROR(B205/C205," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="206" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D206" s="7" t="str">
-        <f>IFERROR(B206/C206," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="207" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D207" s="7" t="str">
-        <f>IFERROR(B207/C207," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="208" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D208" s="7" t="str">
-        <f>IFERROR(B208/C208," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D209" s="7" t="str">
-        <f>IFERROR(B209/C209," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D210" s="7" t="str">
-        <f>IFERROR(B210/C210," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D211" s="7" t="str">
-        <f>IFERROR(B211/C211," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D212" s="7" t="str">
-        <f>IFERROR(B212/C212," ")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D213" s="7" t="str">
-        <f>IFERROR(B213/C213," ")</f>
+        <f t="shared" ref="D213:D276" si="5">IFERROR(B213/C213," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D214" s="7" t="str">
-        <f>IFERROR(B214/C214," ")</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D215" s="7" t="str">
-        <f>IFERROR(B215/C215," ")</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D216" s="7" t="str">
-        <f>IFERROR(B216/C216," ")</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D217" s="7" t="str">
-        <f>IFERROR(B217/C217," ")</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D218" s="7" t="str">
-        <f>IFERROR(B218/C218," ")</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3673,7 +3656,7 @@
         <v>528</v>
       </c>
       <c r="D219" s="7">
-        <f>IFERROR(B219/C219," ")</f>
+        <f t="shared" si="5"/>
         <v>3.787878787878788E-3</v>
       </c>
       <c r="E219" t="s">
@@ -3691,7 +3674,7 @@
         <v>544</v>
       </c>
       <c r="D220" s="7">
-        <f>IFERROR(B220/C220," ")</f>
+        <f t="shared" si="5"/>
         <v>3.6764705882352941E-3</v>
       </c>
       <c r="E220" t="s">
@@ -3709,7 +3692,7 @@
         <v>848</v>
       </c>
       <c r="D221" s="7">
-        <f>IFERROR(B221/C221," ")</f>
+        <f t="shared" si="5"/>
         <v>3.5377358490566039E-3</v>
       </c>
       <c r="E221" t="s">
@@ -3727,7 +3710,7 @@
         <v>864</v>
       </c>
       <c r="D222" s="7">
-        <f>IFERROR(B222/C222," ")</f>
+        <f t="shared" si="5"/>
         <v>3.472222222222222E-3</v>
       </c>
       <c r="E222" t="s">
@@ -3745,7 +3728,7 @@
         <v>616</v>
       </c>
       <c r="D223" s="7">
-        <f>IFERROR(B223/C223," ")</f>
+        <f t="shared" si="5"/>
         <v>3.246753246753247E-3</v>
       </c>
       <c r="E223" t="s">
@@ -3763,7 +3746,7 @@
         <v>320</v>
       </c>
       <c r="D224" s="7">
-        <f>IFERROR(B224/C224," ")</f>
+        <f t="shared" si="5"/>
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="E224" t="s">
@@ -3781,7 +3764,7 @@
         <v>1280</v>
       </c>
       <c r="D225" s="7">
-        <f>IFERROR(B225/C225," ")</f>
+        <f t="shared" si="5"/>
         <v>2.3437499999999999E-3</v>
       </c>
       <c r="E225" t="s">

</xml_diff>

<commit_message>
Added two charles perrow books
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="147">
   <si>
     <t>Book Ranking</t>
   </si>
@@ -453,6 +453,12 @@
   </si>
   <si>
     <t>Would it kill you to stop doing that?</t>
+  </si>
+  <si>
+    <t>Complex Organizations (Charles Perrow)</t>
+  </si>
+  <si>
+    <t>Normal Accidents: Living with High Risk Technologies (Charles Perrow)</t>
   </si>
 </sst>
 </file>
@@ -818,11 +824,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E226"/>
+  <dimension ref="A1:E228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D226" sqref="D226"/>
+      <selection pane="bottomLeft" activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,6 +3788,28 @@
         <v>3</v>
       </c>
       <c r="E226" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B227" s="3">
+        <v>4</v>
+      </c>
+      <c r="E227" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B228" s="3">
+        <v>4</v>
+      </c>
+      <c r="E228" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Marked report as read
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$218</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$228</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -827,8 +827,8 @@
   <dimension ref="A1:E228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E225" sqref="E225"/>
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1032,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>141</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>0.44444444444444442</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1122,7 +1122,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
         <v>144</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
         <v>146</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
         <v>145</v>
       </c>
@@ -3814,7 +3814,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E218">
+  <autoFilter ref="A2:E228">
     <filterColumn colId="3">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>

</xml_diff>

<commit_message>
Created automatic read list
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -7,18 +7,20 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Unread" sheetId="1" r:id="rId1"/>
+    <sheet name="Read" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$228</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Read!$A$2:$E$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unread!$A$2:$E$228</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="147">
   <si>
     <t>Book Ranking</t>
   </si>
@@ -827,8 +829,8 @@
   <dimension ref="A1:E228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3815,13 +3817,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:E228">
-    <filterColumn colId="3">
+    <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
     <filterColumn colId="4">
-      <filters>
+      <filters blank="1">
         <filter val="No"/>
       </filters>
     </filterColumn>
@@ -3848,6 +3850,2898 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E131"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.28515625" customWidth="1"/>
+    <col min="2" max="5" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>Unread!A3</f>
+        <v>The Rubaiyat</v>
+      </c>
+      <c r="B3">
+        <f>Unread!B3</f>
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f>Unread!C3</f>
+        <v>46</v>
+      </c>
+      <c r="D3">
+        <f>Unread!D3</f>
+        <v>8.6956521739130432E-2</v>
+      </c>
+      <c r="E3" t="str">
+        <f>Unread!E3</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>Unread!A4</f>
+        <v>World War I at Home</v>
+      </c>
+      <c r="B4">
+        <f>Unread!B4</f>
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f>Unread!C4</f>
+        <v>0</v>
+      </c>
+      <c r="D4" t="str">
+        <f>Unread!D4</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E4" t="str">
+        <f>Unread!E4</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>Unread!A5</f>
+        <v>World War I (Baldwin)</v>
+      </c>
+      <c r="B5">
+        <f>Unread!B5</f>
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f>Unread!C5</f>
+        <v>0</v>
+      </c>
+      <c r="D5" t="str">
+        <f>Unread!D5</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E5" t="str">
+        <f>Unread!E5</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>Unread!A6</f>
+        <v>Cavalry of the Clouds</v>
+      </c>
+      <c r="B6">
+        <f>Unread!B6</f>
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f>Unread!C6</f>
+        <v>0</v>
+      </c>
+      <c r="D6" t="str">
+        <f>Unread!D6</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E6" t="str">
+        <f>Unread!E6</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>Unread!A7</f>
+        <v>Undertones of War</v>
+      </c>
+      <c r="B7">
+        <f>Unread!B7</f>
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <f>Unread!C7</f>
+        <v>0</v>
+      </c>
+      <c r="D7" t="str">
+        <f>Unread!D7</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E7" t="str">
+        <f>Unread!E7</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>Unread!A8</f>
+        <v>Sinking of the Titanic</v>
+      </c>
+      <c r="B8">
+        <f>Unread!B8</f>
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <f>Unread!C8</f>
+        <v>0</v>
+      </c>
+      <c r="D8" t="str">
+        <f>Unread!D8</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E8" t="str">
+        <f>Unread!E8</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>Unread!A9</f>
+        <v>History of the World War (March)</v>
+      </c>
+      <c r="B9">
+        <f>Unread!B9</f>
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f>Unread!C9</f>
+        <v>0</v>
+      </c>
+      <c r="D9" t="str">
+        <f>Unread!D9</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E9" t="str">
+        <f>Unread!E9</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>Unread!A10</f>
+        <v>World War for Humanity</v>
+      </c>
+      <c r="B10">
+        <f>Unread!B10</f>
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <f>Unread!C10</f>
+        <v>0</v>
+      </c>
+      <c r="D10" t="str">
+        <f>Unread!D10</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E10" t="str">
+        <f>Unread!E10</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>Unread!A11</f>
+        <v>School for Soldiers</v>
+      </c>
+      <c r="B11">
+        <f>Unread!B11</f>
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <f>Unread!C11</f>
+        <v>0</v>
+      </c>
+      <c r="D11" t="str">
+        <f>Unread!D11</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E11" t="str">
+        <f>Unread!E11</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>Unread!A12</f>
+        <v>The First World War (Strachan)</v>
+      </c>
+      <c r="B12">
+        <f>Unread!B12</f>
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <f>Unread!C12</f>
+        <v>0</v>
+      </c>
+      <c r="D12" t="str">
+        <f>Unread!D12</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E12" t="str">
+        <f>Unread!E12</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>Unread!A13</f>
+        <v>Soldier from the Wars Returning (Carrington)</v>
+      </c>
+      <c r="B13">
+        <f>Unread!B13</f>
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <f>Unread!C13</f>
+        <v>0</v>
+      </c>
+      <c r="D13" t="str">
+        <f>Unread!D13</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E13" t="str">
+        <f>Unread!E13</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>Unread!A14</f>
+        <v>Randomness and Mathematical Proof (Report)</v>
+      </c>
+      <c r="B14">
+        <f>Unread!B14</f>
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <f>Unread!C14</f>
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <f>Unread!D14</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E14" t="str">
+        <f>Unread!E14</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>Unread!A15</f>
+        <v>The Waste Land: Poem</v>
+      </c>
+      <c r="B15">
+        <f>Unread!B15</f>
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <f>Unread!C15</f>
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <f>Unread!D15</f>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="E15" t="str">
+        <f>Unread!E15</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>Unread!A16</f>
+        <v>Wisdom and the Context of Knowledge: Knowing that One Doesn't Know: Meacham (Report)</v>
+      </c>
+      <c r="B16">
+        <f>Unread!B16</f>
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <f>Unread!C16</f>
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <f>Unread!D16</f>
+        <v>0.2</v>
+      </c>
+      <c r="E16" t="str">
+        <f>Unread!E16</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>Unread!A17</f>
+        <v>Self-organised criticality-what it is and what it isn't (Report)</v>
+      </c>
+      <c r="B17">
+        <f>Unread!B17</f>
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <f>Unread!C17</f>
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <f>Unread!D17</f>
+        <v>0.15</v>
+      </c>
+      <c r="E17" t="str">
+        <f>Unread!E17</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>Unread!A18</f>
+        <v>Power laws, Pareto distributinos and Zipf's Law (Report)</v>
+      </c>
+      <c r="B18">
+        <f>Unread!B18</f>
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <f>Unread!C18</f>
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <f>Unread!D18</f>
+        <v>0.12</v>
+      </c>
+      <c r="E18" t="str">
+        <f>Unread!E18</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>Unread!A19</f>
+        <v>Zoar (Pamphlet)</v>
+      </c>
+      <c r="B19">
+        <f>Unread!B19</f>
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <f>Unread!C19</f>
+        <v>73</v>
+      </c>
+      <c r="D19">
+        <f>Unread!D19</f>
+        <v>6.8493150684931503E-2</v>
+      </c>
+      <c r="E19" t="str">
+        <f>Unread!E19</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>Unread!A20</f>
+        <v xml:space="preserve">On the Decay of the Art of Lying  </v>
+      </c>
+      <c r="B20">
+        <f>Unread!B20</f>
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <f>Unread!C20</f>
+        <v>30</v>
+      </c>
+      <c r="D20">
+        <f>Unread!D20</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="E20" t="str">
+        <f>Unread!E20</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>Unread!A21</f>
+        <v>A Mathematica Theory of Communication: CE Shannon (Report)</v>
+      </c>
+      <c r="B21">
+        <f>Unread!B21</f>
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <f>Unread!C21</f>
+        <v>55</v>
+      </c>
+      <c r="D21">
+        <f>Unread!D21</f>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="E21" t="str">
+        <f>Unread!E21</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>Unread!A22</f>
+        <v>Guerilla Warfare Mao</v>
+      </c>
+      <c r="B22">
+        <f>Unread!B22</f>
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <f>Unread!C22</f>
+        <v>74</v>
+      </c>
+      <c r="D22">
+        <f>Unread!D22</f>
+        <v>5.4054054054054057E-2</v>
+      </c>
+      <c r="E22" t="str">
+        <f>Unread!E22</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>Unread!A23</f>
+        <v>Thermodynamics</v>
+      </c>
+      <c r="B23">
+        <f>Unread!B23</f>
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <f>Unread!C23</f>
+        <v>120</v>
+      </c>
+      <c r="D23">
+        <f>Unread!D23</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E23" t="str">
+        <f>Unread!E23</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>Unread!A24</f>
+        <v>Campaigns of General Custer</v>
+      </c>
+      <c r="B24">
+        <f>Unread!B24</f>
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <f>Unread!C24</f>
+        <v>72</v>
+      </c>
+      <c r="D24">
+        <f>Unread!D24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E24" t="str">
+        <f>Unread!E24</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>Unread!A25</f>
+        <v>A Monk's Guide to a Clean House</v>
+      </c>
+      <c r="B25">
+        <f>Unread!B25</f>
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <f>Unread!C25</f>
+        <v>128</v>
+      </c>
+      <c r="D25">
+        <f>Unread!D25</f>
+        <v>3.90625E-2</v>
+      </c>
+      <c r="E25" t="str">
+        <f>Unread!E25</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>Unread!A26</f>
+        <v>Maneuver Warfare Handbook</v>
+      </c>
+      <c r="B26">
+        <f>Unread!B26</f>
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <f>Unread!C26</f>
+        <v>133</v>
+      </c>
+      <c r="D26">
+        <f>Unread!D26</f>
+        <v>3.7593984962406013E-2</v>
+      </c>
+      <c r="E26" t="str">
+        <f>Unread!E26</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>Unread!A27</f>
+        <v xml:space="preserve">Drop the Rock: Removing Character Defects - Steps Six and Seven  </v>
+      </c>
+      <c r="B27">
+        <f>Unread!B27</f>
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <f>Unread!C27</f>
+        <v>132</v>
+      </c>
+      <c r="D27">
+        <f>Unread!D27</f>
+        <v>3.0303030303030304E-2</v>
+      </c>
+      <c r="E27" t="str">
+        <f>Unread!E27</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>Unread!A28</f>
+        <v>The Parent's Tao Te Ching</v>
+      </c>
+      <c r="B28">
+        <f>Unread!B28</f>
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <f>Unread!C28</f>
+        <v>160</v>
+      </c>
+      <c r="D28">
+        <f>Unread!D28</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E28" t="str">
+        <f>Unread!E28</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>Unread!A29</f>
+        <v xml:space="preserve">The Gnosis of the Light  </v>
+      </c>
+      <c r="B29">
+        <f>Unread!B29</f>
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f>Unread!C29</f>
+        <v>80</v>
+      </c>
+      <c r="D29">
+        <f>Unread!D29</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E29" t="str">
+        <f>Unread!E29</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>Unread!A30</f>
+        <v>The Elements of Zen</v>
+      </c>
+      <c r="B30">
+        <f>Unread!B30</f>
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <f>Unread!C30</f>
+        <v>124</v>
+      </c>
+      <c r="D30">
+        <f>Unread!D30</f>
+        <v>2.4193548387096774E-2</v>
+      </c>
+      <c r="E30" t="str">
+        <f>Unread!E30</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>Unread!A31</f>
+        <v>Impeachment: A Citizen's Guide</v>
+      </c>
+      <c r="B31">
+        <f>Unread!B31</f>
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <f>Unread!C31</f>
+        <v>208</v>
+      </c>
+      <c r="D31">
+        <f>Unread!D31</f>
+        <v>2.403846153846154E-2</v>
+      </c>
+      <c r="E31" t="str">
+        <f>Unread!E31</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>Unread!A32</f>
+        <v xml:space="preserve">On Tyranny: Twenty Lessons From the Twentieth Century  </v>
+      </c>
+      <c r="B32">
+        <f>Unread!B32</f>
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <f>Unread!C32</f>
+        <v>128</v>
+      </c>
+      <c r="D32">
+        <f>Unread!D32</f>
+        <v>2.34375E-2</v>
+      </c>
+      <c r="E32" t="str">
+        <f>Unread!E32</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>Unread!A33</f>
+        <v>Advice Not Given: A Guide for Getting Over Yourself</v>
+      </c>
+      <c r="B33">
+        <f>Unread!B33</f>
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <f>Unread!C33</f>
+        <v>224</v>
+      </c>
+      <c r="D33">
+        <f>Unread!D33</f>
+        <v>2.2321428571428572E-2</v>
+      </c>
+      <c r="E33" t="str">
+        <f>Unread!E33</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>Unread!A34</f>
+        <v xml:space="preserve">Left of Bang: How the Marine Corps' Combat Hunter Program Can Save Your Life  </v>
+      </c>
+      <c r="B34">
+        <f>Unread!B34</f>
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <f>Unread!C34</f>
+        <v>228</v>
+      </c>
+      <c r="D34">
+        <f>Unread!D34</f>
+        <v>2.1929824561403508E-2</v>
+      </c>
+      <c r="E34" t="str">
+        <f>Unread!E34</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>Unread!A35</f>
+        <v>Markings (Dag)</v>
+      </c>
+      <c r="B35">
+        <f>Unread!B35</f>
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <f>Unread!C35</f>
+        <v>191</v>
+      </c>
+      <c r="D35">
+        <f>Unread!D35</f>
+        <v>2.0942408376963352E-2</v>
+      </c>
+      <c r="E35" t="str">
+        <f>Unread!E35</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>Unread!A36</f>
+        <v xml:space="preserve">Simplicity: The Freedom of Letting Go  </v>
+      </c>
+      <c r="B36">
+        <f>Unread!B36</f>
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <f>Unread!C36</f>
+        <v>192</v>
+      </c>
+      <c r="D36">
+        <f>Unread!D36</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E36" t="str">
+        <f>Unread!E36</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f>Unread!A37</f>
+        <v>Dr. Seuss: American Icon</v>
+      </c>
+      <c r="B37">
+        <f>Unread!B37</f>
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <f>Unread!C37</f>
+        <v>198</v>
+      </c>
+      <c r="D37">
+        <f>Unread!D37</f>
+        <v>2.0202020202020204E-2</v>
+      </c>
+      <c r="E37" t="str">
+        <f>Unread!E37</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f>Unread!A38</f>
+        <v>Promise me Dad</v>
+      </c>
+      <c r="B38">
+        <f>Unread!B38</f>
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <f>Unread!C38</f>
+        <v>258</v>
+      </c>
+      <c r="D38">
+        <f>Unread!D38</f>
+        <v>1.937984496124031E-2</v>
+      </c>
+      <c r="E38" t="str">
+        <f>Unread!E38</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f>Unread!A39</f>
+        <v>Norman Rockwell: A Sixty Year Retrospective</v>
+      </c>
+      <c r="B39">
+        <f>Unread!B39</f>
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <f>Unread!C39</f>
+        <v>157</v>
+      </c>
+      <c r="D39">
+        <f>Unread!D39</f>
+        <v>1.9108280254777069E-2</v>
+      </c>
+      <c r="E39" t="str">
+        <f>Unread!E39</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f>Unread!A40</f>
+        <v xml:space="preserve">The Wisdom of Insecurity  </v>
+      </c>
+      <c r="B40">
+        <f>Unread!B40</f>
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <f>Unread!C40</f>
+        <v>160</v>
+      </c>
+      <c r="D40">
+        <f>Unread!D40</f>
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="E40" t="str">
+        <f>Unread!E40</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f>Unread!A41</f>
+        <v xml:space="preserve">The Obstacle Is the Way: The Timeless Art of Turning Trials Into Triumph  </v>
+      </c>
+      <c r="B41">
+        <f>Unread!B41</f>
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <f>Unread!C41</f>
+        <v>224</v>
+      </c>
+      <c r="D41">
+        <f>Unread!D41</f>
+        <v>1.7857142857142856E-2</v>
+      </c>
+      <c r="E41" t="str">
+        <f>Unread!E41</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f>Unread!A42</f>
+        <v>Flight of the Wild Gander</v>
+      </c>
+      <c r="B42">
+        <f>Unread!B42</f>
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <f>Unread!C42</f>
+        <v>226</v>
+      </c>
+      <c r="D42">
+        <f>Unread!D42</f>
+        <v>1.7699115044247787E-2</v>
+      </c>
+      <c r="E42" t="str">
+        <f>Unread!E42</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f>Unread!A43</f>
+        <v xml:space="preserve">Sprint: How to Solve Big Problems and Test New Ideas in Just Five Days  </v>
+      </c>
+      <c r="B43">
+        <f>Unread!B43</f>
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <f>Unread!C43</f>
+        <v>288</v>
+      </c>
+      <c r="D43">
+        <f>Unread!D43</f>
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="E43" t="str">
+        <f>Unread!E43</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f>Unread!A44</f>
+        <v>Buddhism: An Introduction and Guide</v>
+      </c>
+      <c r="B44">
+        <f>Unread!B44</f>
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <f>Unread!C44</f>
+        <v>231</v>
+      </c>
+      <c r="D44">
+        <f>Unread!D44</f>
+        <v>1.7316017316017316E-2</v>
+      </c>
+      <c r="E44" t="str">
+        <f>Unread!E44</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f>Unread!A45</f>
+        <v>The Ransom of Russian Art</v>
+      </c>
+      <c r="B45">
+        <f>Unread!B45</f>
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <f>Unread!C45</f>
+        <v>181</v>
+      </c>
+      <c r="D45">
+        <f>Unread!D45</f>
+        <v>1.6574585635359115E-2</v>
+      </c>
+      <c r="E45" t="str">
+        <f>Unread!E45</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f>Unread!A46</f>
+        <v>The Gnostic Gospels.</v>
+      </c>
+      <c r="B46">
+        <f>Unread!B46</f>
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <f>Unread!C46</f>
+        <v>182</v>
+      </c>
+      <c r="D46">
+        <f>Unread!D46</f>
+        <v>1.6483516483516484E-2</v>
+      </c>
+      <c r="E46" t="str">
+        <f>Unread!E46</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f>Unread!A47</f>
+        <v>Tao of Jeet Kune Do</v>
+      </c>
+      <c r="B47">
+        <f>Unread!B47</f>
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <f>Unread!C47</f>
+        <v>250</v>
+      </c>
+      <c r="D47">
+        <f>Unread!D47</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="E47" t="str">
+        <f>Unread!E47</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f>Unread!A48</f>
+        <v>Myths to Live By</v>
+      </c>
+      <c r="B48">
+        <f>Unread!B48</f>
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <f>Unread!C48</f>
+        <v>266</v>
+      </c>
+      <c r="D48">
+        <f>Unread!D48</f>
+        <v>1.5037593984962405E-2</v>
+      </c>
+      <c r="E48" t="str">
+        <f>Unread!E48</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f>Unread!A49</f>
+        <v xml:space="preserve">Why Buddhism Is True: The Science and Philosophy of Meditation and Enlightenment  </v>
+      </c>
+      <c r="B49">
+        <f>Unread!B49</f>
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <f>Unread!C49</f>
+        <v>336</v>
+      </c>
+      <c r="D49">
+        <f>Unread!D49</f>
+        <v>1.488095238095238E-2</v>
+      </c>
+      <c r="E49" t="str">
+        <f>Unread!E49</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="str">
+        <f>Unread!A50</f>
+        <v>Mooney</v>
+      </c>
+      <c r="B50">
+        <f>Unread!B50</f>
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <f>Unread!C50</f>
+        <v>137</v>
+      </c>
+      <c r="D50">
+        <f>Unread!D50</f>
+        <v>1.4598540145985401E-2</v>
+      </c>
+      <c r="E50" t="str">
+        <f>Unread!E50</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f>Unread!A51</f>
+        <v>Letters from a Stoic</v>
+      </c>
+      <c r="B51">
+        <f>Unread!B51</f>
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <f>Unread!C51</f>
+        <v>276</v>
+      </c>
+      <c r="D51">
+        <f>Unread!D51</f>
+        <v>1.4492753623188406E-2</v>
+      </c>
+      <c r="E51" t="str">
+        <f>Unread!E51</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <f>Unread!A52</f>
+        <v xml:space="preserve">Probably Approximately Correct: Nature's Algorithms for Learning and Prospering in a Complex World  </v>
+      </c>
+      <c r="B52">
+        <f>Unread!B52</f>
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <f>Unread!C52</f>
+        <v>208</v>
+      </c>
+      <c r="D52">
+        <f>Unread!D52</f>
+        <v>1.4423076923076924E-2</v>
+      </c>
+      <c r="E52" t="str">
+        <f>Unread!E52</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f>Unread!A53</f>
+        <v>The Penguin Guide to the United States Constitution</v>
+      </c>
+      <c r="B53">
+        <f>Unread!B53</f>
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <f>Unread!C53</f>
+        <v>213</v>
+      </c>
+      <c r="D53">
+        <f>Unread!D53</f>
+        <v>1.4084507042253521E-2</v>
+      </c>
+      <c r="E53" t="str">
+        <f>Unread!E53</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
+        <f>Unread!A54</f>
+        <v>Rifleman Dodd</v>
+      </c>
+      <c r="B54">
+        <f>Unread!B54</f>
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <f>Unread!C54</f>
+        <v>220</v>
+      </c>
+      <c r="D54">
+        <f>Unread!D54</f>
+        <v>1.3636363636363636E-2</v>
+      </c>
+      <c r="E54" t="str">
+        <f>Unread!E54</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
+        <f>Unread!A55</f>
+        <v>The Thirteenth Turn: A History of the Noose</v>
+      </c>
+      <c r="B55">
+        <f>Unread!B55</f>
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <f>Unread!C55</f>
+        <v>368</v>
+      </c>
+      <c r="D55">
+        <f>Unread!D55</f>
+        <v>1.358695652173913E-2</v>
+      </c>
+      <c r="E55" t="str">
+        <f>Unread!E55</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
+        <f>Unread!A56</f>
+        <v xml:space="preserve">How We Decide  </v>
+      </c>
+      <c r="B56">
+        <f>Unread!B56</f>
+        <v>4</v>
+      </c>
+      <c r="C56">
+        <f>Unread!C56</f>
+        <v>320</v>
+      </c>
+      <c r="D56">
+        <f>Unread!D56</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="E56" t="str">
+        <f>Unread!E56</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="str">
+        <f>Unread!A57</f>
+        <v>Finite and Infinite Games</v>
+      </c>
+      <c r="B57">
+        <f>Unread!B57</f>
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <f>Unread!C57</f>
+        <v>160</v>
+      </c>
+      <c r="D57">
+        <f>Unread!D57</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="E57" t="str">
+        <f>Unread!E57</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="str">
+        <f>Unread!A58</f>
+        <v xml:space="preserve">The Bread Baker's Apprentice: Mastering the Art of Extraordinary Bread  </v>
+      </c>
+      <c r="B58">
+        <f>Unread!B58</f>
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <f>Unread!C58</f>
+        <v>336</v>
+      </c>
+      <c r="D58">
+        <f>Unread!D58</f>
+        <v>1.1904761904761904E-2</v>
+      </c>
+      <c r="E58" t="str">
+        <f>Unread!E58</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="str">
+        <f>Unread!A59</f>
+        <v>Backbone</v>
+      </c>
+      <c r="B59">
+        <f>Unread!B59</f>
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <f>Unread!C59</f>
+        <v>256</v>
+      </c>
+      <c r="D59">
+        <f>Unread!D59</f>
+        <v>1.171875E-2</v>
+      </c>
+      <c r="E59" t="str">
+        <f>Unread!E59</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="str">
+        <f>Unread!A60</f>
+        <v>Johnny Got His Gun</v>
+      </c>
+      <c r="B60">
+        <f>Unread!B60</f>
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <f>Unread!C60</f>
+        <v>256</v>
+      </c>
+      <c r="D60">
+        <f>Unread!D60</f>
+        <v>1.171875E-2</v>
+      </c>
+      <c r="E60" t="str">
+        <f>Unread!E60</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="str">
+        <f>Unread!A61</f>
+        <v>The Hero with a Thousand Faces</v>
+      </c>
+      <c r="B61">
+        <f>Unread!B61</f>
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <f>Unread!C61</f>
+        <v>432</v>
+      </c>
+      <c r="D61">
+        <f>Unread!D61</f>
+        <v>1.1574074074074073E-2</v>
+      </c>
+      <c r="E61" t="str">
+        <f>Unread!E61</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="str">
+        <f>Unread!A62</f>
+        <v xml:space="preserve">Mind in the Balance: Meditation in Science, Buddhism, and Christianity  </v>
+      </c>
+      <c r="B62">
+        <f>Unread!B62</f>
+        <v>3</v>
+      </c>
+      <c r="C62">
+        <f>Unread!C62</f>
+        <v>264</v>
+      </c>
+      <c r="D62">
+        <f>Unread!D62</f>
+        <v>1.1363636363636364E-2</v>
+      </c>
+      <c r="E62" t="str">
+        <f>Unread!E62</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="str">
+        <f>Unread!A63</f>
+        <v>The Elements of Journalism</v>
+      </c>
+      <c r="B63">
+        <f>Unread!B63</f>
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <f>Unread!C63</f>
+        <v>352</v>
+      </c>
+      <c r="D63">
+        <f>Unread!D63</f>
+        <v>1.1363636363636364E-2</v>
+      </c>
+      <c r="E63" t="str">
+        <f>Unread!E63</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="str">
+        <f>Unread!A64</f>
+        <v>Custer's Last Stand: The Anatomy of an American Myth</v>
+      </c>
+      <c r="B64">
+        <f>Unread!B64</f>
+        <v>3</v>
+      </c>
+      <c r="C64">
+        <f>Unread!C64</f>
+        <v>266</v>
+      </c>
+      <c r="D64">
+        <f>Unread!D64</f>
+        <v>1.1278195488721804E-2</v>
+      </c>
+      <c r="E64" t="str">
+        <f>Unread!E64</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="str">
+        <f>Unread!A65</f>
+        <v>History of Nevada: Elliot</v>
+      </c>
+      <c r="B65">
+        <f>Unread!B65</f>
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <f>Unread!C65</f>
+        <v>277</v>
+      </c>
+      <c r="D65">
+        <f>Unread!D65</f>
+        <v>1.0830324909747292E-2</v>
+      </c>
+      <c r="E65" t="str">
+        <f>Unread!E65</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="str">
+        <f>Unread!A66</f>
+        <v>One Man Against the World</v>
+      </c>
+      <c r="B66">
+        <f>Unread!B66</f>
+        <v>4</v>
+      </c>
+      <c r="C66">
+        <f>Unread!C66</f>
+        <v>384</v>
+      </c>
+      <c r="D66">
+        <f>Unread!D66</f>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E66" t="str">
+        <f>Unread!E66</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="str">
+        <f>Unread!A67</f>
+        <v xml:space="preserve">The Gatekeepers: How the White House Chiefs of Staff Define Every Presidency  </v>
+      </c>
+      <c r="B67">
+        <f>Unread!B67</f>
+        <v>4</v>
+      </c>
+      <c r="C67">
+        <f>Unread!C67</f>
+        <v>384</v>
+      </c>
+      <c r="D67">
+        <f>Unread!D67</f>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E67" t="str">
+        <f>Unread!E67</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="str">
+        <f>Unread!A68</f>
+        <v xml:space="preserve">Storm in a Teacup: The Physics of Everyday Life  </v>
+      </c>
+      <c r="B68">
+        <f>Unread!B68</f>
+        <v>3</v>
+      </c>
+      <c r="C68">
+        <f>Unread!C68</f>
+        <v>288</v>
+      </c>
+      <c r="D68">
+        <f>Unread!D68</f>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E68" t="str">
+        <f>Unread!E68</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="str">
+        <f>Unread!A69</f>
+        <v>14-18: Understanding the Great War</v>
+      </c>
+      <c r="B69">
+        <f>Unread!B69</f>
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <f>Unread!C69</f>
+        <v>288</v>
+      </c>
+      <c r="D69">
+        <f>Unread!D69</f>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E69" t="str">
+        <f>Unread!E69</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="str">
+        <f>Unread!A70</f>
+        <v>The Age of American Unreason</v>
+      </c>
+      <c r="B70">
+        <f>Unread!B70</f>
+        <v>4</v>
+      </c>
+      <c r="C70">
+        <f>Unread!C70</f>
+        <v>400</v>
+      </c>
+      <c r="D70">
+        <f>Unread!D70</f>
+        <v>0.01</v>
+      </c>
+      <c r="E70" t="str">
+        <f>Unread!E70</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="str">
+        <f>Unread!A71</f>
+        <v>Ohio A Personal Portrait of the 17th State</v>
+      </c>
+      <c r="B71">
+        <f>Unread!B71</f>
+        <v>2</v>
+      </c>
+      <c r="C71">
+        <f>Unread!C71</f>
+        <v>200</v>
+      </c>
+      <c r="D71">
+        <f>Unread!D71</f>
+        <v>0.01</v>
+      </c>
+      <c r="E71" t="str">
+        <f>Unread!E71</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="str">
+        <f>Unread!A72</f>
+        <v>Guidebook for Marines</v>
+      </c>
+      <c r="B72">
+        <f>Unread!B72</f>
+        <v>4</v>
+      </c>
+      <c r="C72">
+        <f>Unread!C72</f>
+        <v>400</v>
+      </c>
+      <c r="D72">
+        <f>Unread!D72</f>
+        <v>0.01</v>
+      </c>
+      <c r="E72" t="str">
+        <f>Unread!E72</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="str">
+        <f>Unread!A73</f>
+        <v xml:space="preserve">The Gamble: General Petraeus and the American Military Adventure in Iraq  </v>
+      </c>
+      <c r="B73">
+        <f>Unread!B73</f>
+        <v>4</v>
+      </c>
+      <c r="C73">
+        <f>Unread!C73</f>
+        <v>416</v>
+      </c>
+      <c r="D73">
+        <f>Unread!D73</f>
+        <v>9.6153846153846159E-3</v>
+      </c>
+      <c r="E73" t="str">
+        <f>Unread!E73</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="str">
+        <f>Unread!A74</f>
+        <v>The Alchemist</v>
+      </c>
+      <c r="B74">
+        <f>Unread!B74</f>
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <f>Unread!C74</f>
+        <v>208</v>
+      </c>
+      <c r="D74">
+        <f>Unread!D74</f>
+        <v>9.6153846153846159E-3</v>
+      </c>
+      <c r="E74" t="str">
+        <f>Unread!E74</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="str">
+        <f>Unread!A75</f>
+        <v xml:space="preserve">Physics Made Simple: A Complete Introduction to the Basic Principles of This Fundamental Science (Made    - Simple (Broadway Books))  </v>
+      </c>
+      <c r="B75">
+        <f>Unread!B75</f>
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <f>Unread!C75</f>
+        <v>208</v>
+      </c>
+      <c r="D75">
+        <f>Unread!D75</f>
+        <v>9.6153846153846159E-3</v>
+      </c>
+      <c r="E75" t="str">
+        <f>Unread!E75</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="str">
+        <f>Unread!A76</f>
+        <v>Knocking on Labor's Door</v>
+      </c>
+      <c r="B76">
+        <f>Unread!B76</f>
+        <v>3</v>
+      </c>
+      <c r="C76">
+        <f>Unread!C76</f>
+        <v>312</v>
+      </c>
+      <c r="D76">
+        <f>Unread!D76</f>
+        <v>9.6153846153846159E-3</v>
+      </c>
+      <c r="E76" t="str">
+        <f>Unread!E76</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="str">
+        <f>Unread!A77</f>
+        <v>Boots and Saddles</v>
+      </c>
+      <c r="B77">
+        <f>Unread!B77</f>
+        <v>3</v>
+      </c>
+      <c r="C77">
+        <f>Unread!C77</f>
+        <v>316</v>
+      </c>
+      <c r="D77">
+        <f>Unread!D77</f>
+        <v>9.4936708860759497E-3</v>
+      </c>
+      <c r="E77" t="str">
+        <f>Unread!E77</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="str">
+        <f>Unread!A78</f>
+        <v>Bringing up Bebe</v>
+      </c>
+      <c r="B78">
+        <f>Unread!B78</f>
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <f>Unread!C78</f>
+        <v>432</v>
+      </c>
+      <c r="D78">
+        <f>Unread!D78</f>
+        <v>9.2592592592592587E-3</v>
+      </c>
+      <c r="E78" t="str">
+        <f>Unread!E78</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="str">
+        <f>Unread!A79</f>
+        <v xml:space="preserve">I Am a Strange Loop  </v>
+      </c>
+      <c r="B79">
+        <f>Unread!B79</f>
+        <v>4</v>
+      </c>
+      <c r="C79">
+        <f>Unread!C79</f>
+        <v>436</v>
+      </c>
+      <c r="D79">
+        <f>Unread!D79</f>
+        <v>9.1743119266055051E-3</v>
+      </c>
+      <c r="E79" t="str">
+        <f>Unread!E79</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="str">
+        <f>Unread!A80</f>
+        <v>The Black Swan</v>
+      </c>
+      <c r="B80">
+        <f>Unread!B80</f>
+        <v>4</v>
+      </c>
+      <c r="C80">
+        <f>Unread!C80</f>
+        <v>444</v>
+      </c>
+      <c r="D80">
+        <f>Unread!D80</f>
+        <v>9.0090090090090089E-3</v>
+      </c>
+      <c r="E80" t="str">
+        <f>Unread!E80</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="str">
+        <f>Unread!A81</f>
+        <v xml:space="preserve">Eichmann in Jerusalem: A Report on the Banality of Evil (Penguin Classics)  </v>
+      </c>
+      <c r="B81">
+        <f>Unread!B81</f>
+        <v>3</v>
+      </c>
+      <c r="C81">
+        <f>Unread!C81</f>
+        <v>336</v>
+      </c>
+      <c r="D81">
+        <f>Unread!D81</f>
+        <v>8.9285714285714281E-3</v>
+      </c>
+      <c r="E81" t="str">
+        <f>Unread!E81</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="str">
+        <f>Unread!A82</f>
+        <v>The Relativity of Wrong (Asimov)</v>
+      </c>
+      <c r="B82">
+        <f>Unread!B82</f>
+        <v>2</v>
+      </c>
+      <c r="C82">
+        <f>Unread!C82</f>
+        <v>225</v>
+      </c>
+      <c r="D82">
+        <f>Unread!D82</f>
+        <v>8.8888888888888889E-3</v>
+      </c>
+      <c r="E82" t="str">
+        <f>Unread!E82</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="str">
+        <f>Unread!A83</f>
+        <v>Nuclear Weapons and Coercive Diplomacy</v>
+      </c>
+      <c r="B83">
+        <f>Unread!B83</f>
+        <v>3</v>
+      </c>
+      <c r="C83">
+        <f>Unread!C83</f>
+        <v>344</v>
+      </c>
+      <c r="D83">
+        <f>Unread!D83</f>
+        <v>8.7209302325581394E-3</v>
+      </c>
+      <c r="E83" t="str">
+        <f>Unread!E83</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="str">
+        <f>Unread!A84</f>
+        <v>A Generation of Sociopaths</v>
+      </c>
+      <c r="B84">
+        <f>Unread!B84</f>
+        <v>4</v>
+      </c>
+      <c r="C84">
+        <f>Unread!C84</f>
+        <v>464</v>
+      </c>
+      <c r="D84">
+        <f>Unread!D84</f>
+        <v>8.6206896551724137E-3</v>
+      </c>
+      <c r="E84" t="str">
+        <f>Unread!E84</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="str">
+        <f>Unread!A85</f>
+        <v xml:space="preserve">Abraham Lincoln and the Structure of Reason  </v>
+      </c>
+      <c r="B85">
+        <f>Unread!B85</f>
+        <v>4</v>
+      </c>
+      <c r="C85">
+        <f>Unread!C85</f>
+        <v>464</v>
+      </c>
+      <c r="D85">
+        <f>Unread!D85</f>
+        <v>8.6206896551724137E-3</v>
+      </c>
+      <c r="E85" t="str">
+        <f>Unread!E85</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="str">
+        <f>Unread!A86</f>
+        <v xml:space="preserve">Silence: A Christian History  </v>
+      </c>
+      <c r="B86">
+        <f>Unread!B86</f>
+        <v>3</v>
+      </c>
+      <c r="C86">
+        <f>Unread!C86</f>
+        <v>352</v>
+      </c>
+      <c r="D86">
+        <f>Unread!D86</f>
+        <v>8.5227272727272721E-3</v>
+      </c>
+      <c r="E86" t="str">
+        <f>Unread!E86</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="str">
+        <f>Unread!A87</f>
+        <v>The Eastern Front 1914-1917</v>
+      </c>
+      <c r="B87">
+        <f>Unread!B87</f>
+        <v>3</v>
+      </c>
+      <c r="C87">
+        <f>Unread!C87</f>
+        <v>352</v>
+      </c>
+      <c r="D87">
+        <f>Unread!D87</f>
+        <v>8.5227272727272721E-3</v>
+      </c>
+      <c r="E87" t="str">
+        <f>Unread!E87</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="str">
+        <f>Unread!A88</f>
+        <v>The Battle for God</v>
+      </c>
+      <c r="B88">
+        <f>Unread!B88</f>
+        <v>4</v>
+      </c>
+      <c r="C88">
+        <f>Unread!C88</f>
+        <v>480</v>
+      </c>
+      <c r="D88">
+        <f>Unread!D88</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="E88" t="str">
+        <f>Unread!E88</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="str">
+        <f>Unread!A89</f>
+        <v>Warriors and Citizens</v>
+      </c>
+      <c r="B89">
+        <f>Unread!B89</f>
+        <v>3</v>
+      </c>
+      <c r="C89">
+        <f>Unread!C89</f>
+        <v>360</v>
+      </c>
+      <c r="D89">
+        <f>Unread!D89</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="E89" t="str">
+        <f>Unread!E89</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="str">
+        <f>Unread!A90</f>
+        <v>Bible Nation</v>
+      </c>
+      <c r="B90">
+        <f>Unread!B90</f>
+        <v>2</v>
+      </c>
+      <c r="C90">
+        <f>Unread!C90</f>
+        <v>240</v>
+      </c>
+      <c r="D90">
+        <f>Unread!D90</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="E90" t="str">
+        <f>Unread!E90</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="str">
+        <f>Unread!A91</f>
+        <v>Leaders Eat Last</v>
+      </c>
+      <c r="B91">
+        <f>Unread!B91</f>
+        <v>3</v>
+      </c>
+      <c r="C91">
+        <f>Unread!C91</f>
+        <v>368</v>
+      </c>
+      <c r="D91">
+        <f>Unread!D91</f>
+        <v>8.152173913043478E-3</v>
+      </c>
+      <c r="E91" t="str">
+        <f>Unread!E91</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" t="str">
+        <f>Unread!A92</f>
+        <v>Legionnaire</v>
+      </c>
+      <c r="B92">
+        <f>Unread!B92</f>
+        <v>3</v>
+      </c>
+      <c r="C92">
+        <f>Unread!C92</f>
+        <v>368</v>
+      </c>
+      <c r="D92">
+        <f>Unread!D92</f>
+        <v>8.152173913043478E-3</v>
+      </c>
+      <c r="E92" t="str">
+        <f>Unread!E92</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="str">
+        <f>Unread!A93</f>
+        <v>Empire of the Summer Moon: Quanah Parker and the Rise and Fall of the Comanche's, the Most Powerful</v>
+      </c>
+      <c r="B93">
+        <f>Unread!B93</f>
+        <v>3</v>
+      </c>
+      <c r="C93">
+        <f>Unread!C93</f>
+        <v>371</v>
+      </c>
+      <c r="D93">
+        <f>Unread!D93</f>
+        <v>8.0862533692722376E-3</v>
+      </c>
+      <c r="E93" t="str">
+        <f>Unread!E93</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="str">
+        <f>Unread!A94</f>
+        <v>Thinking Fast and Slow</v>
+      </c>
+      <c r="B94">
+        <f>Unread!B94</f>
+        <v>4</v>
+      </c>
+      <c r="C94">
+        <f>Unread!C94</f>
+        <v>499</v>
+      </c>
+      <c r="D94">
+        <f>Unread!D94</f>
+        <v>8.0160320641282558E-3</v>
+      </c>
+      <c r="E94" t="str">
+        <f>Unread!E94</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="str">
+        <f>Unread!A95</f>
+        <v xml:space="preserve">Living Buddha, Living Christ 10th Anniversary Edition  </v>
+      </c>
+      <c r="B95">
+        <f>Unread!B95</f>
+        <v>2</v>
+      </c>
+      <c r="C95">
+        <f>Unread!C95</f>
+        <v>250</v>
+      </c>
+      <c r="D95">
+        <f>Unread!D95</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E95" t="str">
+        <f>Unread!E95</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="str">
+        <f>Unread!A96</f>
+        <v>Jerusalem: One City Three Faiths</v>
+      </c>
+      <c r="B96">
+        <f>Unread!B96</f>
+        <v>4</v>
+      </c>
+      <c r="C96">
+        <f>Unread!C96</f>
+        <v>512</v>
+      </c>
+      <c r="D96">
+        <f>Unread!D96</f>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="E96" t="str">
+        <f>Unread!E96</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="str">
+        <f>Unread!A97</f>
+        <v>Fiasco</v>
+      </c>
+      <c r="B97">
+        <f>Unread!B97</f>
+        <v>4</v>
+      </c>
+      <c r="C97">
+        <f>Unread!C97</f>
+        <v>512</v>
+      </c>
+      <c r="D97">
+        <f>Unread!D97</f>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="E97" t="str">
+        <f>Unread!E97</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" t="str">
+        <f>Unread!A98</f>
+        <v>Wrapped in the Flag: A Personal History of America's Radical Right</v>
+      </c>
+      <c r="B98">
+        <f>Unread!B98</f>
+        <v>2</v>
+      </c>
+      <c r="C98">
+        <f>Unread!C98</f>
+        <v>264</v>
+      </c>
+      <c r="D98">
+        <f>Unread!D98</f>
+        <v>7.575757575757576E-3</v>
+      </c>
+      <c r="E98" t="str">
+        <f>Unread!E98</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="str">
+        <f>Unread!A99</f>
+        <v xml:space="preserve">War Against War: The American Fight for Peace, 1914-1918    </v>
+      </c>
+      <c r="B99">
+        <f>Unread!B99</f>
+        <v>3</v>
+      </c>
+      <c r="C99">
+        <f>Unread!C99</f>
+        <v>400</v>
+      </c>
+      <c r="D99">
+        <f>Unread!D99</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="E99" t="str">
+        <f>Unread!E99</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="str">
+        <f>Unread!A100</f>
+        <v>The Information: A History, A Theory, A Flood</v>
+      </c>
+      <c r="B100">
+        <f>Unread!B100</f>
+        <v>4</v>
+      </c>
+      <c r="C100">
+        <f>Unread!C100</f>
+        <v>544</v>
+      </c>
+      <c r="D100">
+        <f>Unread!D100</f>
+        <v>7.3529411764705881E-3</v>
+      </c>
+      <c r="E100" t="str">
+        <f>Unread!E100</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="str">
+        <f>Unread!A101</f>
+        <v>On Killing</v>
+      </c>
+      <c r="B101">
+        <f>Unread!B101</f>
+        <v>3</v>
+      </c>
+      <c r="C101">
+        <f>Unread!C101</f>
+        <v>416</v>
+      </c>
+      <c r="D101">
+        <f>Unread!D101</f>
+        <v>7.2115384615384619E-3</v>
+      </c>
+      <c r="E101" t="str">
+        <f>Unread!E101</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="str">
+        <f>Unread!A102</f>
+        <v>Don't Know Much About Mythology</v>
+      </c>
+      <c r="B102">
+        <f>Unread!B102</f>
+        <v>4</v>
+      </c>
+      <c r="C102">
+        <f>Unread!C102</f>
+        <v>560</v>
+      </c>
+      <c r="D102">
+        <f>Unread!D102</f>
+        <v>7.1428571428571426E-3</v>
+      </c>
+      <c r="E102" t="str">
+        <f>Unread!E102</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A103" t="str">
+        <f>Unread!A103</f>
+        <v>A Saturnalia of Bunk</v>
+      </c>
+      <c r="B103">
+        <f>Unread!B103</f>
+        <v>2</v>
+      </c>
+      <c r="C103">
+        <f>Unread!C103</f>
+        <v>284</v>
+      </c>
+      <c r="D103">
+        <f>Unread!D103</f>
+        <v>7.0422535211267607E-3</v>
+      </c>
+      <c r="E103" t="str">
+        <f>Unread!E103</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A104" t="str">
+        <f>Unread!A104</f>
+        <v xml:space="preserve">The Psychopath Test: A Journey Through the Madness Industry  </v>
+      </c>
+      <c r="B104">
+        <f>Unread!B104</f>
+        <v>2</v>
+      </c>
+      <c r="C104">
+        <f>Unread!C104</f>
+        <v>288</v>
+      </c>
+      <c r="D104">
+        <f>Unread!D104</f>
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E104" t="str">
+        <f>Unread!E104</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A105" t="str">
+        <f>Unread!A105</f>
+        <v>A Testament of Hope: The Essential Writings and Speeches (MLK)</v>
+      </c>
+      <c r="B105">
+        <f>Unread!B105</f>
+        <v>5</v>
+      </c>
+      <c r="C105">
+        <f>Unread!C105</f>
+        <v>736</v>
+      </c>
+      <c r="D105">
+        <f>Unread!D105</f>
+        <v>6.793478260869565E-3</v>
+      </c>
+      <c r="E105" t="str">
+        <f>Unread!E105</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" t="str">
+        <f>Unread!A106</f>
+        <v xml:space="preserve">History of Religion a Sketch of Primitive Religious Beliefs and Practices, and of the Origin and Character of the Great Systems  </v>
+      </c>
+      <c r="B106">
+        <f>Unread!B106</f>
+        <v>1</v>
+      </c>
+      <c r="C106">
+        <f>Unread!C106</f>
+        <v>148</v>
+      </c>
+      <c r="D106">
+        <f>Unread!D106</f>
+        <v>6.7567567567567571E-3</v>
+      </c>
+      <c r="E106" t="str">
+        <f>Unread!E106</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A107" t="str">
+        <f>Unread!A107</f>
+        <v>The Big Bonanza</v>
+      </c>
+      <c r="B107">
+        <f>Unread!B107</f>
+        <v>3</v>
+      </c>
+      <c r="C107">
+        <f>Unread!C107</f>
+        <v>450</v>
+      </c>
+      <c r="D107">
+        <f>Unread!D107</f>
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="E107" t="str">
+        <f>Unread!E107</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108" t="str">
+        <f>Unread!A108</f>
+        <v>The New Knighthood</v>
+      </c>
+      <c r="B108">
+        <f>Unread!B108</f>
+        <v>3</v>
+      </c>
+      <c r="C108">
+        <f>Unread!C108</f>
+        <v>464</v>
+      </c>
+      <c r="D108">
+        <f>Unread!D108</f>
+        <v>6.4655172413793103E-3</v>
+      </c>
+      <c r="E108" t="str">
+        <f>Unread!E108</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="str">
+        <f>Unread!A109</f>
+        <v>Hard Times</v>
+      </c>
+      <c r="B109">
+        <f>Unread!B109</f>
+        <v>3</v>
+      </c>
+      <c r="C109">
+        <f>Unread!C109</f>
+        <v>480</v>
+      </c>
+      <c r="D109">
+        <f>Unread!D109</f>
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="E109" t="str">
+        <f>Unread!E109</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110" t="str">
+        <f>Unread!A110</f>
+        <v xml:space="preserve">Black Earth: The Holocaust as History and Warning  </v>
+      </c>
+      <c r="B110">
+        <f>Unread!B110</f>
+        <v>3</v>
+      </c>
+      <c r="C110">
+        <f>Unread!C110</f>
+        <v>480</v>
+      </c>
+      <c r="D110">
+        <f>Unread!D110</f>
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="E110" t="str">
+        <f>Unread!E110</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A111" t="str">
+        <f>Unread!A111</f>
+        <v xml:space="preserve">Liberty or Death: The French Revolution </v>
+      </c>
+      <c r="B111">
+        <f>Unread!B111</f>
+        <v>3</v>
+      </c>
+      <c r="C111">
+        <f>Unread!C111</f>
+        <v>488</v>
+      </c>
+      <c r="D111">
+        <f>Unread!D111</f>
+        <v>6.1475409836065573E-3</v>
+      </c>
+      <c r="E111" t="str">
+        <f>Unread!E111</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112" t="str">
+        <f>Unread!A112</f>
+        <v>How Democracies Die</v>
+      </c>
+      <c r="B112">
+        <f>Unread!B112</f>
+        <v>2</v>
+      </c>
+      <c r="C112">
+        <f>Unread!C112</f>
+        <v>332</v>
+      </c>
+      <c r="D112">
+        <f>Unread!D112</f>
+        <v>6.024096385542169E-3</v>
+      </c>
+      <c r="E112" t="str">
+        <f>Unread!E112</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A113" t="str">
+        <f>Unread!A113</f>
+        <v>Venetian Masque</v>
+      </c>
+      <c r="B113">
+        <f>Unread!B113</f>
+        <v>2</v>
+      </c>
+      <c r="C113">
+        <f>Unread!C113</f>
+        <v>332</v>
+      </c>
+      <c r="D113">
+        <f>Unread!D113</f>
+        <v>6.024096385542169E-3</v>
+      </c>
+      <c r="E113" t="str">
+        <f>Unread!E113</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="str">
+        <f>Unread!A114</f>
+        <v>A Pictorial History of the Great Lakes</v>
+      </c>
+      <c r="B114">
+        <f>Unread!B114</f>
+        <v>2</v>
+      </c>
+      <c r="C114">
+        <f>Unread!C114</f>
+        <v>344</v>
+      </c>
+      <c r="D114">
+        <f>Unread!D114</f>
+        <v>5.8139534883720929E-3</v>
+      </c>
+      <c r="E114" t="str">
+        <f>Unread!E114</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A115" t="str">
+        <f>Unread!A115</f>
+        <v>A Man in Full</v>
+      </c>
+      <c r="B115">
+        <f>Unread!B115</f>
+        <v>4</v>
+      </c>
+      <c r="C115">
+        <f>Unread!C115</f>
+        <v>704</v>
+      </c>
+      <c r="D115">
+        <f>Unread!D115</f>
+        <v>5.681818181818182E-3</v>
+      </c>
+      <c r="E115" t="str">
+        <f>Unread!E115</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" t="str">
+        <f>Unread!A116</f>
+        <v>The Last King</v>
+      </c>
+      <c r="B116">
+        <f>Unread!B116</f>
+        <v>2</v>
+      </c>
+      <c r="C116">
+        <f>Unread!C116</f>
+        <v>366</v>
+      </c>
+      <c r="D116">
+        <f>Unread!D116</f>
+        <v>5.4644808743169399E-3</v>
+      </c>
+      <c r="E116" t="str">
+        <f>Unread!E116</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A117" t="str">
+        <f>Unread!A117</f>
+        <v xml:space="preserve">Tools of Titans: The Tactics, Routines, and Habits of Billionaires, Icons, and World-Class Performers  </v>
+      </c>
+      <c r="B117">
+        <f>Unread!B117</f>
+        <v>4</v>
+      </c>
+      <c r="C117">
+        <f>Unread!C117</f>
+        <v>736</v>
+      </c>
+      <c r="D117">
+        <f>Unread!D117</f>
+        <v>5.434782608695652E-3</v>
+      </c>
+      <c r="E117" t="str">
+        <f>Unread!E117</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A118" t="str">
+        <f>Unread!A118</f>
+        <v xml:space="preserve">Nom De Plume: A (Secret) History of Pseudonyms </v>
+      </c>
+      <c r="B118">
+        <f>Unread!B118</f>
+        <v>2</v>
+      </c>
+      <c r="C118">
+        <f>Unread!C118</f>
+        <v>373</v>
+      </c>
+      <c r="D118">
+        <f>Unread!D118</f>
+        <v>5.3619302949061663E-3</v>
+      </c>
+      <c r="E118" t="str">
+        <f>Unread!E118</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119" t="str">
+        <f>Unread!A119</f>
+        <v>Enemies: A History of the FBI</v>
+      </c>
+      <c r="B119">
+        <f>Unread!B119</f>
+        <v>3</v>
+      </c>
+      <c r="C119">
+        <f>Unread!C119</f>
+        <v>560</v>
+      </c>
+      <c r="D119">
+        <f>Unread!D119</f>
+        <v>5.3571428571428572E-3</v>
+      </c>
+      <c r="E119" t="str">
+        <f>Unread!E119</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A120" t="str">
+        <f>Unread!A120</f>
+        <v>Don't Know Much About the Bible</v>
+      </c>
+      <c r="B120">
+        <f>Unread!B120</f>
+        <v>3</v>
+      </c>
+      <c r="C120">
+        <f>Unread!C120</f>
+        <v>560</v>
+      </c>
+      <c r="D120">
+        <f>Unread!D120</f>
+        <v>5.3571428571428572E-3</v>
+      </c>
+      <c r="E120" t="str">
+        <f>Unread!E120</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="str">
+        <f>Unread!A121</f>
+        <v xml:space="preserve">The Origins of Totalitarianism </v>
+      </c>
+      <c r="B121">
+        <f>Unread!B121</f>
+        <v>3</v>
+      </c>
+      <c r="C121">
+        <f>Unread!C121</f>
+        <v>576</v>
+      </c>
+      <c r="D121">
+        <f>Unread!D121</f>
+        <v>5.208333333333333E-3</v>
+      </c>
+      <c r="E121" t="str">
+        <f>Unread!E121</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="str">
+        <f>Unread!A122</f>
+        <v>How Music Works</v>
+      </c>
+      <c r="B122">
+        <f>Unread!B122</f>
+        <v>2</v>
+      </c>
+      <c r="C122">
+        <f>Unread!C122</f>
+        <v>384</v>
+      </c>
+      <c r="D122">
+        <f>Unread!D122</f>
+        <v>5.208333333333333E-3</v>
+      </c>
+      <c r="E122" t="str">
+        <f>Unread!E122</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="str">
+        <f>Unread!A123</f>
+        <v>The Great Unknown</v>
+      </c>
+      <c r="B123">
+        <f>Unread!B123</f>
+        <v>1</v>
+      </c>
+      <c r="C123">
+        <f>Unread!C123</f>
+        <v>200</v>
+      </c>
+      <c r="D123">
+        <f>Unread!D123</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E123" t="str">
+        <f>Unread!E123</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="str">
+        <f>Unread!A124</f>
+        <v>The Way of the Knife</v>
+      </c>
+      <c r="B124">
+        <f>Unread!B124</f>
+        <v>2</v>
+      </c>
+      <c r="C124">
+        <f>Unread!C124</f>
+        <v>400</v>
+      </c>
+      <c r="D124">
+        <f>Unread!D124</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E124" t="str">
+        <f>Unread!E124</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A125" t="str">
+        <f>Unread!A125</f>
+        <v>Biblical Literalism</v>
+      </c>
+      <c r="B125">
+        <f>Unread!B125</f>
+        <v>2</v>
+      </c>
+      <c r="C125">
+        <f>Unread!C125</f>
+        <v>416</v>
+      </c>
+      <c r="D125">
+        <f>Unread!D125</f>
+        <v>4.807692307692308E-3</v>
+      </c>
+      <c r="E125" t="str">
+        <f>Unread!E125</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="str">
+        <f>Unread!A126</f>
+        <v xml:space="preserve">Red Notice: A True Story of High Finance, Murder, and One Man’s Fight for Justice  </v>
+      </c>
+      <c r="B126">
+        <f>Unread!B126</f>
+        <v>2</v>
+      </c>
+      <c r="C126">
+        <f>Unread!C126</f>
+        <v>416</v>
+      </c>
+      <c r="D126">
+        <f>Unread!D126</f>
+        <v>4.807692307692308E-3</v>
+      </c>
+      <c r="E126" t="str">
+        <f>Unread!E126</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="str">
+        <f>Unread!A127</f>
+        <v>An Unfinished Life</v>
+      </c>
+      <c r="B127">
+        <f>Unread!B127</f>
+        <v>4</v>
+      </c>
+      <c r="C127">
+        <f>Unread!C127</f>
+        <v>848</v>
+      </c>
+      <c r="D127">
+        <f>Unread!D127</f>
+        <v>4.7169811320754715E-3</v>
+      </c>
+      <c r="E127" t="str">
+        <f>Unread!E127</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A128" t="str">
+        <f>Unread!A128</f>
+        <v>The War To End All Wars (Coffman)</v>
+      </c>
+      <c r="B128">
+        <f>Unread!B128</f>
+        <v>2</v>
+      </c>
+      <c r="C128">
+        <f>Unread!C128</f>
+        <v>440</v>
+      </c>
+      <c r="D128">
+        <f>Unread!D128</f>
+        <v>4.5454545454545452E-3</v>
+      </c>
+      <c r="E128" t="str">
+        <f>Unread!E128</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A129" t="str">
+        <f>Unread!A129</f>
+        <v>1000 Beautiful Things</v>
+      </c>
+      <c r="B129">
+        <f>Unread!B129</f>
+        <v>2</v>
+      </c>
+      <c r="C129">
+        <f>Unread!C129</f>
+        <v>456</v>
+      </c>
+      <c r="D129">
+        <f>Unread!D129</f>
+        <v>4.3859649122807015E-3</v>
+      </c>
+      <c r="E129" t="str">
+        <f>Unread!E129</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <f>Unread!A130</f>
+        <v>0</v>
+      </c>
+      <c r="B130">
+        <f>Unread!B130</f>
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <f>Unread!C130</f>
+        <v>0</v>
+      </c>
+      <c r="D130" t="str">
+        <f>Unread!D130</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E130">
+        <f>Unread!E130</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <f>Unread!A131</f>
+        <v>0</v>
+      </c>
+      <c r="B131">
+        <f>Unread!B131</f>
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <f>Unread!C131</f>
+        <v>0</v>
+      </c>
+      <c r="D131" t="str">
+        <f>Unread!D131</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E131">
+        <f>Unread!E131</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:E131">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added two books and marked as read.
</commit_message>
<xml_diff>
--- a/Book Ranking.xlsx
+++ b/Book Ranking.xlsx
@@ -20,13 +20,13 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="163">
   <si>
     <t>Book Ranking</t>
   </si>
@@ -509,6 +509,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Scattered</t>
+  </si>
+  <si>
+    <t>Managing the Unexpected</t>
   </si>
 </sst>
 </file>
@@ -2722,7 +2728,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1">
   <location ref="A4:A110" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -5861,7 +5867,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6088,7 +6094,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>155</v>
       </c>
@@ -6106,7 +6112,7 @@
         <v>0.36363636363636365</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6151,7 +6157,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>140</v>
       </c>
@@ -6169,7 +6175,7 @@
         <v>0.21428571428571427</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -8325,7 +8331,7 @@
         <v>736</v>
       </c>
       <c r="E121" s="7">
-        <f t="shared" ref="E121:E152" si="5">IFERROR(C121/D121," ")</f>
+        <f t="shared" ref="E121:E140" si="5">IFERROR(C121/D121," ")</f>
         <v>5.434782608695652E-3</v>
       </c>
       <c r="F121" t="s">
@@ -9139,7 +9145,7 @@
     </row>
     <row r="207" spans="5:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="E207" s="7" t="str">
-        <f t="shared" ref="E207:E238" si="8">IFERROR(C207/D207," ")</f>
+        <f t="shared" ref="E207:E218" si="8">IFERROR(C207/D207," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -9220,8 +9226,34 @@
         <v>72</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B220" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C220" s="3">
+        <v>4</v>
+      </c>
+      <c r="F220" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B221" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C221" s="3">
+        <v>3</v>
+      </c>
+      <c r="F221" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
@@ -9576,7 +9608,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>Unread!A15</f>
         <v>Enhancing our Grasp of Complex Arguments (Paper)</v>
@@ -9595,7 +9627,7 @@
       </c>
       <c r="E15" t="str">
         <f>Unread!F15</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -9642,7 +9674,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>Unread!A18</f>
         <v>The Waste Land: Poem</v>
@@ -9661,7 +9693,7 @@
       </c>
       <c r="E18" t="str">
         <f>Unread!F18</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>